<commit_message>
Pass settings object to model for custom nodes
Links are still hard coded, but cascade node labels are passed in via a
settings object.
Step forward function edited so that all nodes without pre-allocation
have arrays extended (rather than the ones that are just linked). More
robust.
Accordingly, run model.py for this commit to see dynamics for a
mostly-unlinked cascade.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -32,157 +32,157 @@
     <t>Susceptible</t>
   </si>
   <si>
+    <t>lte</t>
+  </si>
+  <si>
+    <t>Early-Stage Latent</t>
+  </si>
+  <si>
+    <t>s+e</t>
+  </si>
+  <si>
+    <t>Early-Stage Smear-Positive</t>
+  </si>
+  <si>
+    <t>s-e</t>
+  </si>
+  <si>
+    <t>Early-Stage Smear-Negative</t>
+  </si>
+  <si>
+    <t>pue</t>
+  </si>
+  <si>
+    <t>Early-Stage Pulmonary</t>
+  </si>
+  <si>
+    <t>ltsu</t>
+  </si>
+  <si>
+    <t>ltfu</t>
+  </si>
+  <si>
+    <t>Slow Latent Untreated</t>
+  </si>
+  <si>
+    <t>Fast Latent Untreated</t>
+  </si>
+  <si>
+    <t>ltst</t>
+  </si>
+  <si>
+    <t>ltft</t>
+  </si>
+  <si>
+    <t>Slow Latent Treated</t>
+  </si>
+  <si>
+    <t>Fast Latent Treated</t>
+  </si>
+  <si>
+    <t>s+du</t>
+  </si>
+  <si>
+    <t>Drug-Susceptible Smear-Positive Untreated</t>
+  </si>
+  <si>
+    <t>s+dt</t>
+  </si>
+  <si>
+    <t>Drug-Susceptible Smear-Positive Treated</t>
+  </si>
+  <si>
+    <t>s+mu</t>
+  </si>
+  <si>
+    <t>s+mt</t>
+  </si>
+  <si>
+    <t>s+xu</t>
+  </si>
+  <si>
+    <t>s+xt</t>
+  </si>
+  <si>
+    <t>Multidrug-Resistant Smear-Positive Untreated</t>
+  </si>
+  <si>
+    <t>Multidrug-Resistant Smear-Positive Treated</t>
+  </si>
+  <si>
+    <t>Extensively Drug-Resistant Smear-Positive Untreated</t>
+  </si>
+  <si>
+    <t>Extensively Drug-Resistant Smear-Positive Treated</t>
+  </si>
+  <si>
+    <t>s-du</t>
+  </si>
+  <si>
+    <t>s-dt</t>
+  </si>
+  <si>
+    <t>s-mu</t>
+  </si>
+  <si>
+    <t>s-mt</t>
+  </si>
+  <si>
+    <t>s-xu</t>
+  </si>
+  <si>
+    <t>s-xt</t>
+  </si>
+  <si>
+    <t>Drug-Susceptible Smear-Negative Untreated</t>
+  </si>
+  <si>
+    <t>Drug-Susceptible Smear-Negative Treated</t>
+  </si>
+  <si>
+    <t>Multidrug-Resistant Smear-Negative Untreated</t>
+  </si>
+  <si>
+    <t>Multidrug-Resistant Smear-Negative Treated</t>
+  </si>
+  <si>
+    <t>Extensively Drug-Resistant Smear-Negative Untreated</t>
+  </si>
+  <si>
+    <t>Extensively Drug-Resistant Smear-Negative Treated</t>
+  </si>
+  <si>
+    <t>pudu</t>
+  </si>
+  <si>
+    <t>pudt</t>
+  </si>
+  <si>
+    <t>pumu</t>
+  </si>
+  <si>
+    <t>pumt</t>
+  </si>
+  <si>
+    <t>puxu</t>
+  </si>
+  <si>
+    <t>puxt</t>
+  </si>
+  <si>
+    <t>rec</t>
+  </si>
+  <si>
+    <t>dead</t>
+  </si>
+  <si>
+    <t>Recovered</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
     <t>Vaccinated</t>
-  </si>
-  <si>
-    <t>lte</t>
-  </si>
-  <si>
-    <t>Early-Stage Latent</t>
-  </si>
-  <si>
-    <t>s+e</t>
-  </si>
-  <si>
-    <t>Early-Stage Smear-Positive</t>
-  </si>
-  <si>
-    <t>s-e</t>
-  </si>
-  <si>
-    <t>Early-Stage Smear-Negative</t>
-  </si>
-  <si>
-    <t>pue</t>
-  </si>
-  <si>
-    <t>Early-Stage Pulmonary</t>
-  </si>
-  <si>
-    <t>ltsu</t>
-  </si>
-  <si>
-    <t>ltfu</t>
-  </si>
-  <si>
-    <t>Slow Latent Untreated</t>
-  </si>
-  <si>
-    <t>Fast Latent Untreated</t>
-  </si>
-  <si>
-    <t>ltst</t>
-  </si>
-  <si>
-    <t>ltft</t>
-  </si>
-  <si>
-    <t>Slow Latent Treated</t>
-  </si>
-  <si>
-    <t>Fast Latent Treated</t>
-  </si>
-  <si>
-    <t>s+du</t>
-  </si>
-  <si>
-    <t>Drug-Susceptible Smear-Positive Untreated</t>
-  </si>
-  <si>
-    <t>s+dt</t>
-  </si>
-  <si>
-    <t>Drug-Susceptible Smear-Positive Treated</t>
-  </si>
-  <si>
-    <t>s+mu</t>
-  </si>
-  <si>
-    <t>s+mt</t>
-  </si>
-  <si>
-    <t>s+xu</t>
-  </si>
-  <si>
-    <t>s+xt</t>
-  </si>
-  <si>
-    <t>Multidrug-Resistant Smear-Positive Untreated</t>
-  </si>
-  <si>
-    <t>Multidrug-Resistant Smear-Positive Treated</t>
-  </si>
-  <si>
-    <t>Extensively Drug-Resistant Smear-Positive Untreated</t>
-  </si>
-  <si>
-    <t>Extensively Drug-Resistant Smear-Positive Treated</t>
-  </si>
-  <si>
-    <t>s-du</t>
-  </si>
-  <si>
-    <t>s-dt</t>
-  </si>
-  <si>
-    <t>s-mu</t>
-  </si>
-  <si>
-    <t>s-mt</t>
-  </si>
-  <si>
-    <t>s-xu</t>
-  </si>
-  <si>
-    <t>s-xt</t>
-  </si>
-  <si>
-    <t>Drug-Susceptible Smear-Negative Untreated</t>
-  </si>
-  <si>
-    <t>Drug-Susceptible Smear-Negative Treated</t>
-  </si>
-  <si>
-    <t>Multidrug-Resistant Smear-Negative Untreated</t>
-  </si>
-  <si>
-    <t>Multidrug-Resistant Smear-Negative Treated</t>
-  </si>
-  <si>
-    <t>Extensively Drug-Resistant Smear-Negative Untreated</t>
-  </si>
-  <si>
-    <t>Extensively Drug-Resistant Smear-Negative Treated</t>
-  </si>
-  <si>
-    <t>pudu</t>
-  </si>
-  <si>
-    <t>pudt</t>
-  </si>
-  <si>
-    <t>pumu</t>
-  </si>
-  <si>
-    <t>pumt</t>
-  </si>
-  <si>
-    <t>puxu</t>
-  </si>
-  <si>
-    <t>puxt</t>
-  </si>
-  <si>
-    <t>rec</t>
-  </si>
-  <si>
-    <t>dead</t>
-  </si>
-  <si>
-    <t>Recovered</t>
-  </si>
-  <si>
-    <t>Dead</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,231 +563,231 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
         <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
         <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -817,88 +817,88 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
-        <v>29</v>
-      </c>
       <c r="P1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" t="s">
         <v>34</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>37</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" t="s">
-        <v>39</v>
-      </c>
       <c r="W1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>50</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>52</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
@@ -913,142 +913,142 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transitions worksheet handling with quality checks
Settings object can now load up an appropriate arbitrary transitions
matrix between nodes. Each transition must currently have a unique
label.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Choose your own cascade
Node/Link cascade files have been designed for simple network
(cascade-simple.xlsx) and the default complex one (cascade.xlsx).
Run model.py after choosing which to load with settings.
Note that 2000 to 2030 in timesteps of 0.25 take about half a minute on
my machine to run for two populations in the full cascade.
That's not promising, given what is left to be implemented.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="134">
   <si>
     <t>Code Label</t>
   </si>
@@ -183,13 +183,247 @@
   </si>
   <si>
     <t>Vaccinated</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>ag</t>
+  </si>
+  <si>
+    <t>ah</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>bd</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>bf</t>
+  </si>
+  <si>
+    <t>bg</t>
+  </si>
+  <si>
+    <t>bh</t>
+  </si>
+  <si>
+    <t>bi</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>cb</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>ce</t>
+  </si>
+  <si>
+    <t>cf</t>
+  </si>
+  <si>
+    <t>cg</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>ci</t>
+  </si>
+  <si>
+    <t>aj</t>
+  </si>
+  <si>
+    <t>ak</t>
+  </si>
+  <si>
+    <t>al</t>
+  </si>
+  <si>
+    <t>bj</t>
+  </si>
+  <si>
+    <t>bk</t>
+  </si>
+  <si>
+    <t>bl</t>
+  </si>
+  <si>
+    <t>cj</t>
+  </si>
+  <si>
+    <t>ck</t>
+  </si>
+  <si>
+    <t>cl</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>an</t>
+  </si>
+  <si>
+    <t>ao</t>
+  </si>
+  <si>
+    <t>ap</t>
+  </si>
+  <si>
+    <t>aq</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>bm</t>
+  </si>
+  <si>
+    <t>bn</t>
+  </si>
+  <si>
+    <t>bo</t>
+  </si>
+  <si>
+    <t>bp</t>
+  </si>
+  <si>
+    <t>bq</t>
+  </si>
+  <si>
+    <t>br</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>cn</t>
+  </si>
+  <si>
+    <t>co</t>
+  </si>
+  <si>
+    <t>cp</t>
+  </si>
+  <si>
+    <t>cq</t>
+  </si>
+  <si>
+    <t>cr</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,16 +439,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -222,15 +492,140 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,256 +1195,1313 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="31" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="8"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="11"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="11"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="11"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE6" s="11"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="11"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE8" s="11"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" s="8"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="8"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="11" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE11" s="11" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="11" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE13" s="11" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="11" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="O15" s="14"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE15" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="V16" s="8"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="8"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE18" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="U19" s="10"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AE20" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="W21" s="9"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="V22" s="14"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AC22" s="14"/>
+      <c r="AD22" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE22" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="8"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="10"/>
+      <c r="AB24" s="10"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="10"/>
+      <c r="AE24" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE25" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="10"/>
+      <c r="AE26" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="11"/>
+      <c r="AD27" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE27" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="10"/>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD28" s="10"/>
+      <c r="AE28" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="14"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
+      <c r="Z29" s="13"/>
+      <c r="AA29" s="13"/>
+      <c r="AB29" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC29" s="14"/>
+      <c r="AD29" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE29" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="11"/>
+      <c r="AD30" s="10"/>
+      <c r="AE30" s="11"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="13"/>
+      <c r="AB31" s="13"/>
+      <c r="AC31" s="14"/>
+      <c r="AD31" s="13"/>
+      <c r="AE31" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Transition parameters completed for full cascade
Running project.py should plot both cascades, although viewing the full
cascade is not reasonable at this time.
Either way, parameters corresponding to links are within the settings
object.
Next up on the agenda is setting defaults in the cascade sheet and maybe
even generating a country data spreadsheet from this...
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
     <sheet name="Transitions" sheetId="2" r:id="rId2"/>
+    <sheet name="Transition Parameters" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="291">
   <si>
     <t>Code Label</t>
   </si>
@@ -417,6 +418,477 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Vaccination Rate</t>
+  </si>
+  <si>
+    <t>Infection Rate (Susceptible)</t>
+  </si>
+  <si>
+    <t>Infection Rate (Vaccinated)</t>
+  </si>
+  <si>
+    <t>Slow-LTBI Partition Fraction</t>
+  </si>
+  <si>
+    <t>Fast-LTBI Partition Fraction</t>
+  </si>
+  <si>
+    <t>Slow-LTBI Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>Slow-LTBI Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>Fast-LTBI Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>Fast-LTBI Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Slow Untreated)</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Slow Treated)</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Fast Untreated)</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Fast Treated)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Slow Untreated)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Slow Treated)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Fast Untreated)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Fast Treated)</t>
+  </si>
+  <si>
+    <t>LTBI-Pulm Progression Rate (Slow Untreated)</t>
+  </si>
+  <si>
+    <t>LTBI-Pulm Progression Rate (Slow Treated)</t>
+  </si>
+  <si>
+    <t>LTBI-Pulm Progression Rate (Fast Untreated)</t>
+  </si>
+  <si>
+    <t>LTBI-Pulm Progression Rate (Fast Treated)</t>
+  </si>
+  <si>
+    <t>Slow-LTBI Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>Fast-LTBI Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>Reinfection Rate (Recovered)</t>
+  </si>
+  <si>
+    <t>SPos MDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>SPos XDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>SPos DS Partition Fraction</t>
+  </si>
+  <si>
+    <t>SPos DS Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SPos DS Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SPos MDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SPos MDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SPos XDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SPos XDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SPos DS Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SPos MDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SPos XDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SPos DS Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>SPos DS Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SPos MDR Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>SPos MDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SPos XDR Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>SPos XDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SNeg DS Partition Fraction</t>
+  </si>
+  <si>
+    <t>SNeg MDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>SNeg XDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>SNeg DS Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SNeg DS Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SNeg MDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SNeg MDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SNeg XDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SNeg XDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SNeg DS Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SNeg MDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SNeg XDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SNeg DS Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>SNeg DS Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SNeg MDR Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>SNeg MDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SNeg XDR Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>SNeg XDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>Pulm DS Partition Fraction</t>
+  </si>
+  <si>
+    <t>Pulm MDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>Pulm XDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>Pulm DS Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>Pulm DS Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>Pulm MDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>Pulm MDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>Pulm XDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>Pulm XDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>Pulm DS Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>Pulm MDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>Pulm XDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>Pulm DS Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>Pulm DS Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>Pulm MDR Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>Pulm MDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>Pulm XDR Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>Pulm XDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>v_rate</t>
+  </si>
+  <si>
+    <t>infs_rate</t>
+  </si>
+  <si>
+    <t>infv_rate</t>
+  </si>
+  <si>
+    <t>lts_frac</t>
+  </si>
+  <si>
+    <t>ltf_frac</t>
+  </si>
+  <si>
+    <t>ltsyes_rate</t>
+  </si>
+  <si>
+    <t>ltsno_rate</t>
+  </si>
+  <si>
+    <t>ltfyes_rate</t>
+  </si>
+  <si>
+    <t>ltfno_rate</t>
+  </si>
+  <si>
+    <t>ltsus+_rate</t>
+  </si>
+  <si>
+    <t>ltsts+_rate</t>
+  </si>
+  <si>
+    <t>ltfus+_rate</t>
+  </si>
+  <si>
+    <t>ltfts+_rate</t>
+  </si>
+  <si>
+    <t>ltsus-_rate</t>
+  </si>
+  <si>
+    <t>ltsts-_rate</t>
+  </si>
+  <si>
+    <t>ltfus-_rate</t>
+  </si>
+  <si>
+    <t>ltfts-_rate</t>
+  </si>
+  <si>
+    <t>ltsupu_rate</t>
+  </si>
+  <si>
+    <t>ltstpu_rate</t>
+  </si>
+  <si>
+    <t>ltfupu_rate</t>
+  </si>
+  <si>
+    <t>ltftpu_rate</t>
+  </si>
+  <si>
+    <t>infr_rate</t>
+  </si>
+  <si>
+    <t>ltssuc_rate</t>
+  </si>
+  <si>
+    <t>ltfsuc_rate</t>
+  </si>
+  <si>
+    <t>s+d_frac</t>
+  </si>
+  <si>
+    <t>s+m_frac</t>
+  </si>
+  <si>
+    <t>s+x_frac</t>
+  </si>
+  <si>
+    <t>s+dyes_rate</t>
+  </si>
+  <si>
+    <t>s+dno_rate</t>
+  </si>
+  <si>
+    <t>s+myes_rate</t>
+  </si>
+  <si>
+    <t>s+mno_rate</t>
+  </si>
+  <si>
+    <t>s+xyes_rate</t>
+  </si>
+  <si>
+    <t>s+xno_rate</t>
+  </si>
+  <si>
+    <t>s+dsuc_rate</t>
+  </si>
+  <si>
+    <t>s+msuc_rate</t>
+  </si>
+  <si>
+    <t>s+xsuc_rate</t>
+  </si>
+  <si>
+    <t>s+dud_rate</t>
+  </si>
+  <si>
+    <t>s+dtd_rate</t>
+  </si>
+  <si>
+    <t>s+mud_rate</t>
+  </si>
+  <si>
+    <t>s+mtd_rate</t>
+  </si>
+  <si>
+    <t>s+xud_rate</t>
+  </si>
+  <si>
+    <t>s+xtd_rate</t>
+  </si>
+  <si>
+    <t>s-d_frac</t>
+  </si>
+  <si>
+    <t>s-m_frac</t>
+  </si>
+  <si>
+    <t>s-x_frac</t>
+  </si>
+  <si>
+    <t>s-dyes_rate</t>
+  </si>
+  <si>
+    <t>s-dno_rate</t>
+  </si>
+  <si>
+    <t>s-myes_rate</t>
+  </si>
+  <si>
+    <t>s-mno_rate</t>
+  </si>
+  <si>
+    <t>s-xyes_rate</t>
+  </si>
+  <si>
+    <t>s-xno_rate</t>
+  </si>
+  <si>
+    <t>s-dsuc_rate</t>
+  </si>
+  <si>
+    <t>s-msuc_rate</t>
+  </si>
+  <si>
+    <t>s-xsuc_rate</t>
+  </si>
+  <si>
+    <t>s-dud_rate</t>
+  </si>
+  <si>
+    <t>s-dtd_rate</t>
+  </si>
+  <si>
+    <t>s-mud_rate</t>
+  </si>
+  <si>
+    <t>s-mtd_rate</t>
+  </si>
+  <si>
+    <t>s-xud_rate</t>
+  </si>
+  <si>
+    <t>s-xtd_rate</t>
+  </si>
+  <si>
+    <t>pud_frac</t>
+  </si>
+  <si>
+    <t>pum_frac</t>
+  </si>
+  <si>
+    <t>pux_frac</t>
+  </si>
+  <si>
+    <t>pudyes_rate</t>
+  </si>
+  <si>
+    <t>pudno_rate</t>
+  </si>
+  <si>
+    <t>pumyes_rate</t>
+  </si>
+  <si>
+    <t>pumno_rate</t>
+  </si>
+  <si>
+    <t>puxyes_rate</t>
+  </si>
+  <si>
+    <t>puxno_rate</t>
+  </si>
+  <si>
+    <t>pudsuc_rate</t>
+  </si>
+  <si>
+    <t>pumsuc_rate</t>
+  </si>
+  <si>
+    <t>puxsuc_rate</t>
+  </si>
+  <si>
+    <t>pudud_rate</t>
+  </si>
+  <si>
+    <t>pudtd_rate</t>
+  </si>
+  <si>
+    <t>pumud_rate</t>
+  </si>
+  <si>
+    <t>pumtd_rate</t>
+  </si>
+  <si>
+    <t>puxud_rate</t>
+  </si>
+  <si>
+    <t>puxtd_rate</t>
   </si>
 </sst>
 </file>
@@ -579,7 +1051,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -619,6 +1091,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -927,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -2506,4 +2981,893 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>228</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>229</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>235</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>236</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>234</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>238</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>239</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>241</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>242</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>243</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>244</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>245</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>246</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>247</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>248</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>249</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>250</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>251</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>252</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>253</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>254</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>255</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>256</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>257</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>259</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>260</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>262</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>263</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>264</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>265</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>266</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>267</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>268</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>269</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>270</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>271</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>272</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>273</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>274</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>275</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>276</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>277</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C66" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>278</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>279</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>280</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C69" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>281</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>282</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>283</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>284</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>285</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C74" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>286</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C75" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>287</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>288</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C77" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>289</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C78" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>290</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement cascade plot coordinates
Cascade spreadsheet now allows for an optional 'Plot Coordinates'
column, giving finer control in plotting schematics.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="322">
   <si>
     <t>Code Label</t>
   </si>
@@ -889,6 +889,99 @@
   </si>
   <si>
     <t>puxtd_rate</t>
+  </si>
+  <si>
+    <t>Plot Coordinates</t>
+  </si>
+  <si>
+    <t>(-8.5,1)</t>
+  </si>
+  <si>
+    <t>(-7.5,0)</t>
+  </si>
+  <si>
+    <t>(-6.5,1)</t>
+  </si>
+  <si>
+    <t>(-5.5,0)</t>
+  </si>
+  <si>
+    <t>(-4.5,1)</t>
+  </si>
+  <si>
+    <t>(-3.5,0)</t>
+  </si>
+  <si>
+    <t>(-2.5,1)</t>
+  </si>
+  <si>
+    <t>(-1.5,0)</t>
+  </si>
+  <si>
+    <t>(-0.5,1)</t>
+  </si>
+  <si>
+    <t>(0.5,0)</t>
+  </si>
+  <si>
+    <t>(1.5,1)</t>
+  </si>
+  <si>
+    <t>(2.5,0)</t>
+  </si>
+  <si>
+    <t>(3.5,1)</t>
+  </si>
+  <si>
+    <t>(4.5,0)</t>
+  </si>
+  <si>
+    <t>(5.5,1)</t>
+  </si>
+  <si>
+    <t>(6.5,0)</t>
+  </si>
+  <si>
+    <t>(7.5,1)</t>
+  </si>
+  <si>
+    <t>(8.5,0)</t>
+  </si>
+  <si>
+    <t>(-6,2)</t>
+  </si>
+  <si>
+    <t>(6,2)</t>
+  </si>
+  <si>
+    <t>(0,2)</t>
+  </si>
+  <si>
+    <t>(0,-1)</t>
+  </si>
+  <si>
+    <t>(4,-1)</t>
+  </si>
+  <si>
+    <t>(-2,3)</t>
+  </si>
+  <si>
+    <t>(-6,3)</t>
+  </si>
+  <si>
+    <t>(2,3)</t>
+  </si>
+  <si>
+    <t>(6,3)</t>
+  </si>
+  <si>
+    <t>(0,4)</t>
+  </si>
+  <si>
+    <t>(-3,5)</t>
+  </si>
+  <si>
+    <t>(3,5)</t>
   </si>
 </sst>
 </file>
@@ -1400,264 +1493,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="15" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
       <c r="B19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
       <c r="B22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>46</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>47</v>
       </c>
       <c r="B26" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
       <c r="B27" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>49</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>50</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>51</v>
       </c>
       <c r="B30" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
       <c r="B31" t="s">
         <v>54</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2987,7 +3174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improved full cascade coordinates
Just a minor tweak to plot schematic arrangement. Basically a sanity
check.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -894,75 +894,12 @@
     <t>Plot Coordinates</t>
   </si>
   <si>
-    <t>(-8.5,1)</t>
-  </si>
-  <si>
-    <t>(-7.5,0)</t>
-  </si>
-  <si>
-    <t>(-6.5,1)</t>
-  </si>
-  <si>
-    <t>(-5.5,0)</t>
-  </si>
-  <si>
-    <t>(-4.5,1)</t>
-  </si>
-  <si>
-    <t>(-3.5,0)</t>
-  </si>
-  <si>
-    <t>(-2.5,1)</t>
-  </si>
-  <si>
-    <t>(-1.5,0)</t>
-  </si>
-  <si>
-    <t>(-0.5,1)</t>
-  </si>
-  <si>
-    <t>(0.5,0)</t>
-  </si>
-  <si>
-    <t>(1.5,1)</t>
-  </si>
-  <si>
-    <t>(2.5,0)</t>
-  </si>
-  <si>
-    <t>(3.5,1)</t>
-  </si>
-  <si>
-    <t>(4.5,0)</t>
-  </si>
-  <si>
-    <t>(5.5,1)</t>
-  </si>
-  <si>
-    <t>(6.5,0)</t>
-  </si>
-  <si>
-    <t>(7.5,1)</t>
-  </si>
-  <si>
-    <t>(8.5,0)</t>
-  </si>
-  <si>
-    <t>(-6,2)</t>
-  </si>
-  <si>
-    <t>(6,2)</t>
-  </si>
-  <si>
     <t>(0,2)</t>
   </si>
   <si>
     <t>(0,-1)</t>
   </si>
   <si>
-    <t>(4,-1)</t>
-  </si>
-  <si>
     <t>(-2,3)</t>
   </si>
   <si>
@@ -982,6 +919,69 @@
   </si>
   <si>
     <t>(3,5)</t>
+  </si>
+  <si>
+    <t>(-2,1)</t>
+  </si>
+  <si>
+    <t>(-2,-1)</t>
+  </si>
+  <si>
+    <t>(0,1)</t>
+  </si>
+  <si>
+    <t>(2,1)</t>
+  </si>
+  <si>
+    <t>(2,-1)</t>
+  </si>
+  <si>
+    <t>(-8,2)</t>
+  </si>
+  <si>
+    <t>(-10,1)</t>
+  </si>
+  <si>
+    <t>(-10,-1)</t>
+  </si>
+  <si>
+    <t>(-8,1)</t>
+  </si>
+  <si>
+    <t>(-8,-1)</t>
+  </si>
+  <si>
+    <t>(-6,1)</t>
+  </si>
+  <si>
+    <t>(-6,-1)</t>
+  </si>
+  <si>
+    <t>(8,2)</t>
+  </si>
+  <si>
+    <t>(6,1)</t>
+  </si>
+  <si>
+    <t>(6,-1)</t>
+  </si>
+  <si>
+    <t>(8,1)</t>
+  </si>
+  <si>
+    <t>(8,-1)</t>
+  </si>
+  <si>
+    <t>(10,1)</t>
+  </si>
+  <si>
+    <t>(10,-1)</t>
+  </si>
+  <si>
+    <t>(-4,0)</t>
+  </si>
+  <si>
+    <t>(4,0)</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1496,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1525,7 +1525,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1536,7 +1536,7 @@
         <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1547,7 +1547,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1558,7 +1558,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1569,7 +1569,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1580,7 +1580,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1591,7 +1591,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1602,7 +1602,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1613,7 +1613,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1624,7 +1624,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1635,7 +1635,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1646,7 +1646,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1657,7 +1657,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1668,7 +1668,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1679,7 +1679,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1690,7 +1690,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1701,7 +1701,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1712,7 +1712,7 @@
         <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1723,7 +1723,7 @@
         <v>42</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1734,7 +1734,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1745,7 +1745,7 @@
         <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1756,7 +1756,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1767,7 +1767,7 @@
         <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1778,7 +1778,7 @@
         <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1789,7 +1789,7 @@
         <v>41</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1800,7 +1800,7 @@
         <v>42</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1811,7 +1811,7 @@
         <v>43</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1822,7 +1822,7 @@
         <v>44</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1833,7 +1833,7 @@
         <v>53</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1844,7 +1844,7 @@
         <v>54</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Default values in cascade
The modded data-book is no longer necessary as the cascade sheets now
allow for a column of default values (assumptions) to be specified for
link parameters.
Currently, cascade.xlsx has a few values that create a state cycle
involving early latent, untreated fast latent, early smear positive,
untreated smear positive, treated smear positive and recovered.
Also; the previous issue involving an equation not being calculated if
the generated xlsx file is not opened/saved in Excel before loading?
That applies to all equations.
Default values must be included with each call to the xlsxwriter write
function.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="323">
   <si>
     <t>Code Label</t>
   </si>
@@ -982,6 +982,9 @@
   </si>
   <si>
     <t>(4,0)</t>
+  </si>
+  <si>
+    <t>Default Value</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -3172,10 +3175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3183,9 +3186,10 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
     <col min="3" max="3" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3195,8 +3199,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="15" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>213</v>
       </c>
@@ -3207,7 +3214,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -3217,8 +3224,11 @@
       <c r="C3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -3229,7 +3239,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -3240,7 +3250,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>217</v>
       </c>
@@ -3250,8 +3260,11 @@
       <c r="C6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>218</v>
       </c>
@@ -3262,7 +3275,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>219</v>
       </c>
@@ -3273,7 +3286,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>220</v>
       </c>
@@ -3284,7 +3297,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>221</v>
       </c>
@@ -3295,7 +3308,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>222</v>
       </c>
@@ -3306,7 +3319,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -3317,7 +3330,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -3327,8 +3340,11 @@
       <c r="C13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>225</v>
       </c>
@@ -3339,7 +3355,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>226</v>
       </c>
@@ -3350,7 +3366,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>227</v>
       </c>
@@ -3361,7 +3377,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>228</v>
       </c>
@@ -3372,7 +3388,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>229</v>
       </c>
@@ -3383,7 +3399,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>230</v>
       </c>
@@ -3394,7 +3410,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>231</v>
       </c>
@@ -3405,7 +3421,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>232</v>
       </c>
@@ -3416,7 +3432,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>233</v>
       </c>
@@ -3427,7 +3443,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>235</v>
       </c>
@@ -3438,7 +3454,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>236</v>
       </c>
@@ -3449,7 +3465,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>234</v>
       </c>
@@ -3459,8 +3475,11 @@
       <c r="C25" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>237</v>
       </c>
@@ -3470,8 +3489,11 @@
       <c r="C26" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>238</v>
       </c>
@@ -3482,7 +3504,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>239</v>
       </c>
@@ -3493,7 +3515,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>240</v>
       </c>
@@ -3503,8 +3525,11 @@
       <c r="C29" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>241</v>
       </c>
@@ -3515,7 +3540,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>242</v>
       </c>
@@ -3526,7 +3551,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>243</v>
       </c>
@@ -3537,7 +3562,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>244</v>
       </c>
@@ -3548,7 +3573,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>245</v>
       </c>
@@ -3559,7 +3584,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>246</v>
       </c>
@@ -3569,8 +3594,11 @@
       <c r="C35" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>247</v>
       </c>
@@ -3581,7 +3609,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>248</v>
       </c>
@@ -3592,7 +3620,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>249</v>
       </c>
@@ -3603,7 +3631,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>250</v>
       </c>
@@ -3614,7 +3642,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>251</v>
       </c>
@@ -3625,7 +3653,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>252</v>
       </c>
@@ -3636,7 +3664,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>253</v>
       </c>
@@ -3647,7 +3675,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>254</v>
       </c>
@@ -3658,7 +3686,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>255</v>
       </c>
@@ -3669,7 +3697,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>256</v>
       </c>
@@ -3680,7 +3708,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>257</v>
       </c>
@@ -3691,7 +3719,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>258</v>
       </c>
@@ -3702,7 +3730,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>259</v>
       </c>
@@ -4056,5 +4084,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor cascade sheet reordering
The order of parameters in the cascade transition parameter sheet is the
order that is used in generating a project databook.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -1822,7 +1822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -4543,8 +4543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4607,1137 +4607,1134 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>144</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>358</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>312</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>343</v>
+        <v>212</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>328</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>359</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>58</v>
+        <v>313</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>344</v>
+        <v>197</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>329</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>345</v>
+        <v>213</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>330</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
+        <v>314</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>322</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>347</v>
+        <v>201</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>315</v>
       </c>
       <c r="C19" t="s">
-        <v>332</v>
+        <v>323</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>344</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>140</v>
+        <v>329</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>348</v>
+        <v>202</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>333</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>316</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>212</v>
+        <v>345</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>125</v>
+        <v>317</v>
       </c>
       <c r="C25" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>214</v>
+        <v>346</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
+        <v>318</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>217</v>
+        <v>347</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
+        <v>332</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>76</v>
+        <v>319</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>327</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>220</v>
+        <v>348</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>151</v>
+        <v>333</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>153</v>
+        <v>147</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
-      </c>
-      <c r="D35" s="2">
-        <v>1</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>225</v>
+        <v>378</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>100</v>
+        <v>360</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>369</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>349</v>
+        <v>217</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>334</v>
+        <v>148</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>350</v>
+        <v>223</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C40" t="s">
-        <v>335</v>
+        <v>154</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>229</v>
+        <v>379</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>110</v>
+        <v>361</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>351</v>
+        <v>219</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>336</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>233</v>
+        <v>380</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>81</v>
+        <v>362</v>
       </c>
       <c r="C45" t="s">
-        <v>161</v>
+        <v>371</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>85</v>
+        <v>387</v>
       </c>
       <c r="C49" t="s">
-        <v>165</v>
+        <v>396</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>238</v>
+        <v>349</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="C50" t="s">
-        <v>166</v>
+        <v>334</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="C51" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>88</v>
+        <v>388</v>
       </c>
       <c r="C52" t="s">
-        <v>168</v>
+        <v>397</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>241</v>
+        <v>350</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>169</v>
+        <v>335</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>103</v>
+        <v>389</v>
       </c>
       <c r="C55" t="s">
-        <v>171</v>
+        <v>398</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C56" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C57" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>353</v>
+        <v>232</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>338</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>354</v>
+        <v>234</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>339</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>249</v>
+        <v>381</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>118</v>
+        <v>363</v>
       </c>
       <c r="C61" t="s">
-        <v>174</v>
+        <v>372</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C64" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>253</v>
+        <v>382</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>92</v>
+        <v>364</v>
       </c>
       <c r="C65" t="s">
-        <v>178</v>
+        <v>373</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C68" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>257</v>
+        <v>383</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>96</v>
+        <v>365</v>
       </c>
       <c r="C69" t="s">
-        <v>182</v>
+        <v>374</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C70" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C71" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>106</v>
+        <v>390</v>
       </c>
       <c r="C73" t="s">
-        <v>186</v>
+        <v>399</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C74" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C75" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>356</v>
+        <v>246</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>121</v>
+        <v>391</v>
       </c>
       <c r="C76" t="s">
-        <v>341</v>
+        <v>400</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>265</v>
+        <v>353</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C77" t="s">
-        <v>188</v>
+        <v>338</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>357</v>
+        <v>247</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C78" t="s">
-        <v>342</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>124</v>
+        <v>392</v>
       </c>
       <c r="C79" t="s">
-        <v>189</v>
+        <v>401</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>312</v>
+        <v>117</v>
       </c>
       <c r="C80" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>359</v>
+        <v>249</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>313</v>
+        <v>118</v>
       </c>
       <c r="C81" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>199</v>
+        <v>250</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>314</v>
+        <v>89</v>
       </c>
       <c r="C82" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>315</v>
+        <v>90</v>
       </c>
       <c r="C83" t="s">
-        <v>323</v>
-      </c>
-      <c r="D83" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>203</v>
+        <v>252</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>316</v>
+        <v>91</v>
       </c>
       <c r="C84" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>205</v>
+        <v>384</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>317</v>
+        <v>366</v>
       </c>
       <c r="C85" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>207</v>
+        <v>253</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>318</v>
+        <v>92</v>
       </c>
       <c r="C86" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>209</v>
+        <v>254</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>319</v>
+        <v>93</v>
       </c>
       <c r="C87" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>378</v>
+        <v>259</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>360</v>
+        <v>104</v>
       </c>
       <c r="C88" t="s">
-        <v>369</v>
-      </c>
-      <c r="D88" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="C89" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>380</v>
+        <v>255</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>362</v>
+        <v>94</v>
       </c>
       <c r="C90" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>381</v>
+        <v>256</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>363</v>
+        <v>95</v>
       </c>
       <c r="C91" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>382</v>
+        <v>260</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>364</v>
+        <v>105</v>
       </c>
       <c r="C92" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C93" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>384</v>
+        <v>257</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>366</v>
+        <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>385</v>
+        <v>258</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>367</v>
+        <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>386</v>
+        <v>261</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>368</v>
+        <v>106</v>
       </c>
       <c r="C96" t="s">
-        <v>377</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="C97" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>228</v>
+        <v>355</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>388</v>
+        <v>119</v>
       </c>
       <c r="C98" t="s">
-        <v>397</v>
+        <v>340</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>230</v>
+        <v>263</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>389</v>
+        <v>120</v>
       </c>
       <c r="C99" t="s">
-        <v>398</v>
+        <v>187</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C100" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>246</v>
+        <v>356</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>391</v>
+        <v>121</v>
       </c>
       <c r="C101" t="s">
-        <v>400</v>
+        <v>341</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>392</v>
+        <v>122</v>
       </c>
       <c r="C102" t="s">
-        <v>401</v>
+        <v>188</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C103" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>264</v>
+        <v>357</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>394</v>
+        <v>123</v>
       </c>
       <c r="C104" t="s">
-        <v>403</v>
+        <v>342</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>395</v>
+        <v>124</v>
       </c>
       <c r="C105" t="s">
-        <v>404</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extrapulmonary states cut from cascade
Old 'full' cascade is saved as a backup, although it may be deleted
within some time, due to commits.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Transitions" sheetId="2" r:id="rId2"/>
     <sheet name="Transition Parameters" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="320">
   <si>
     <t>Code Label</t>
   </si>
@@ -51,12 +51,6 @@
     <t>Early-Stage Smear-Negative</t>
   </si>
   <si>
-    <t>pue</t>
-  </si>
-  <si>
-    <t>Early-Stage Pulmonary</t>
-  </si>
-  <si>
     <t>ltsu</t>
   </si>
   <si>
@@ -129,24 +123,6 @@
     <t>Extensively Drug-Resistant Smear-Negative Treated</t>
   </si>
   <si>
-    <t>pudu</t>
-  </si>
-  <si>
-    <t>pudt</t>
-  </si>
-  <si>
-    <t>pumu</t>
-  </si>
-  <si>
-    <t>pumt</t>
-  </si>
-  <si>
-    <t>puxu</t>
-  </si>
-  <si>
-    <t>puxt</t>
-  </si>
-  <si>
     <t>rec</t>
   </si>
   <si>
@@ -213,18 +189,6 @@
     <t>q</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
@@ -285,33 +249,6 @@
     <t>bi</t>
   </si>
   <si>
-    <t>ca</t>
-  </si>
-  <si>
-    <t>cb</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>cd</t>
-  </si>
-  <si>
-    <t>ce</t>
-  </si>
-  <si>
-    <t>cf</t>
-  </si>
-  <si>
-    <t>cg</t>
-  </si>
-  <si>
-    <t>ch</t>
-  </si>
-  <si>
-    <t>ci</t>
-  </si>
-  <si>
     <t>aj</t>
   </si>
   <si>
@@ -330,15 +267,6 @@
     <t>bl</t>
   </si>
   <si>
-    <t>cj</t>
-  </si>
-  <si>
-    <t>ck</t>
-  </si>
-  <si>
-    <t>cl</t>
-  </si>
-  <si>
     <t>am</t>
   </si>
   <si>
@@ -375,24 +303,6 @@
     <t>br</t>
   </si>
   <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>cn</t>
-  </si>
-  <si>
-    <t>co</t>
-  </si>
-  <si>
-    <t>cp</t>
-  </si>
-  <si>
-    <t>cq</t>
-  </si>
-  <si>
-    <t>cr</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -438,12 +348,6 @@
     <t>LTBI-SNeg Progression Rate (Fast Treated)</t>
   </si>
   <si>
-    <t>LTBI-Pulm Progression Rate (Slow Treated)</t>
-  </si>
-  <si>
-    <t>LTBI-Pulm Progression Rate (Fast Treated)</t>
-  </si>
-  <si>
     <t>Slow-LTBI Treatment Success Rate</t>
   </si>
   <si>
@@ -543,51 +447,6 @@
     <t>SNeg XDR Death Rate (Treated)</t>
   </si>
   <si>
-    <t>Pulm DS Partition Fraction</t>
-  </si>
-  <si>
-    <t>Pulm MDR Partition Fraction</t>
-  </si>
-  <si>
-    <t>Pulm XDR Partition Fraction</t>
-  </si>
-  <si>
-    <t>Pulm DS Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>Pulm DS Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>Pulm MDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>Pulm MDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>Pulm XDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>Pulm XDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>Pulm DS Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>Pulm MDR Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>Pulm XDR Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>Pulm DS Death Rate (Treated)</t>
-  </si>
-  <si>
-    <t>Pulm MDR Death Rate (Treated)</t>
-  </si>
-  <si>
-    <t>Pulm XDR Death Rate (Treated)</t>
-  </si>
-  <si>
     <t>v_rate</t>
   </si>
   <si>
@@ -639,18 +498,6 @@
     <t>ltfts-_rate</t>
   </si>
   <si>
-    <t>ltsupu_rate</t>
-  </si>
-  <si>
-    <t>ltstpu_rate</t>
-  </si>
-  <si>
-    <t>ltfupu_rate</t>
-  </si>
-  <si>
-    <t>ltftpu_rate</t>
-  </si>
-  <si>
     <t>infr_rate</t>
   </si>
   <si>
@@ -768,84 +615,9 @@
     <t>s-xtd_rate</t>
   </si>
   <si>
-    <t>pud_frac</t>
-  </si>
-  <si>
-    <t>pum_frac</t>
-  </si>
-  <si>
-    <t>pux_frac</t>
-  </si>
-  <si>
-    <t>pudyes_rate</t>
-  </si>
-  <si>
-    <t>pudno_rate</t>
-  </si>
-  <si>
-    <t>pumyes_rate</t>
-  </si>
-  <si>
-    <t>pumno_rate</t>
-  </si>
-  <si>
-    <t>puxyes_rate</t>
-  </si>
-  <si>
-    <t>puxno_rate</t>
-  </si>
-  <si>
-    <t>pudsuc_rate</t>
-  </si>
-  <si>
-    <t>pumsuc_rate</t>
-  </si>
-  <si>
-    <t>puxsuc_rate</t>
-  </si>
-  <si>
-    <t>pudud_rate</t>
-  </si>
-  <si>
-    <t>pudtd_rate</t>
-  </si>
-  <si>
-    <t>pumud_rate</t>
-  </si>
-  <si>
-    <t>pumtd_rate</t>
-  </si>
-  <si>
-    <t>puxud_rate</t>
-  </si>
-  <si>
-    <t>puxtd_rate</t>
-  </si>
-  <si>
     <t>Plot Coordinates</t>
   </si>
   <si>
-    <t>(0,2)</t>
-  </si>
-  <si>
-    <t>(0,-1)</t>
-  </si>
-  <si>
-    <t>(-2,1)</t>
-  </si>
-  <si>
-    <t>(-2,-1)</t>
-  </si>
-  <si>
-    <t>(0,1)</t>
-  </si>
-  <si>
-    <t>(2,1)</t>
-  </si>
-  <si>
-    <t>(2,-1)</t>
-  </si>
-  <si>
     <t>(-10,1)</t>
   </si>
   <si>
@@ -921,15 +693,6 @@
     <t>Extensively Drug-Resistant Smear-Negative Diagnosed</t>
   </si>
   <si>
-    <t>pudd</t>
-  </si>
-  <si>
-    <t>pumd</t>
-  </si>
-  <si>
-    <t>puxd</t>
-  </si>
-  <si>
     <t>Slow Latent Undiagnosed</t>
   </si>
   <si>
@@ -972,12 +735,6 @@
     <t>df</t>
   </si>
   <si>
-    <t>dg</t>
-  </si>
-  <si>
-    <t>dh</t>
-  </si>
-  <si>
     <t>Slow-LTBI Diagnosis Rate</t>
   </si>
   <si>
@@ -996,12 +753,6 @@
     <t>LTBI-SNeg Progression Rate (Fast Undiagnosed)</t>
   </si>
   <si>
-    <t>LTBI-Pulm Progression Rate (Slow Undiagnosed)</t>
-  </si>
-  <si>
-    <t>LTBI-Pulm Progression Rate (Fast Undiagnosed)</t>
-  </si>
-  <si>
     <t>LTBI-SPos Progression Rate (Slow Diagnosed)</t>
   </si>
   <si>
@@ -1014,12 +765,6 @@
     <t>LTBI-SNeg Progression Rate (Fast Diagnosed)</t>
   </si>
   <si>
-    <t>LTBI-Pulm Progression Rate (Slow Diagnosed)</t>
-  </si>
-  <si>
-    <t>LTBI-Pulm Progression Rate (Fast Diagnosed)</t>
-  </si>
-  <si>
     <t>SPos DS Death Rate (Diagnosed)</t>
   </si>
   <si>
@@ -1038,15 +783,6 @@
     <t>SNeg XDR Death Rate (Diagnosed)</t>
   </si>
   <si>
-    <t>Pulm DS Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>Pulm MDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>Pulm XDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
     <t>ltsds+_rate</t>
   </si>
   <si>
@@ -1059,12 +795,6 @@
     <t>ltfds-_rate</t>
   </si>
   <si>
-    <t>ltsdpu_rate</t>
-  </si>
-  <si>
-    <t>ltfdpu_rate</t>
-  </si>
-  <si>
     <t>s+ddd_rate</t>
   </si>
   <si>
@@ -1083,15 +813,6 @@
     <t>s-xdd_rate</t>
   </si>
   <si>
-    <t>puddd_rate</t>
-  </si>
-  <si>
-    <t>pumdd_rate</t>
-  </si>
-  <si>
-    <t>puxdd_rate</t>
-  </si>
-  <si>
     <t>ltsdiag_rate</t>
   </si>
   <si>
@@ -1116,15 +837,6 @@
     <t>ef</t>
   </si>
   <si>
-    <t>eg</t>
-  </si>
-  <si>
-    <t>eh</t>
-  </si>
-  <si>
-    <t>ei</t>
-  </si>
-  <si>
     <t>SPos DS Diagnosis Rate</t>
   </si>
   <si>
@@ -1143,15 +855,6 @@
     <t>SNeg XDR Diagnosis Rate</t>
   </si>
   <si>
-    <t>Pulm DS Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>Pulm MDR Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>Pulm XDR Diagnosis Rate</t>
-  </si>
-  <si>
     <t>s+ddiag_rate</t>
   </si>
   <si>
@@ -1170,15 +873,6 @@
     <t>s-xdiag_rate</t>
   </si>
   <si>
-    <t>puddiag_rate</t>
-  </si>
-  <si>
-    <t>pumdiag_rate</t>
-  </si>
-  <si>
-    <t>puxdiag_rate</t>
-  </si>
-  <si>
     <t>fa</t>
   </si>
   <si>
@@ -1197,15 +891,6 @@
     <t>ff</t>
   </si>
   <si>
-    <t>fg</t>
-  </si>
-  <si>
-    <t>fh</t>
-  </si>
-  <si>
-    <t>fi</t>
-  </si>
-  <si>
     <t>SPos DS Death Rate (Undiagnosed)</t>
   </si>
   <si>
@@ -1224,15 +909,6 @@
     <t>SNeg XDR Death Rate (Undiagnosed)</t>
   </si>
   <si>
-    <t>Pulm DS Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>Pulm MDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>Pulm XDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
     <t>(-12,1)</t>
   </si>
   <si>
@@ -1258,15 +934,6 @@
   </si>
   <si>
     <t>(-8,0)</t>
-  </si>
-  <si>
-    <t>(-2,0)</t>
-  </si>
-  <si>
-    <t>(0,0)</t>
-  </si>
-  <si>
-    <t>(2,0)</t>
   </si>
   <si>
     <t>(8,0)</t>
@@ -1820,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1841,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>268</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1852,7 +1519,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>430</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1860,10 +1527,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>429</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1874,73 +1541,73 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>428</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>304</v>
+        <v>225</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>424</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>285</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>210</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>425</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>422</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>305</v>
+        <v>226</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>426</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>287</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>212</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>427</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>423</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1951,106 +1618,106 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>409</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>306</v>
+        <v>227</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>405</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>289</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>290</v>
+        <v>214</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>411</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>406</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>307</v>
+        <v>228</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>276</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>291</v>
+        <v>215</v>
       </c>
       <c r="B16" t="s">
-        <v>292</v>
+        <v>216</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>412</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>277</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>229</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>278</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>293</v>
+        <v>217</v>
       </c>
       <c r="B19" t="s">
-        <v>294</v>
+        <v>218</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>413</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>279</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -2061,238 +1728,128 @@
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>269</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>309</v>
+        <v>230</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>271</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>295</v>
+        <v>219</v>
       </c>
       <c r="B23" t="s">
-        <v>296</v>
+        <v>220</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>414</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>272</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>310</v>
+        <v>231</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>273</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>297</v>
+        <v>221</v>
       </c>
       <c r="B26" t="s">
-        <v>298</v>
+        <v>222</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>415</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>270</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>311</v>
+        <v>232</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>299</v>
+        <v>223</v>
       </c>
       <c r="B29" t="s">
-        <v>300</v>
+        <v>224</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>416</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>410</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>309</v>
+        <v>38</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>301</v>
-      </c>
-      <c r="B33" t="s">
-        <v>296</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" t="s">
         <v>310</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>302</v>
-      </c>
-      <c r="B36" t="s">
-        <v>298</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" t="s">
-        <v>311</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>303</v>
-      </c>
-      <c r="B39" t="s">
-        <v>300</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -2303,18 +1860,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP42"/>
+  <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AP43" sqref="AP43"/>
+      <selection activeCell="AA39" sqref="AA39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="42" width="5.77734375" customWidth="1"/>
+    <col min="1" max="32" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -2326,130 +1883,100 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>289</v>
+        <v>213</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="U1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="V1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="X1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP1" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -2477,27 +2004,17 @@
       <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
       <c r="AD2" s="8"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7"/>
-      <c r="AM2" s="7"/>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="7"/>
-      <c r="AP2" s="8"/>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="8"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -2525,20 +2042,10 @@
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
       <c r="AD3" s="11"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="10"/>
-      <c r="AP3" s="11"/>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="11"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -2546,12 +2053,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="11"/>
@@ -2575,36 +2082,26 @@
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
       <c r="AD4" s="11"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="10"/>
-      <c r="AP4" s="11"/>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="11"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>312</v>
+        <v>233</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="11"/>
       <c r="K5" s="9" t="s">
-        <v>314</v>
+        <v>235</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
@@ -2616,7 +2113,7 @@
       <c r="S5" s="10"/>
       <c r="T5" s="11"/>
       <c r="U5" s="9" t="s">
-        <v>316</v>
+        <v>237</v>
       </c>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
@@ -2627,24 +2124,12 @@
       <c r="AB5" s="10"/>
       <c r="AC5" s="10"/>
       <c r="AD5" s="11"/>
-      <c r="AE5" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="AF5" s="10"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="10"/>
-      <c r="AL5" s="10"/>
-      <c r="AM5" s="10"/>
-      <c r="AN5" s="11"/>
-      <c r="AO5" s="10"/>
-      <c r="AP5" s="11"/>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="11"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>285</v>
+        <v>209</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
@@ -2652,13 +2137,13 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="11"/>
       <c r="K6" s="9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -2670,7 +2155,7 @@
       <c r="S6" s="10"/>
       <c r="T6" s="11"/>
       <c r="U6" s="9" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
@@ -2681,38 +2166,26 @@
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
       <c r="AD6" s="11"/>
-      <c r="AE6" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF6" s="10"/>
-      <c r="AG6" s="10"/>
-      <c r="AH6" s="10"/>
-      <c r="AI6" s="10"/>
-      <c r="AJ6" s="10"/>
-      <c r="AK6" s="10"/>
-      <c r="AL6" s="10"/>
-      <c r="AM6" s="10"/>
-      <c r="AN6" s="11"/>
-      <c r="AO6" s="10"/>
-      <c r="AP6" s="11"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="11"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="11"/>
       <c r="K7" s="9" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -2724,7 +2197,7 @@
       <c r="S7" s="10"/>
       <c r="T7" s="11"/>
       <c r="U7" s="9" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
@@ -2735,26 +2208,14 @@
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>
       <c r="AD7" s="11"/>
-      <c r="AE7" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF7" s="10"/>
-      <c r="AG7" s="10"/>
-      <c r="AH7" s="10"/>
-      <c r="AI7" s="10"/>
-      <c r="AJ7" s="10"/>
-      <c r="AK7" s="10"/>
-      <c r="AL7" s="10"/>
-      <c r="AM7" s="10"/>
-      <c r="AN7" s="11"/>
-      <c r="AO7" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP7" s="11"/>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF7" s="11"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
@@ -2764,11 +2225,11 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10" t="s">
-        <v>313</v>
+        <v>234</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="9" t="s">
-        <v>315</v>
+        <v>236</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -2780,7 +2241,7 @@
       <c r="S8" s="10"/>
       <c r="T8" s="11"/>
       <c r="U8" s="9" t="s">
-        <v>317</v>
+        <v>238</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
@@ -2791,24 +2252,12 @@
       <c r="AB8" s="10"/>
       <c r="AC8" s="10"/>
       <c r="AD8" s="11"/>
-      <c r="AE8" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="AF8" s="10"/>
-      <c r="AG8" s="10"/>
-      <c r="AH8" s="10"/>
-      <c r="AI8" s="10"/>
-      <c r="AJ8" s="10"/>
-      <c r="AK8" s="10"/>
-      <c r="AL8" s="10"/>
-      <c r="AM8" s="10"/>
-      <c r="AN8" s="11"/>
-      <c r="AO8" s="10"/>
-      <c r="AP8" s="11"/>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="11"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>287</v>
+        <v>211</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
@@ -2819,10 +2268,10 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -2834,7 +2283,7 @@
       <c r="S9" s="10"/>
       <c r="T9" s="11"/>
       <c r="U9" s="9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -2845,24 +2294,12 @@
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
       <c r="AD9" s="11"/>
-      <c r="AE9" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
-      <c r="AH9" s="10"/>
-      <c r="AI9" s="10"/>
-      <c r="AJ9" s="10"/>
-      <c r="AK9" s="10"/>
-      <c r="AL9" s="10"/>
-      <c r="AM9" s="10"/>
-      <c r="AN9" s="11"/>
-      <c r="AO9" s="10"/>
-      <c r="AP9" s="11"/>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="11"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
@@ -2872,11 +2309,11 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
@@ -2888,7 +2325,7 @@
       <c r="S10" s="10"/>
       <c r="T10" s="11"/>
       <c r="U10" s="9" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
@@ -2899,24 +2336,12 @@
       <c r="AB10" s="10"/>
       <c r="AC10" s="10"/>
       <c r="AD10" s="11"/>
-      <c r="AE10" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
-      <c r="AH10" s="10"/>
-      <c r="AI10" s="10"/>
-      <c r="AJ10" s="10"/>
-      <c r="AK10" s="10"/>
-      <c r="AL10" s="10"/>
-      <c r="AM10" s="10"/>
-      <c r="AN10" s="11"/>
-      <c r="AO10" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP10" s="11"/>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF10" s="11"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -2931,17 +2356,17 @@
       <c r="J11" s="8"/>
       <c r="K11" s="6"/>
       <c r="L11" s="7" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="S11" s="7"/>
       <c r="T11" s="8"/>
@@ -2955,22 +2380,12 @@
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="8"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="7"/>
-      <c r="AG11" s="7"/>
-      <c r="AH11" s="7"/>
-      <c r="AI11" s="7"/>
-      <c r="AJ11" s="7"/>
-      <c r="AK11" s="7"/>
-      <c r="AL11" s="7"/>
-      <c r="AM11" s="7"/>
-      <c r="AN11" s="8"/>
-      <c r="AO11" s="7"/>
-      <c r="AP11" s="8"/>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="8"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
@@ -2984,7 +2399,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10" t="s">
-        <v>360</v>
+        <v>267</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -3003,24 +2418,14 @@
       <c r="AB12" s="10"/>
       <c r="AC12" s="10"/>
       <c r="AD12" s="11"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="10"/>
-      <c r="AG12" s="10"/>
-      <c r="AH12" s="10"/>
-      <c r="AI12" s="10"/>
-      <c r="AJ12" s="10"/>
-      <c r="AK12" s="10"/>
-      <c r="AL12" s="10"/>
-      <c r="AM12" s="10"/>
-      <c r="AN12" s="11"/>
-      <c r="AO12" s="10"/>
-      <c r="AP12" s="11" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>289</v>
+        <v>213</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
@@ -3035,7 +2440,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
@@ -3053,24 +2458,14 @@
       <c r="AB13" s="10"/>
       <c r="AC13" s="10"/>
       <c r="AD13" s="11"/>
-      <c r="AE13" s="9"/>
-      <c r="AF13" s="10"/>
-      <c r="AG13" s="10"/>
-      <c r="AH13" s="10"/>
-      <c r="AI13" s="10"/>
-      <c r="AJ13" s="10"/>
-      <c r="AK13" s="10"/>
-      <c r="AL13" s="10"/>
-      <c r="AM13" s="10"/>
-      <c r="AN13" s="11"/>
-      <c r="AO13" s="10"/>
-      <c r="AP13" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
@@ -3084,7 +2479,7 @@
       <c r="K14" s="9"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -3103,26 +2498,16 @@
       <c r="AB14" s="10"/>
       <c r="AC14" s="10"/>
       <c r="AD14" s="11"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="10"/>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="10"/>
-      <c r="AI14" s="10"/>
-      <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="10"/>
-      <c r="AM14" s="10"/>
-      <c r="AN14" s="11"/>
-      <c r="AO14" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AP14" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF14" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
@@ -3139,7 +2524,7 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10" t="s">
-        <v>361</v>
+        <v>268</v>
       </c>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
@@ -3155,24 +2540,14 @@
       <c r="AB15" s="10"/>
       <c r="AC15" s="10"/>
       <c r="AD15" s="11"/>
-      <c r="AE15" s="9"/>
-      <c r="AF15" s="10"/>
-      <c r="AG15" s="10"/>
-      <c r="AH15" s="10"/>
-      <c r="AI15" s="10"/>
-      <c r="AJ15" s="10"/>
-      <c r="AK15" s="10"/>
-      <c r="AL15" s="10"/>
-      <c r="AM15" s="10"/>
-      <c r="AN15" s="11"/>
-      <c r="AO15" s="10"/>
-      <c r="AP15" s="11" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE15" s="10"/>
+      <c r="AF15" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>291</v>
+        <v>215</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -3190,7 +2565,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
@@ -3205,24 +2580,14 @@
       <c r="AB16" s="10"/>
       <c r="AC16" s="10"/>
       <c r="AD16" s="11"/>
-      <c r="AE16" s="9"/>
-      <c r="AF16" s="10"/>
-      <c r="AG16" s="10"/>
-      <c r="AH16" s="10"/>
-      <c r="AI16" s="10"/>
-      <c r="AJ16" s="10"/>
-      <c r="AK16" s="10"/>
-      <c r="AL16" s="10"/>
-      <c r="AM16" s="10"/>
-      <c r="AN16" s="11"/>
-      <c r="AO16" s="10"/>
-      <c r="AP16" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE16" s="10"/>
+      <c r="AF16" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
@@ -3239,7 +2604,7 @@
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
@@ -3255,26 +2620,16 @@
       <c r="AB17" s="10"/>
       <c r="AC17" s="10"/>
       <c r="AD17" s="11"/>
-      <c r="AE17" s="9"/>
-      <c r="AF17" s="10"/>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="10"/>
-      <c r="AI17" s="10"/>
-      <c r="AJ17" s="10"/>
-      <c r="AK17" s="10"/>
-      <c r="AL17" s="10"/>
-      <c r="AM17" s="10"/>
-      <c r="AN17" s="11"/>
-      <c r="AO17" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AP17" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF17" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -3294,7 +2649,7 @@
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10" t="s">
-        <v>362</v>
+        <v>269</v>
       </c>
       <c r="T18" s="11"/>
       <c r="U18" s="9"/>
@@ -3307,24 +2662,14 @@
       <c r="AB18" s="10"/>
       <c r="AC18" s="10"/>
       <c r="AD18" s="11"/>
-      <c r="AE18" s="9"/>
-      <c r="AF18" s="10"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="10"/>
-      <c r="AJ18" s="10"/>
-      <c r="AK18" s="10"/>
-      <c r="AL18" s="10"/>
-      <c r="AM18" s="10"/>
-      <c r="AN18" s="11"/>
-      <c r="AO18" s="10"/>
-      <c r="AP18" s="11" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE18" s="10"/>
+      <c r="AF18" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>293</v>
+        <v>217</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
@@ -3345,7 +2690,7 @@
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="11" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="U19" s="9"/>
       <c r="V19" s="10"/>
@@ -3357,24 +2702,14 @@
       <c r="AB19" s="10"/>
       <c r="AC19" s="10"/>
       <c r="AD19" s="11"/>
-      <c r="AE19" s="9"/>
-      <c r="AF19" s="10"/>
-      <c r="AG19" s="10"/>
-      <c r="AH19" s="10"/>
-      <c r="AI19" s="10"/>
-      <c r="AJ19" s="10"/>
-      <c r="AK19" s="10"/>
-      <c r="AL19" s="10"/>
-      <c r="AM19" s="10"/>
-      <c r="AN19" s="11"/>
-      <c r="AO19" s="10"/>
-      <c r="AP19" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
@@ -3394,7 +2729,7 @@
       <c r="Q20" s="13"/>
       <c r="R20" s="13"/>
       <c r="S20" s="13" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="T20" s="14"/>
       <c r="U20" s="12"/>
@@ -3407,24 +2742,14 @@
       <c r="AB20" s="13"/>
       <c r="AC20" s="13"/>
       <c r="AD20" s="14"/>
-      <c r="AE20" s="12"/>
-      <c r="AF20" s="13"/>
-      <c r="AG20" s="13"/>
-      <c r="AH20" s="13"/>
-      <c r="AI20" s="13"/>
-      <c r="AJ20" s="13"/>
-      <c r="AK20" s="13"/>
-      <c r="AL20" s="13"/>
-      <c r="AM20" s="13"/>
-      <c r="AN20" s="14"/>
-      <c r="AO20" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AP20" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE20" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF20" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
@@ -3449,36 +2774,26 @@
       <c r="T21" s="8"/>
       <c r="U21" s="6"/>
       <c r="V21" s="7" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
       <c r="Y21" s="7" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Z21" s="7"/>
       <c r="AA21" s="7"/>
       <c r="AB21" s="7" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="AC21" s="7"/>
       <c r="AD21" s="8"/>
-      <c r="AE21" s="6"/>
-      <c r="AF21" s="7"/>
-      <c r="AG21" s="7"/>
-      <c r="AH21" s="7"/>
-      <c r="AI21" s="7"/>
-      <c r="AJ21" s="7"/>
-      <c r="AK21" s="7"/>
-      <c r="AL21" s="7"/>
-      <c r="AM21" s="7"/>
-      <c r="AN21" s="8"/>
-      <c r="AO21" s="7"/>
-      <c r="AP21" s="8"/>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="8"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
@@ -3502,7 +2817,7 @@
       <c r="U22" s="9"/>
       <c r="V22" s="10"/>
       <c r="W22" s="10" t="s">
-        <v>363</v>
+        <v>270</v>
       </c>
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
@@ -3511,24 +2826,14 @@
       <c r="AB22" s="10"/>
       <c r="AC22" s="10"/>
       <c r="AD22" s="11"/>
-      <c r="AE22" s="9"/>
-      <c r="AF22" s="10"/>
-      <c r="AG22" s="10"/>
-      <c r="AH22" s="10"/>
-      <c r="AI22" s="10"/>
-      <c r="AJ22" s="10"/>
-      <c r="AK22" s="10"/>
-      <c r="AL22" s="10"/>
-      <c r="AM22" s="10"/>
-      <c r="AN22" s="11"/>
-      <c r="AO22" s="10"/>
-      <c r="AP22" s="11" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>295</v>
+        <v>219</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -3553,7 +2858,7 @@
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
       <c r="X23" s="10" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="10"/>
@@ -3561,24 +2866,14 @@
       <c r="AB23" s="10"/>
       <c r="AC23" s="10"/>
       <c r="AD23" s="11"/>
-      <c r="AE23" s="9"/>
-      <c r="AF23" s="10"/>
-      <c r="AG23" s="10"/>
-      <c r="AH23" s="10"/>
-      <c r="AI23" s="10"/>
-      <c r="AJ23" s="10"/>
-      <c r="AK23" s="10"/>
-      <c r="AL23" s="10"/>
-      <c r="AM23" s="10"/>
-      <c r="AN23" s="11"/>
-      <c r="AO23" s="10"/>
-      <c r="AP23" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE23" s="10"/>
+      <c r="AF23" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -3602,7 +2897,7 @@
       <c r="U24" s="9"/>
       <c r="V24" s="10"/>
       <c r="W24" s="10" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="X24" s="10"/>
       <c r="Y24" s="10"/>
@@ -3611,26 +2906,16 @@
       <c r="AB24" s="10"/>
       <c r="AC24" s="10"/>
       <c r="AD24" s="11"/>
-      <c r="AE24" s="9"/>
-      <c r="AF24" s="10"/>
-      <c r="AG24" s="10"/>
-      <c r="AH24" s="10"/>
-      <c r="AI24" s="10"/>
-      <c r="AJ24" s="10"/>
-      <c r="AK24" s="10"/>
-      <c r="AL24" s="10"/>
-      <c r="AM24" s="10"/>
-      <c r="AN24" s="11"/>
-      <c r="AO24" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="AP24" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE24" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF24" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -3657,30 +2942,20 @@
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
       <c r="Z25" s="10" t="s">
-        <v>364</v>
+        <v>271</v>
       </c>
       <c r="AA25" s="10"/>
       <c r="AB25" s="10"/>
       <c r="AC25" s="10"/>
       <c r="AD25" s="11"/>
-      <c r="AE25" s="9"/>
-      <c r="AF25" s="10"/>
-      <c r="AG25" s="10"/>
-      <c r="AH25" s="10"/>
-      <c r="AI25" s="10"/>
-      <c r="AJ25" s="10"/>
-      <c r="AK25" s="10"/>
-      <c r="AL25" s="10"/>
-      <c r="AM25" s="10"/>
-      <c r="AN25" s="11"/>
-      <c r="AO25" s="10"/>
-      <c r="AP25" s="11" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE25" s="10"/>
+      <c r="AF25" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>297</v>
+        <v>221</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
@@ -3708,29 +2983,19 @@
       <c r="Y26" s="10"/>
       <c r="Z26" s="10"/>
       <c r="AA26" s="10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="AB26" s="10"/>
       <c r="AC26" s="10"/>
       <c r="AD26" s="11"/>
-      <c r="AE26" s="9"/>
-      <c r="AF26" s="10"/>
-      <c r="AG26" s="10"/>
-      <c r="AH26" s="10"/>
-      <c r="AI26" s="10"/>
-      <c r="AJ26" s="10"/>
-      <c r="AK26" s="10"/>
-      <c r="AL26" s="10"/>
-      <c r="AM26" s="10"/>
-      <c r="AN26" s="11"/>
-      <c r="AO26" s="10"/>
-      <c r="AP26" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE26" s="10"/>
+      <c r="AF26" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
@@ -3757,32 +3022,22 @@
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
       <c r="Z27" s="10" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="AA27" s="10"/>
       <c r="AB27" s="10"/>
       <c r="AC27" s="10"/>
       <c r="AD27" s="11"/>
-      <c r="AE27" s="9"/>
-      <c r="AF27" s="10"/>
-      <c r="AG27" s="10"/>
-      <c r="AH27" s="10"/>
-      <c r="AI27" s="10"/>
-      <c r="AJ27" s="10"/>
-      <c r="AK27" s="10"/>
-      <c r="AL27" s="10"/>
-      <c r="AM27" s="10"/>
-      <c r="AN27" s="11"/>
-      <c r="AO27" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="AP27" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE27" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF27" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
@@ -3812,27 +3067,17 @@
       <c r="AA28" s="10"/>
       <c r="AB28" s="10"/>
       <c r="AC28" s="10" t="s">
-        <v>365</v>
+        <v>272</v>
       </c>
       <c r="AD28" s="11"/>
-      <c r="AE28" s="9"/>
-      <c r="AF28" s="10"/>
-      <c r="AG28" s="10"/>
-      <c r="AH28" s="10"/>
-      <c r="AI28" s="10"/>
-      <c r="AJ28" s="10"/>
-      <c r="AK28" s="10"/>
-      <c r="AL28" s="10"/>
-      <c r="AM28" s="10"/>
-      <c r="AN28" s="11"/>
-      <c r="AO28" s="10"/>
-      <c r="AP28" s="11" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AE28" s="10"/>
+      <c r="AF28" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>299</v>
+        <v>223</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
@@ -3863,26 +3108,16 @@
       <c r="AB29" s="10"/>
       <c r="AC29" s="10"/>
       <c r="AD29" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE29" s="9"/>
-      <c r="AF29" s="10"/>
-      <c r="AG29" s="10"/>
-      <c r="AH29" s="10"/>
-      <c r="AI29" s="10"/>
-      <c r="AJ29" s="10"/>
-      <c r="AK29" s="10"/>
-      <c r="AL29" s="10"/>
-      <c r="AM29" s="10"/>
-      <c r="AN29" s="11"/>
-      <c r="AO29" s="10"/>
-      <c r="AP29" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="AE29" s="10"/>
+      <c r="AF29" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
@@ -3912,627 +3147,89 @@
       <c r="AA30" s="13"/>
       <c r="AB30" s="13"/>
       <c r="AC30" s="13" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="AD30" s="14"/>
-      <c r="AE30" s="12"/>
-      <c r="AF30" s="13"/>
-      <c r="AG30" s="13"/>
-      <c r="AH30" s="13"/>
-      <c r="AI30" s="13"/>
-      <c r="AJ30" s="13"/>
-      <c r="AK30" s="13"/>
-      <c r="AL30" s="13"/>
-      <c r="AM30" s="13"/>
-      <c r="AN30" s="14"/>
-      <c r="AO30" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP30" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="7"/>
-      <c r="AB31" s="7"/>
-      <c r="AC31" s="7"/>
-      <c r="AD31" s="8"/>
-      <c r="AE31" s="6"/>
-      <c r="AF31" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG31" s="7"/>
-      <c r="AH31" s="7"/>
-      <c r="AI31" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="AJ31" s="7"/>
-      <c r="AK31" s="7"/>
-      <c r="AL31" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM31" s="7"/>
-      <c r="AN31" s="8"/>
-      <c r="AO31" s="7"/>
-      <c r="AP31" s="8"/>
-    </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
-      <c r="S32" s="10"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="10"/>
-      <c r="W32" s="10"/>
-      <c r="X32" s="10"/>
-      <c r="Y32" s="10"/>
-      <c r="Z32" s="10"/>
-      <c r="AA32" s="10"/>
-      <c r="AB32" s="10"/>
-      <c r="AC32" s="10"/>
-      <c r="AD32" s="11"/>
-      <c r="AE32" s="9"/>
-      <c r="AF32" s="10"/>
-      <c r="AG32" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="AH32" s="10"/>
-      <c r="AI32" s="10"/>
-      <c r="AJ32" s="10"/>
-      <c r="AK32" s="10"/>
-      <c r="AL32" s="10"/>
-      <c r="AM32" s="10"/>
-      <c r="AN32" s="11"/>
-      <c r="AO32" s="10"/>
-      <c r="AP32" s="11" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="10"/>
-      <c r="W33" s="10"/>
-      <c r="X33" s="10"/>
-      <c r="Y33" s="10"/>
-      <c r="Z33" s="10"/>
-      <c r="AA33" s="10"/>
-      <c r="AB33" s="10"/>
-      <c r="AC33" s="10"/>
-      <c r="AD33" s="11"/>
-      <c r="AE33" s="9"/>
-      <c r="AF33" s="10"/>
-      <c r="AG33" s="10"/>
-      <c r="AH33" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI33" s="10"/>
-      <c r="AJ33" s="10"/>
-      <c r="AK33" s="10"/>
-      <c r="AL33" s="10"/>
-      <c r="AM33" s="10"/>
-      <c r="AN33" s="11"/>
-      <c r="AO33" s="10"/>
-      <c r="AP33" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="11"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="10"/>
-      <c r="W34" s="10"/>
-      <c r="X34" s="10"/>
-      <c r="Y34" s="10"/>
-      <c r="Z34" s="10"/>
-      <c r="AA34" s="10"/>
-      <c r="AB34" s="10"/>
-      <c r="AC34" s="10"/>
-      <c r="AD34" s="11"/>
-      <c r="AE34" s="9"/>
-      <c r="AF34" s="10"/>
-      <c r="AG34" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="AH34" s="10"/>
-      <c r="AI34" s="10"/>
-      <c r="AJ34" s="10"/>
-      <c r="AK34" s="10"/>
-      <c r="AL34" s="10"/>
-      <c r="AM34" s="10"/>
-      <c r="AN34" s="11"/>
-      <c r="AO34" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="AP34" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-      <c r="T35" s="11"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="10"/>
-      <c r="W35" s="10"/>
-      <c r="X35" s="10"/>
-      <c r="Y35" s="10"/>
-      <c r="Z35" s="10"/>
-      <c r="AA35" s="10"/>
-      <c r="AB35" s="10"/>
-      <c r="AC35" s="10"/>
-      <c r="AD35" s="11"/>
-      <c r="AE35" s="9"/>
-      <c r="AF35" s="10"/>
-      <c r="AG35" s="10"/>
-      <c r="AH35" s="10"/>
-      <c r="AI35" s="10"/>
-      <c r="AJ35" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="AK35" s="10"/>
-      <c r="AL35" s="10"/>
-      <c r="AM35" s="10"/>
-      <c r="AN35" s="11"/>
-      <c r="AO35" s="10"/>
-      <c r="AP35" s="11" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="10"/>
-      <c r="W36" s="10"/>
-      <c r="X36" s="10"/>
-      <c r="Y36" s="10"/>
-      <c r="Z36" s="10"/>
-      <c r="AA36" s="10"/>
-      <c r="AB36" s="10"/>
-      <c r="AC36" s="10"/>
-      <c r="AD36" s="11"/>
-      <c r="AE36" s="9"/>
-      <c r="AF36" s="10"/>
-      <c r="AG36" s="10"/>
-      <c r="AH36" s="10"/>
-      <c r="AI36" s="10"/>
-      <c r="AJ36" s="10"/>
-      <c r="AK36" s="10" t="s">
+      <c r="AE30" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF30" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="AL36" s="10"/>
-      <c r="AM36" s="10"/>
-      <c r="AN36" s="11"/>
-      <c r="AO36" s="10"/>
-      <c r="AP36" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="10"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="10"/>
-      <c r="W37" s="10"/>
-      <c r="X37" s="10"/>
-      <c r="Y37" s="10"/>
-      <c r="Z37" s="10"/>
-      <c r="AA37" s="10"/>
-      <c r="AB37" s="10"/>
-      <c r="AC37" s="10"/>
-      <c r="AD37" s="11"/>
-      <c r="AE37" s="9"/>
-      <c r="AF37" s="10"/>
-      <c r="AG37" s="10"/>
-      <c r="AH37" s="10"/>
-      <c r="AI37" s="10"/>
-      <c r="AJ37" s="10" t="s">
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="AK37" s="10"/>
-      <c r="AL37" s="10"/>
-      <c r="AM37" s="10"/>
-      <c r="AN37" s="11"/>
-      <c r="AO37" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP37" s="11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="10"/>
-      <c r="T38" s="11"/>
-      <c r="U38" s="9"/>
-      <c r="V38" s="10"/>
-      <c r="W38" s="10"/>
-      <c r="X38" s="10"/>
-      <c r="Y38" s="10"/>
-      <c r="Z38" s="10"/>
-      <c r="AA38" s="10"/>
-      <c r="AB38" s="10"/>
-      <c r="AC38" s="10"/>
-      <c r="AD38" s="11"/>
-      <c r="AE38" s="9"/>
-      <c r="AF38" s="10"/>
-      <c r="AG38" s="10"/>
-      <c r="AH38" s="10"/>
-      <c r="AI38" s="10"/>
-      <c r="AJ38" s="10"/>
-      <c r="AK38" s="10"/>
-      <c r="AL38" s="10"/>
-      <c r="AM38" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="AN38" s="11"/>
-      <c r="AO38" s="10"/>
-      <c r="AP38" s="11" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="11"/>
-      <c r="U39" s="9"/>
-      <c r="V39" s="10"/>
-      <c r="W39" s="10"/>
-      <c r="X39" s="10"/>
-      <c r="Y39" s="10"/>
-      <c r="Z39" s="10"/>
-      <c r="AA39" s="10"/>
-      <c r="AB39" s="10"/>
-      <c r="AC39" s="10"/>
-      <c r="AD39" s="11"/>
-      <c r="AE39" s="9"/>
-      <c r="AF39" s="10"/>
-      <c r="AG39" s="10"/>
-      <c r="AH39" s="10"/>
-      <c r="AI39" s="10"/>
-      <c r="AJ39" s="10"/>
-      <c r="AK39" s="10"/>
-      <c r="AL39" s="10"/>
-      <c r="AM39" s="10"/>
-      <c r="AN39" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="AO39" s="10"/>
-      <c r="AP39" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="13"/>
-      <c r="S40" s="13"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="12"/>
-      <c r="V40" s="13"/>
-      <c r="W40" s="13"/>
-      <c r="X40" s="13"/>
-      <c r="Y40" s="13"/>
-      <c r="Z40" s="13"/>
-      <c r="AA40" s="13"/>
-      <c r="AB40" s="13"/>
-      <c r="AC40" s="13"/>
-      <c r="AD40" s="14"/>
-      <c r="AE40" s="12"/>
-      <c r="AF40" s="13"/>
-      <c r="AG40" s="13"/>
-      <c r="AH40" s="13"/>
-      <c r="AI40" s="13"/>
-      <c r="AJ40" s="13"/>
-      <c r="AK40" s="13"/>
-      <c r="AL40" s="13"/>
-      <c r="AM40" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="AN40" s="14"/>
-      <c r="AO40" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="AP40" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-      <c r="S41" s="10"/>
-      <c r="T41" s="11"/>
-      <c r="U41" s="9"/>
-      <c r="V41" s="10"/>
-      <c r="W41" s="10"/>
-      <c r="X41" s="10"/>
-      <c r="Y41" s="10"/>
-      <c r="Z41" s="10"/>
-      <c r="AA41" s="10"/>
-      <c r="AB41" s="10"/>
-      <c r="AC41" s="10"/>
-      <c r="AD41" s="11"/>
-      <c r="AE41" s="9"/>
-      <c r="AF41" s="10"/>
-      <c r="AG41" s="10"/>
-      <c r="AH41" s="10"/>
-      <c r="AI41" s="10"/>
-      <c r="AJ41" s="10"/>
-      <c r="AK41" s="10"/>
-      <c r="AL41" s="10"/>
-      <c r="AM41" s="10"/>
-      <c r="AN41" s="11"/>
-      <c r="AO41" s="10"/>
-      <c r="AP41" s="11"/>
-    </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="13"/>
-      <c r="S42" s="13"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="12"/>
-      <c r="V42" s="13"/>
-      <c r="W42" s="13"/>
-      <c r="X42" s="13"/>
-      <c r="Y42" s="13"/>
-      <c r="Z42" s="13"/>
-      <c r="AA42" s="13"/>
-      <c r="AB42" s="13"/>
-      <c r="AC42" s="13"/>
-      <c r="AD42" s="14"/>
-      <c r="AE42" s="12"/>
-      <c r="AF42" s="13"/>
-      <c r="AG42" s="13"/>
-      <c r="AH42" s="13"/>
-      <c r="AI42" s="13"/>
-      <c r="AJ42" s="13"/>
-      <c r="AK42" s="13"/>
-      <c r="AL42" s="13"/>
-      <c r="AM42" s="13"/>
-      <c r="AN42" s="14"/>
-      <c r="AO42" s="13"/>
-      <c r="AP42" s="14"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="10"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="10"/>
+      <c r="AF31" s="11"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+      <c r="AA32" s="13"/>
+      <c r="AB32" s="13"/>
+      <c r="AC32" s="13"/>
+      <c r="AD32" s="14"/>
+      <c r="AE32" s="13"/>
+      <c r="AF32" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4541,10 +3238,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4560,35 +3257,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>284</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>143</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -4596,24 +3293,24 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>145</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>160</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -4621,24 +3318,24 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>146</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>147</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -4646,134 +3343,134 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>358</v>
+        <v>265</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>312</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s">
-        <v>320</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>195</v>
+        <v>148</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>196</v>
+        <v>149</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>359</v>
+        <v>266</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>313</v>
+        <v>234</v>
       </c>
       <c r="C12" t="s">
-        <v>321</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>150</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>151</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>162</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>314</v>
+        <v>235</v>
       </c>
       <c r="C16" t="s">
-        <v>322</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>343</v>
+        <v>255</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>328</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>153</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>201</v>
+        <v>154</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>315</v>
+        <v>236</v>
       </c>
       <c r="C19" t="s">
-        <v>323</v>
+        <v>242</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -4781,167 +3478,176 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>344</v>
+        <v>256</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>329</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>202</v>
+        <v>155</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>316</v>
+        <v>237</v>
       </c>
       <c r="C22" t="s">
-        <v>324</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>345</v>
+        <v>257</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>330</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>157</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>205</v>
+        <v>158</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>317</v>
+        <v>238</v>
       </c>
       <c r="C25" t="s">
-        <v>325</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>346</v>
+        <v>258</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>331</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>206</v>
+        <v>159</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>318</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>326</v>
+        <v>115</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>347</v>
+        <v>164</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>332</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>209</v>
+        <v>279</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>319</v>
+        <v>267</v>
       </c>
       <c r="C31" t="s">
-        <v>327</v>
+        <v>273</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>348</v>
+        <v>166</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>333</v>
+        <v>116</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>210</v>
+        <v>167</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>214</v>
+        <v>172</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="D34" s="2">
         <v>1</v>
@@ -4949,792 +3655,453 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>215</v>
+        <v>280</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>72</v>
+        <v>268</v>
       </c>
       <c r="C35" t="s">
-        <v>145</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>378</v>
+        <v>169</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>360</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>369</v>
-      </c>
-      <c r="D37" s="2">
-        <v>1</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>148</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>218</v>
+        <v>281</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>75</v>
+        <v>269</v>
       </c>
       <c r="C39" t="s">
-        <v>149</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>223</v>
+        <v>170</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>154</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>379</v>
+        <v>171</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>361</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>370</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>220</v>
+        <v>175</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>77</v>
+        <v>285</v>
       </c>
       <c r="C43" t="s">
-        <v>151</v>
+        <v>291</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>380</v>
+        <v>176</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>362</v>
+        <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>371</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>221</v>
+        <v>177</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>78</v>
+        <v>286</v>
       </c>
       <c r="C46" t="s">
-        <v>152</v>
+        <v>292</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>222</v>
+        <v>260</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>250</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>225</v>
+        <v>178</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="C48" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>226</v>
+        <v>179</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>387</v>
+        <v>287</v>
       </c>
       <c r="C49" t="s">
-        <v>396</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>349</v>
+        <v>261</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>334</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>227</v>
+        <v>180</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C51" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>228</v>
+        <v>181</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>388</v>
+        <v>68</v>
       </c>
       <c r="C52" t="s">
-        <v>397</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>350</v>
+        <v>182</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="C53" t="s">
-        <v>335</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>229</v>
+        <v>183</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>389</v>
+        <v>270</v>
       </c>
       <c r="C55" t="s">
-        <v>398</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>351</v>
+        <v>184</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>336</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>233</v>
+        <v>283</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>81</v>
+        <v>271</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>381</v>
+        <v>187</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>363</v>
+        <v>74</v>
       </c>
       <c r="C61" t="s">
-        <v>372</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>236</v>
+        <v>284</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>84</v>
+        <v>272</v>
       </c>
       <c r="C63" t="s">
-        <v>164</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>241</v>
+        <v>188</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>382</v>
+        <v>189</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>364</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>373</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>86</v>
+        <v>288</v>
       </c>
       <c r="C67" t="s">
-        <v>166</v>
+        <v>294</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C68" t="s">
-        <v>170</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>383</v>
+        <v>194</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>365</v>
+        <v>90</v>
       </c>
       <c r="C69" t="s">
-        <v>374</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>239</v>
+        <v>195</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>87</v>
+        <v>289</v>
       </c>
       <c r="C70" t="s">
-        <v>167</v>
+        <v>295</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>240</v>
+        <v>263</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>168</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>243</v>
+        <v>196</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>244</v>
+        <v>197</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>390</v>
+        <v>290</v>
       </c>
       <c r="C73" t="s">
-        <v>399</v>
+        <v>296</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>352</v>
+        <v>264</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="C74" t="s">
-        <v>337</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>245</v>
+        <v>198</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>246</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C76" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>353</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C77" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>247</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C78" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>248</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C79" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>354</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C80" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>249</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C81" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>250</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C82" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>251</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C83" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>252</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C84" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>384</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="C85" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>253</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C86" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>254</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C87" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>259</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C88" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>385</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C89" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>255</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C90" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>256</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C91" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>260</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C92" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>386</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="C93" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>257</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C94" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>258</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C95" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>261</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C96" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>262</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C97" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>355</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C98" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>263</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C99" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>264</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="C100" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>356</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C101" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>265</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C102" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>266</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="C103" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>357</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C104" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>267</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C105" t="s">
-        <v>189</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
One tag for many links
Transition for deaths due to other causes has been introduced.
Given that this is statistically likely to affect all compartments in a
similar manner, tags in the cascade transitions sheet no longer need be
unique.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="327">
   <si>
     <t>Code Label</t>
   </si>
@@ -126,856 +126,877 @@
     <t>rec</t>
   </si>
   <si>
-    <t>dead</t>
-  </si>
-  <si>
     <t>Recovered</t>
   </si>
   <si>
+    <t>Vaccinated</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>ag</t>
+  </si>
+  <si>
+    <t>ah</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>bd</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>bf</t>
+  </si>
+  <si>
+    <t>bg</t>
+  </si>
+  <si>
+    <t>bh</t>
+  </si>
+  <si>
+    <t>bi</t>
+  </si>
+  <si>
+    <t>aj</t>
+  </si>
+  <si>
+    <t>ak</t>
+  </si>
+  <si>
+    <t>al</t>
+  </si>
+  <si>
+    <t>bj</t>
+  </si>
+  <si>
+    <t>bk</t>
+  </si>
+  <si>
+    <t>bl</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>an</t>
+  </si>
+  <si>
+    <t>ao</t>
+  </si>
+  <si>
+    <t>ap</t>
+  </si>
+  <si>
+    <t>aq</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>bm</t>
+  </si>
+  <si>
+    <t>bn</t>
+  </si>
+  <si>
+    <t>bo</t>
+  </si>
+  <si>
+    <t>bp</t>
+  </si>
+  <si>
+    <t>bq</t>
+  </si>
+  <si>
+    <t>br</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Vaccination Rate</t>
+  </si>
+  <si>
+    <t>Infection Rate (Susceptible)</t>
+  </si>
+  <si>
+    <t>Infection Rate (Vaccinated)</t>
+  </si>
+  <si>
+    <t>Slow-LTBI Partition Fraction</t>
+  </si>
+  <si>
+    <t>Fast-LTBI Partition Fraction</t>
+  </si>
+  <si>
+    <t>Slow-LTBI Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>Slow-LTBI Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>Fast-LTBI Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>Fast-LTBI Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Slow Treated)</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Fast Treated)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Slow Treated)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Fast Treated)</t>
+  </si>
+  <si>
+    <t>Slow-LTBI Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>Fast-LTBI Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>Reinfection Rate (Recovered)</t>
+  </si>
+  <si>
+    <t>SPos MDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>SPos XDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>SPos DS Partition Fraction</t>
+  </si>
+  <si>
+    <t>SPos DS Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SPos DS Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SPos MDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SPos MDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SPos XDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SPos XDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SPos DS Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SPos MDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SPos XDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SPos DS Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SPos MDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SPos XDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SNeg DS Partition Fraction</t>
+  </si>
+  <si>
+    <t>SNeg MDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>SNeg XDR Partition Fraction</t>
+  </si>
+  <si>
+    <t>SNeg DS Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SNeg DS Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SNeg MDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SNeg MDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SNeg XDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SNeg XDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SNeg DS Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SNeg MDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SNeg XDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SNeg DS Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SNeg MDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>SNeg XDR Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>v_rate</t>
+  </si>
+  <si>
+    <t>infs_rate</t>
+  </si>
+  <si>
+    <t>infv_rate</t>
+  </si>
+  <si>
+    <t>lts_frac</t>
+  </si>
+  <si>
+    <t>ltf_frac</t>
+  </si>
+  <si>
+    <t>ltsyes_rate</t>
+  </si>
+  <si>
+    <t>ltsno_rate</t>
+  </si>
+  <si>
+    <t>ltfyes_rate</t>
+  </si>
+  <si>
+    <t>ltfno_rate</t>
+  </si>
+  <si>
+    <t>ltsus+_rate</t>
+  </si>
+  <si>
+    <t>ltsts+_rate</t>
+  </si>
+  <si>
+    <t>ltfus+_rate</t>
+  </si>
+  <si>
+    <t>ltfts+_rate</t>
+  </si>
+  <si>
+    <t>ltsus-_rate</t>
+  </si>
+  <si>
+    <t>ltsts-_rate</t>
+  </si>
+  <si>
+    <t>ltfus-_rate</t>
+  </si>
+  <si>
+    <t>ltfts-_rate</t>
+  </si>
+  <si>
+    <t>infr_rate</t>
+  </si>
+  <si>
+    <t>ltssuc_rate</t>
+  </si>
+  <si>
+    <t>ltfsuc_rate</t>
+  </si>
+  <si>
+    <t>s+d_frac</t>
+  </si>
+  <si>
+    <t>s+m_frac</t>
+  </si>
+  <si>
+    <t>s+x_frac</t>
+  </si>
+  <si>
+    <t>s+dyes_rate</t>
+  </si>
+  <si>
+    <t>s+dno_rate</t>
+  </si>
+  <si>
+    <t>s+myes_rate</t>
+  </si>
+  <si>
+    <t>s+mno_rate</t>
+  </si>
+  <si>
+    <t>s+xyes_rate</t>
+  </si>
+  <si>
+    <t>s+xno_rate</t>
+  </si>
+  <si>
+    <t>s+dsuc_rate</t>
+  </si>
+  <si>
+    <t>s+msuc_rate</t>
+  </si>
+  <si>
+    <t>s+xsuc_rate</t>
+  </si>
+  <si>
+    <t>s+dud_rate</t>
+  </si>
+  <si>
+    <t>s+dtd_rate</t>
+  </si>
+  <si>
+    <t>s+mud_rate</t>
+  </si>
+  <si>
+    <t>s+mtd_rate</t>
+  </si>
+  <si>
+    <t>s+xud_rate</t>
+  </si>
+  <si>
+    <t>s+xtd_rate</t>
+  </si>
+  <si>
+    <t>s-d_frac</t>
+  </si>
+  <si>
+    <t>s-m_frac</t>
+  </si>
+  <si>
+    <t>s-x_frac</t>
+  </si>
+  <si>
+    <t>s-dyes_rate</t>
+  </si>
+  <si>
+    <t>s-dno_rate</t>
+  </si>
+  <si>
+    <t>s-myes_rate</t>
+  </si>
+  <si>
+    <t>s-mno_rate</t>
+  </si>
+  <si>
+    <t>s-xyes_rate</t>
+  </si>
+  <si>
+    <t>s-xno_rate</t>
+  </si>
+  <si>
+    <t>s-dsuc_rate</t>
+  </si>
+  <si>
+    <t>s-msuc_rate</t>
+  </si>
+  <si>
+    <t>s-xsuc_rate</t>
+  </si>
+  <si>
+    <t>s-dud_rate</t>
+  </si>
+  <si>
+    <t>s-dtd_rate</t>
+  </si>
+  <si>
+    <t>s-mud_rate</t>
+  </si>
+  <si>
+    <t>s-mtd_rate</t>
+  </si>
+  <si>
+    <t>s-xud_rate</t>
+  </si>
+  <si>
+    <t>s-xtd_rate</t>
+  </si>
+  <si>
+    <t>Plot Coordinates</t>
+  </si>
+  <si>
+    <t>(-10,1)</t>
+  </si>
+  <si>
+    <t>(-10,-1)</t>
+  </si>
+  <si>
+    <t>(-8,1)</t>
+  </si>
+  <si>
+    <t>(-8,-1)</t>
+  </si>
+  <si>
+    <t>(8,1)</t>
+  </si>
+  <si>
+    <t>(8,-1)</t>
+  </si>
+  <si>
+    <t>(10,1)</t>
+  </si>
+  <si>
+    <t>(10,-1)</t>
+  </si>
+  <si>
+    <t>Default Value</t>
+  </si>
+  <si>
+    <t>ltsd</t>
+  </si>
+  <si>
+    <t>Slow Latent Diagnosed</t>
+  </si>
+  <si>
+    <t>ltfd</t>
+  </si>
+  <si>
+    <t>Fast Latent Diagnosed</t>
+  </si>
+  <si>
+    <t>s+dd</t>
+  </si>
+  <si>
+    <t>Drug-Susceptible Smear-Positive Diagnosed</t>
+  </si>
+  <si>
+    <t>s+md</t>
+  </si>
+  <si>
+    <t>Multidrug-Resistant Smear-Positive Diagnosed</t>
+  </si>
+  <si>
+    <t>s+xd</t>
+  </si>
+  <si>
+    <t>Extensively Drug-Resistant Smear-Positive Diagnosed</t>
+  </si>
+  <si>
+    <t>s-dd</t>
+  </si>
+  <si>
+    <t>Drug-Susceptible Smear-Negative Diagnosed</t>
+  </si>
+  <si>
+    <t>s-md</t>
+  </si>
+  <si>
+    <t>Multidrug-Resistant Smear-Negative Diagnosed</t>
+  </si>
+  <si>
+    <t>s-xd</t>
+  </si>
+  <si>
+    <t>Extensively Drug-Resistant Smear-Negative Diagnosed</t>
+  </si>
+  <si>
+    <t>Slow Latent Undiagnosed</t>
+  </si>
+  <si>
+    <t>Fast Latent Undiagnosed</t>
+  </si>
+  <si>
+    <t>Drug-Susceptible Smear-Positive Undiagnosed</t>
+  </si>
+  <si>
+    <t>Multidrug-Resistant Smear-Positive Undiagnosed</t>
+  </si>
+  <si>
+    <t>Extensively Drug-Resistant Smear-Positive Undiagnosed</t>
+  </si>
+  <si>
+    <t>Drug-Susceptible Smear-Negative Undiagnosed</t>
+  </si>
+  <si>
+    <t>Multidrug-Resistant Smear-Negative Undiagnosed</t>
+  </si>
+  <si>
+    <t>Extensively Drug-Resistant Smear-Negative Undiagnosed</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>Slow-LTBI Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>Fast-LTBI Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Slow Undiagnosed)</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Fast Undiagnosed)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Slow Undiagnosed)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Fast Undiagnosed)</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Slow Diagnosed)</t>
+  </si>
+  <si>
+    <t>LTBI-SPos Progression Rate (Fast Diagnosed)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Slow Diagnosed)</t>
+  </si>
+  <si>
+    <t>LTBI-SNeg Progression Rate (Fast Diagnosed)</t>
+  </si>
+  <si>
+    <t>SPos DS Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SPos MDR Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SPos XDR Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SNeg DS Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SNeg MDR Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SNeg XDR Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>ltsds+_rate</t>
+  </si>
+  <si>
+    <t>ltfds+_rate</t>
+  </si>
+  <si>
+    <t>ltsds-_rate</t>
+  </si>
+  <si>
+    <t>ltfds-_rate</t>
+  </si>
+  <si>
+    <t>s+ddd_rate</t>
+  </si>
+  <si>
+    <t>s+mdd_rate</t>
+  </si>
+  <si>
+    <t>s+xdd_rate</t>
+  </si>
+  <si>
+    <t>s-ddd_rate</t>
+  </si>
+  <si>
+    <t>s-mdd_rate</t>
+  </si>
+  <si>
+    <t>s-xdd_rate</t>
+  </si>
+  <si>
+    <t>ltsdiag_rate</t>
+  </si>
+  <si>
+    <t>ltfdiag_rate</t>
+  </si>
+  <si>
+    <t>ea</t>
+  </si>
+  <si>
+    <t>eb</t>
+  </si>
+  <si>
+    <t>ec</t>
+  </si>
+  <si>
+    <t>ed</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>ef</t>
+  </si>
+  <si>
+    <t>SPos DS Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SPos MDR Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SPos XDR Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SNeg DS Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SNeg MDR Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SNeg XDR Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>s+ddiag_rate</t>
+  </si>
+  <si>
+    <t>s+mdiag_rate</t>
+  </si>
+  <si>
+    <t>s+xdiag_rate</t>
+  </si>
+  <si>
+    <t>s-ddiag_rate</t>
+  </si>
+  <si>
+    <t>s-mdiag_rate</t>
+  </si>
+  <si>
+    <t>s-xdiag_rate</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>fb</t>
+  </si>
+  <si>
+    <t>fc</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
+    <t>fe</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>SPos DS Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SPos MDR Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SPos XDR Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SNeg DS Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SNeg MDR Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SNeg XDR Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>(-12,1)</t>
+  </si>
+  <si>
+    <t>(-12,-1)</t>
+  </si>
+  <si>
+    <t>(12,1)</t>
+  </si>
+  <si>
+    <t>(12,-1)</t>
+  </si>
+  <si>
+    <t>(-10,2)</t>
+  </si>
+  <si>
+    <t>(10,2)</t>
+  </si>
+  <si>
+    <t>(-12,0)</t>
+  </si>
+  <si>
+    <t>(-10,0)</t>
+  </si>
+  <si>
+    <t>(-8,0)</t>
+  </si>
+  <si>
+    <t>(8,0)</t>
+  </si>
+  <si>
+    <t>(10,0)</t>
+  </si>
+  <si>
+    <t>(12,0)</t>
+  </si>
+  <si>
+    <t>(-5,-0.5)</t>
+  </si>
+  <si>
+    <t>(5,-0.5)</t>
+  </si>
+  <si>
+    <t>(-9,3)</t>
+  </si>
+  <si>
+    <t>(9,3)</t>
+  </si>
+  <si>
+    <t>(-2,4)</t>
+  </si>
+  <si>
+    <t>(-5.5,3.5)</t>
+  </si>
+  <si>
+    <t>(2,4)</t>
+  </si>
+  <si>
+    <t>(5.5,3.5)</t>
+  </si>
+  <si>
+    <t>(0,5)</t>
+  </si>
+  <si>
+    <t>(5,5.5)</t>
+  </si>
+  <si>
+    <t>(-5,5.5)</t>
+  </si>
+  <si>
+    <t>ddis</t>
+  </si>
+  <si>
+    <t>doth</t>
+  </si>
+  <si>
+    <t>Dead (Cause: TB)</t>
+  </si>
+  <si>
+    <t>Dead (Cause: Other)</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>doth_rate</t>
+  </si>
+  <si>
+    <t>Death Rate (Other Causes)</t>
+  </si>
+  <si>
     <t>Dead</t>
   </si>
   <si>
-    <t>Vaccinated</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>ac</t>
-  </si>
-  <si>
-    <t>ad</t>
-  </si>
-  <si>
-    <t>ae</t>
-  </si>
-  <si>
-    <t>af</t>
-  </si>
-  <si>
-    <t>ag</t>
-  </si>
-  <si>
-    <t>ah</t>
-  </si>
-  <si>
-    <t>ai</t>
-  </si>
-  <si>
-    <t>ba</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>bc</t>
-  </si>
-  <si>
-    <t>bd</t>
-  </si>
-  <si>
-    <t>be</t>
-  </si>
-  <si>
-    <t>bf</t>
-  </si>
-  <si>
-    <t>bg</t>
-  </si>
-  <si>
-    <t>bh</t>
-  </si>
-  <si>
-    <t>bi</t>
-  </si>
-  <si>
-    <t>aj</t>
-  </si>
-  <si>
-    <t>ak</t>
-  </si>
-  <si>
-    <t>al</t>
-  </si>
-  <si>
-    <t>bj</t>
-  </si>
-  <si>
-    <t>bk</t>
-  </si>
-  <si>
-    <t>bl</t>
-  </si>
-  <si>
-    <t>am</t>
-  </si>
-  <si>
-    <t>an</t>
-  </si>
-  <si>
-    <t>ao</t>
-  </si>
-  <si>
-    <t>ap</t>
-  </si>
-  <si>
-    <t>aq</t>
-  </si>
-  <si>
-    <t>ar</t>
-  </si>
-  <si>
-    <t>bm</t>
-  </si>
-  <si>
-    <t>bn</t>
-  </si>
-  <si>
-    <t>bo</t>
-  </si>
-  <si>
-    <t>bp</t>
-  </si>
-  <si>
-    <t>bq</t>
-  </si>
-  <si>
-    <t>br</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>Vaccination Rate</t>
-  </si>
-  <si>
-    <t>Infection Rate (Susceptible)</t>
-  </si>
-  <si>
-    <t>Infection Rate (Vaccinated)</t>
-  </si>
-  <si>
-    <t>Slow-LTBI Partition Fraction</t>
-  </si>
-  <si>
-    <t>Fast-LTBI Partition Fraction</t>
-  </si>
-  <si>
-    <t>Slow-LTBI Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>Slow-LTBI Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>Fast-LTBI Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>Fast-LTBI Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>LTBI-SPos Progression Rate (Slow Treated)</t>
-  </si>
-  <si>
-    <t>LTBI-SPos Progression Rate (Fast Treated)</t>
-  </si>
-  <si>
-    <t>LTBI-SNeg Progression Rate (Slow Treated)</t>
-  </si>
-  <si>
-    <t>LTBI-SNeg Progression Rate (Fast Treated)</t>
-  </si>
-  <si>
-    <t>Slow-LTBI Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>Fast-LTBI Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>Reinfection Rate (Recovered)</t>
-  </si>
-  <si>
-    <t>SPos MDR Partition Fraction</t>
-  </si>
-  <si>
-    <t>SPos XDR Partition Fraction</t>
-  </si>
-  <si>
-    <t>SPos DS Partition Fraction</t>
-  </si>
-  <si>
-    <t>SPos DS Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SPos DS Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SPos MDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SPos MDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SPos XDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SPos XDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SPos DS Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SPos MDR Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SPos XDR Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SPos DS Death Rate (Treated)</t>
-  </si>
-  <si>
-    <t>SPos MDR Death Rate (Treated)</t>
-  </si>
-  <si>
-    <t>SPos XDR Death Rate (Treated)</t>
-  </si>
-  <si>
-    <t>SNeg DS Partition Fraction</t>
-  </si>
-  <si>
-    <t>SNeg MDR Partition Fraction</t>
-  </si>
-  <si>
-    <t>SNeg XDR Partition Fraction</t>
-  </si>
-  <si>
-    <t>SNeg DS Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SNeg DS Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SNeg MDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SNeg MDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SNeg XDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SNeg XDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SNeg DS Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SNeg MDR Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SNeg XDR Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SNeg DS Death Rate (Treated)</t>
-  </si>
-  <si>
-    <t>SNeg MDR Death Rate (Treated)</t>
-  </si>
-  <si>
-    <t>SNeg XDR Death Rate (Treated)</t>
-  </si>
-  <si>
-    <t>v_rate</t>
-  </si>
-  <si>
-    <t>infs_rate</t>
-  </si>
-  <si>
-    <t>infv_rate</t>
-  </si>
-  <si>
-    <t>lts_frac</t>
-  </si>
-  <si>
-    <t>ltf_frac</t>
-  </si>
-  <si>
-    <t>ltsyes_rate</t>
-  </si>
-  <si>
-    <t>ltsno_rate</t>
-  </si>
-  <si>
-    <t>ltfyes_rate</t>
-  </si>
-  <si>
-    <t>ltfno_rate</t>
-  </si>
-  <si>
-    <t>ltsus+_rate</t>
-  </si>
-  <si>
-    <t>ltsts+_rate</t>
-  </si>
-  <si>
-    <t>ltfus+_rate</t>
-  </si>
-  <si>
-    <t>ltfts+_rate</t>
-  </si>
-  <si>
-    <t>ltsus-_rate</t>
-  </si>
-  <si>
-    <t>ltsts-_rate</t>
-  </si>
-  <si>
-    <t>ltfus-_rate</t>
-  </si>
-  <si>
-    <t>ltfts-_rate</t>
-  </si>
-  <si>
-    <t>infr_rate</t>
-  </si>
-  <si>
-    <t>ltssuc_rate</t>
-  </si>
-  <si>
-    <t>ltfsuc_rate</t>
-  </si>
-  <si>
-    <t>s+d_frac</t>
-  </si>
-  <si>
-    <t>s+m_frac</t>
-  </si>
-  <si>
-    <t>s+x_frac</t>
-  </si>
-  <si>
-    <t>s+dyes_rate</t>
-  </si>
-  <si>
-    <t>s+dno_rate</t>
-  </si>
-  <si>
-    <t>s+myes_rate</t>
-  </si>
-  <si>
-    <t>s+mno_rate</t>
-  </si>
-  <si>
-    <t>s+xyes_rate</t>
-  </si>
-  <si>
-    <t>s+xno_rate</t>
-  </si>
-  <si>
-    <t>s+dsuc_rate</t>
-  </si>
-  <si>
-    <t>s+msuc_rate</t>
-  </si>
-  <si>
-    <t>s+xsuc_rate</t>
-  </si>
-  <si>
-    <t>s+dud_rate</t>
-  </si>
-  <si>
-    <t>s+dtd_rate</t>
-  </si>
-  <si>
-    <t>s+mud_rate</t>
-  </si>
-  <si>
-    <t>s+mtd_rate</t>
-  </si>
-  <si>
-    <t>s+xud_rate</t>
-  </si>
-  <si>
-    <t>s+xtd_rate</t>
-  </si>
-  <si>
-    <t>s-d_frac</t>
-  </si>
-  <si>
-    <t>s-m_frac</t>
-  </si>
-  <si>
-    <t>s-x_frac</t>
-  </si>
-  <si>
-    <t>s-dyes_rate</t>
-  </si>
-  <si>
-    <t>s-dno_rate</t>
-  </si>
-  <si>
-    <t>s-myes_rate</t>
-  </si>
-  <si>
-    <t>s-mno_rate</t>
-  </si>
-  <si>
-    <t>s-xyes_rate</t>
-  </si>
-  <si>
-    <t>s-xno_rate</t>
-  </si>
-  <si>
-    <t>s-dsuc_rate</t>
-  </si>
-  <si>
-    <t>s-msuc_rate</t>
-  </si>
-  <si>
-    <t>s-xsuc_rate</t>
-  </si>
-  <si>
-    <t>s-dud_rate</t>
-  </si>
-  <si>
-    <t>s-dtd_rate</t>
-  </si>
-  <si>
-    <t>s-mud_rate</t>
-  </si>
-  <si>
-    <t>s-mtd_rate</t>
-  </si>
-  <si>
-    <t>s-xud_rate</t>
-  </si>
-  <si>
-    <t>s-xtd_rate</t>
-  </si>
-  <si>
-    <t>Plot Coordinates</t>
-  </si>
-  <si>
-    <t>(-10,1)</t>
-  </si>
-  <si>
-    <t>(-10,-1)</t>
-  </si>
-  <si>
-    <t>(-8,1)</t>
-  </si>
-  <si>
-    <t>(-8,-1)</t>
-  </si>
-  <si>
-    <t>(8,1)</t>
-  </si>
-  <si>
-    <t>(8,-1)</t>
-  </si>
-  <si>
-    <t>(10,1)</t>
-  </si>
-  <si>
-    <t>(10,-1)</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>ltsd</t>
-  </si>
-  <si>
-    <t>Slow Latent Diagnosed</t>
-  </si>
-  <si>
-    <t>ltfd</t>
-  </si>
-  <si>
-    <t>Fast Latent Diagnosed</t>
-  </si>
-  <si>
-    <t>s+dd</t>
-  </si>
-  <si>
-    <t>Drug-Susceptible Smear-Positive Diagnosed</t>
-  </si>
-  <si>
-    <t>s+md</t>
-  </si>
-  <si>
-    <t>Multidrug-Resistant Smear-Positive Diagnosed</t>
-  </si>
-  <si>
-    <t>s+xd</t>
-  </si>
-  <si>
-    <t>Extensively Drug-Resistant Smear-Positive Diagnosed</t>
-  </si>
-  <si>
-    <t>s-dd</t>
-  </si>
-  <si>
-    <t>Drug-Susceptible Smear-Negative Diagnosed</t>
-  </si>
-  <si>
-    <t>s-md</t>
-  </si>
-  <si>
-    <t>Multidrug-Resistant Smear-Negative Diagnosed</t>
-  </si>
-  <si>
-    <t>s-xd</t>
-  </si>
-  <si>
-    <t>Extensively Drug-Resistant Smear-Negative Diagnosed</t>
-  </si>
-  <si>
-    <t>Slow Latent Undiagnosed</t>
-  </si>
-  <si>
-    <t>Fast Latent Undiagnosed</t>
-  </si>
-  <si>
-    <t>Drug-Susceptible Smear-Positive Undiagnosed</t>
-  </si>
-  <si>
-    <t>Multidrug-Resistant Smear-Positive Undiagnosed</t>
-  </si>
-  <si>
-    <t>Extensively Drug-Resistant Smear-Positive Undiagnosed</t>
-  </si>
-  <si>
-    <t>Drug-Susceptible Smear-Negative Undiagnosed</t>
-  </si>
-  <si>
-    <t>Multidrug-Resistant Smear-Negative Undiagnosed</t>
-  </si>
-  <si>
-    <t>Extensively Drug-Resistant Smear-Negative Undiagnosed</t>
-  </si>
-  <si>
-    <t>da</t>
-  </si>
-  <si>
-    <t>db</t>
-  </si>
-  <si>
-    <t>dc</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>Slow-LTBI Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>Fast-LTBI Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>LTBI-SPos Progression Rate (Slow Undiagnosed)</t>
-  </si>
-  <si>
-    <t>LTBI-SPos Progression Rate (Fast Undiagnosed)</t>
-  </si>
-  <si>
-    <t>LTBI-SNeg Progression Rate (Slow Undiagnosed)</t>
-  </si>
-  <si>
-    <t>LTBI-SNeg Progression Rate (Fast Undiagnosed)</t>
-  </si>
-  <si>
-    <t>LTBI-SPos Progression Rate (Slow Diagnosed)</t>
-  </si>
-  <si>
-    <t>LTBI-SPos Progression Rate (Fast Diagnosed)</t>
-  </si>
-  <si>
-    <t>LTBI-SNeg Progression Rate (Slow Diagnosed)</t>
-  </si>
-  <si>
-    <t>LTBI-SNeg Progression Rate (Fast Diagnosed)</t>
-  </si>
-  <si>
-    <t>SPos DS Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SPos MDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SPos XDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg DS Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg MDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg XDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>ltsds+_rate</t>
-  </si>
-  <si>
-    <t>ltfds+_rate</t>
-  </si>
-  <si>
-    <t>ltsds-_rate</t>
-  </si>
-  <si>
-    <t>ltfds-_rate</t>
-  </si>
-  <si>
-    <t>s+ddd_rate</t>
-  </si>
-  <si>
-    <t>s+mdd_rate</t>
-  </si>
-  <si>
-    <t>s+xdd_rate</t>
-  </si>
-  <si>
-    <t>s-ddd_rate</t>
-  </si>
-  <si>
-    <t>s-mdd_rate</t>
-  </si>
-  <si>
-    <t>s-xdd_rate</t>
-  </si>
-  <si>
-    <t>ltsdiag_rate</t>
-  </si>
-  <si>
-    <t>ltfdiag_rate</t>
-  </si>
-  <si>
-    <t>ea</t>
-  </si>
-  <si>
-    <t>eb</t>
-  </si>
-  <si>
-    <t>ec</t>
-  </si>
-  <si>
-    <t>ed</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>ef</t>
-  </si>
-  <si>
-    <t>SPos DS Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SPos MDR Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SPos XDR Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SNeg DS Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SNeg MDR Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SNeg XDR Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>s+ddiag_rate</t>
-  </si>
-  <si>
-    <t>s+mdiag_rate</t>
-  </si>
-  <si>
-    <t>s+xdiag_rate</t>
-  </si>
-  <si>
-    <t>s-ddiag_rate</t>
-  </si>
-  <si>
-    <t>s-mdiag_rate</t>
-  </si>
-  <si>
-    <t>s-xdiag_rate</t>
-  </si>
-  <si>
-    <t>fa</t>
-  </si>
-  <si>
-    <t>fb</t>
-  </si>
-  <si>
-    <t>fc</t>
-  </si>
-  <si>
-    <t>fd</t>
-  </si>
-  <si>
-    <t>fe</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>SPos DS Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SPos MDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SPos XDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg DS Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg MDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg XDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>(-12,1)</t>
-  </si>
-  <si>
-    <t>(-12,-1)</t>
-  </si>
-  <si>
-    <t>(12,1)</t>
-  </si>
-  <si>
-    <t>(12,-1)</t>
-  </si>
-  <si>
-    <t>(-10,2)</t>
-  </si>
-  <si>
-    <t>(10,2)</t>
-  </si>
-  <si>
-    <t>(-12,0)</t>
-  </si>
-  <si>
-    <t>(-10,0)</t>
-  </si>
-  <si>
-    <t>(-8,0)</t>
-  </si>
-  <si>
-    <t>(8,0)</t>
-  </si>
-  <si>
-    <t>(10,0)</t>
-  </si>
-  <si>
-    <t>(12,0)</t>
-  </si>
-  <si>
-    <t>(-5,-0.5)</t>
-  </si>
-  <si>
-    <t>(5,-0.5)</t>
-  </si>
-  <si>
-    <t>(-9,3)</t>
-  </si>
-  <si>
-    <t>(9,3)</t>
-  </si>
-  <si>
-    <t>(-2,4)</t>
-  </si>
-  <si>
-    <t>(-5.5,3.5)</t>
-  </si>
-  <si>
-    <t>(2,4)</t>
-  </si>
-  <si>
-    <t>(5.5,3.5)</t>
-  </si>
-  <si>
-    <t>(0,5)</t>
-  </si>
-  <si>
-    <t>(5,5.5)</t>
-  </si>
-  <si>
-    <t>(-5,5.5)</t>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -1487,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1498,9 +1519,10 @@
     <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1508,10 +1530,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1519,21 +1544,21 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1541,32 +1566,32 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1574,32 +1599,32 @@
         <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1607,10 +1632,10 @@
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1618,32 +1643,32 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1651,32 +1676,32 @@
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1684,32 +1709,32 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1717,10 +1742,10 @@
         <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1728,32 +1753,32 @@
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1761,32 +1786,32 @@
         <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1794,32 +1819,32 @@
         <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1827,29 +1852,43 @@
         <v>34</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>318</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>320</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>319</v>
+      </c>
+      <c r="B33" t="s">
+        <v>321</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -1860,18 +1899,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF32"/>
+  <dimension ref="A1:AG33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA39" sqref="AA39"/>
+      <selection activeCell="AG31" sqref="AG31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="32" width="5.77734375" customWidth="1"/>
+    <col min="1" max="33" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -1886,7 +1925,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>13</v>
@@ -1895,7 +1934,7 @@
         <v>12</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>14</v>
@@ -1907,7 +1946,7 @@
         <v>17</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>18</v>
@@ -1916,7 +1955,7 @@
         <v>20</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>21</v>
@@ -1925,7 +1964,7 @@
         <v>22</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>23</v>
@@ -1937,7 +1976,7 @@
         <v>26</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="X1" s="5" t="s">
         <v>27</v>
@@ -1946,7 +1985,7 @@
         <v>28</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AA1" s="5" t="s">
         <v>29</v>
@@ -1955,7 +1994,7 @@
         <v>30</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AD1" s="5" t="s">
         <v>31</v>
@@ -1964,19 +2003,22 @@
         <v>35</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -2004,17 +2046,20 @@
       <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
       <c r="AD2" s="8"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="8"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -2042,10 +2087,13 @@
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
       <c r="AD3" s="11"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="11"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -2053,12 +2101,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="11"/>
@@ -2082,10 +2130,13 @@
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
       <c r="AD4" s="11"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="11"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -2094,14 +2145,14 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="11"/>
       <c r="K5" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
@@ -2113,7 +2164,7 @@
       <c r="S5" s="10"/>
       <c r="T5" s="11"/>
       <c r="U5" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
@@ -2124,12 +2175,15 @@
       <c r="AB5" s="10"/>
       <c r="AC5" s="10"/>
       <c r="AD5" s="11"/>
-      <c r="AE5" s="10"/>
-      <c r="AF5" s="11"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
@@ -2137,13 +2191,13 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="11"/>
       <c r="K6" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -2155,7 +2209,7 @@
       <c r="S6" s="10"/>
       <c r="T6" s="11"/>
       <c r="U6" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
@@ -2166,10 +2220,13 @@
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
       <c r="AD6" s="11"/>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="11"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -2178,14 +2235,14 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="11"/>
       <c r="K7" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -2197,7 +2254,7 @@
       <c r="S7" s="10"/>
       <c r="T7" s="11"/>
       <c r="U7" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
@@ -2208,12 +2265,15 @@
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>
       <c r="AD7" s="11"/>
-      <c r="AE7" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF7" s="11"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -2225,11 +2285,11 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -2241,7 +2301,7 @@
       <c r="S8" s="10"/>
       <c r="T8" s="11"/>
       <c r="U8" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
@@ -2252,12 +2312,15 @@
       <c r="AB8" s="10"/>
       <c r="AC8" s="10"/>
       <c r="AD8" s="11"/>
-      <c r="AE8" s="10"/>
-      <c r="AF8" s="11"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
@@ -2268,10 +2331,10 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -2283,7 +2346,7 @@
       <c r="S9" s="10"/>
       <c r="T9" s="11"/>
       <c r="U9" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -2294,10 +2357,13 @@
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
       <c r="AD9" s="11"/>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="11"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -2309,11 +2375,11 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
@@ -2325,7 +2391,7 @@
       <c r="S10" s="10"/>
       <c r="T10" s="11"/>
       <c r="U10" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
@@ -2336,12 +2402,15 @@
       <c r="AB10" s="10"/>
       <c r="AC10" s="10"/>
       <c r="AD10" s="11"/>
-      <c r="AE10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF10" s="11"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="14" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -2356,17 +2425,17 @@
       <c r="J11" s="8"/>
       <c r="K11" s="6"/>
       <c r="L11" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S11" s="7"/>
       <c r="T11" s="8"/>
@@ -2380,10 +2449,13 @@
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="8"/>
-      <c r="AE11" s="7"/>
-      <c r="AF11" s="8"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
@@ -2399,7 +2471,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -2418,14 +2490,17 @@
       <c r="AB12" s="10"/>
       <c r="AC12" s="10"/>
       <c r="AD12" s="11"/>
-      <c r="AE12" s="10"/>
-      <c r="AF12" s="11" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="AG12" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
@@ -2440,7 +2515,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
@@ -2458,12 +2533,15 @@
       <c r="AB13" s="10"/>
       <c r="AC13" s="10"/>
       <c r="AD13" s="11"/>
-      <c r="AE13" s="10"/>
-      <c r="AF13" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG13" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -2479,7 +2557,7 @@
       <c r="K14" s="9"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2498,14 +2576,17 @@
       <c r="AB14" s="10"/>
       <c r="AC14" s="10"/>
       <c r="AD14" s="11"/>
-      <c r="AE14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF14" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF14" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG14" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
@@ -2524,7 +2605,7 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
@@ -2540,14 +2621,17 @@
       <c r="AB15" s="10"/>
       <c r="AC15" s="10"/>
       <c r="AD15" s="11"/>
-      <c r="AE15" s="10"/>
-      <c r="AF15" s="11" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="AG15" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -2565,7 +2649,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
@@ -2580,12 +2664,15 @@
       <c r="AB16" s="10"/>
       <c r="AC16" s="10"/>
       <c r="AD16" s="11"/>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG16" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -2604,7 +2691,7 @@
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
@@ -2620,14 +2707,17 @@
       <c r="AB17" s="10"/>
       <c r="AC17" s="10"/>
       <c r="AD17" s="11"/>
-      <c r="AE17" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF17" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE17" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG17" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
@@ -2649,7 +2739,7 @@
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="T18" s="11"/>
       <c r="U18" s="9"/>
@@ -2662,14 +2752,17 @@
       <c r="AB18" s="10"/>
       <c r="AC18" s="10"/>
       <c r="AD18" s="11"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="11" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="AG18" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
@@ -2690,7 +2783,7 @@
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="U19" s="9"/>
       <c r="V19" s="10"/>
@@ -2702,12 +2795,15 @@
       <c r="AB19" s="10"/>
       <c r="AC19" s="10"/>
       <c r="AD19" s="11"/>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG19" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
@@ -2729,7 +2825,7 @@
       <c r="Q20" s="13"/>
       <c r="R20" s="13"/>
       <c r="S20" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T20" s="14"/>
       <c r="U20" s="12"/>
@@ -2742,14 +2838,17 @@
       <c r="AB20" s="13"/>
       <c r="AC20" s="13"/>
       <c r="AD20" s="14"/>
-      <c r="AE20" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF20" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE20" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF20" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG20" s="14" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
@@ -2774,24 +2873,27 @@
       <c r="T21" s="8"/>
       <c r="U21" s="6"/>
       <c r="V21" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
       <c r="Y21" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Z21" s="7"/>
       <c r="AA21" s="7"/>
       <c r="AB21" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AC21" s="7"/>
       <c r="AD21" s="8"/>
-      <c r="AE21" s="7"/>
-      <c r="AF21" s="8"/>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -2817,7 +2919,7 @@
       <c r="U22" s="9"/>
       <c r="V22" s="10"/>
       <c r="W22" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
@@ -2826,14 +2928,17 @@
       <c r="AB22" s="10"/>
       <c r="AC22" s="10"/>
       <c r="AD22" s="11"/>
-      <c r="AE22" s="10"/>
-      <c r="AF22" s="11" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="AG22" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -2858,7 +2963,7 @@
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
       <c r="X23" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="10"/>
@@ -2866,12 +2971,15 @@
       <c r="AB23" s="10"/>
       <c r="AC23" s="10"/>
       <c r="AD23" s="11"/>
-      <c r="AE23" s="10"/>
-      <c r="AF23" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG23" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
@@ -2897,7 +3005,7 @@
       <c r="U24" s="9"/>
       <c r="V24" s="10"/>
       <c r="W24" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="X24" s="10"/>
       <c r="Y24" s="10"/>
@@ -2906,14 +3014,17 @@
       <c r="AB24" s="10"/>
       <c r="AC24" s="10"/>
       <c r="AD24" s="11"/>
-      <c r="AE24" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF24" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE24" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF24" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG24" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
@@ -2942,20 +3053,23 @@
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
       <c r="Z25" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="AA25" s="10"/>
       <c r="AB25" s="10"/>
       <c r="AC25" s="10"/>
       <c r="AD25" s="11"/>
-      <c r="AE25" s="10"/>
-      <c r="AF25" s="11" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="AG25" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
@@ -2983,17 +3097,20 @@
       <c r="Y26" s="10"/>
       <c r="Z26" s="10"/>
       <c r="AA26" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AB26" s="10"/>
       <c r="AC26" s="10"/>
       <c r="AD26" s="11"/>
-      <c r="AE26" s="10"/>
-      <c r="AF26" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG26" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
@@ -3022,20 +3139,23 @@
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
       <c r="Z27" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AA27" s="10"/>
       <c r="AB27" s="10"/>
       <c r="AC27" s="10"/>
       <c r="AD27" s="11"/>
-      <c r="AE27" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF27" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE27" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG27" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -3067,17 +3187,20 @@
       <c r="AA28" s="10"/>
       <c r="AB28" s="10"/>
       <c r="AC28" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AD28" s="11"/>
-      <c r="AE28" s="10"/>
-      <c r="AF28" s="11" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="AG28" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
@@ -3108,14 +3231,17 @@
       <c r="AB29" s="10"/>
       <c r="AC29" s="10"/>
       <c r="AD29" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE29" s="10"/>
-      <c r="AF29" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG29" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>31</v>
       </c>
@@ -3147,24 +3273,27 @@
       <c r="AA30" s="13"/>
       <c r="AB30" s="13"/>
       <c r="AC30" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AD30" s="14"/>
-      <c r="AE30" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF30" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE30" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF30" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG30" s="14" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -3192,44 +3321,85 @@
       <c r="AB31" s="10"/>
       <c r="AC31" s="10"/>
       <c r="AD31" s="11"/>
-      <c r="AE31" s="10"/>
-      <c r="AF31" s="11"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AE31" s="6"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="12"/>
-      <c r="V32" s="13"/>
-      <c r="W32" s="13"/>
-      <c r="X32" s="13"/>
-      <c r="Y32" s="13"/>
-      <c r="Z32" s="13"/>
-      <c r="AA32" s="13"/>
-      <c r="AB32" s="13"/>
-      <c r="AC32" s="13"/>
-      <c r="AD32" s="14"/>
-      <c r="AE32" s="13"/>
-      <c r="AF32" s="14"/>
+        <v>318</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+      <c r="X32" s="10"/>
+      <c r="Y32" s="10"/>
+      <c r="Z32" s="10"/>
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="10"/>
+      <c r="AC32" s="10"/>
+      <c r="AD32" s="11"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="11"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="13"/>
+      <c r="AA33" s="13"/>
+      <c r="AB33" s="13"/>
+      <c r="AC33" s="13"/>
+      <c r="AD33" s="14"/>
+      <c r="AE33" s="12"/>
+      <c r="AF33" s="13"/>
+      <c r="AG33" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3238,10 +3408,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3257,35 +3427,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -3293,24 +3463,24 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -3318,24 +3488,24 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -3343,134 +3513,134 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -3478,101 +3648,101 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D28" s="2">
         <v>1</v>
@@ -3580,35 +3750,35 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C31" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
@@ -3616,13 +3786,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D32" s="2">
         <v>1</v>
@@ -3630,24 +3800,24 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D34" s="2">
         <v>1</v>
@@ -3655,453 +3825,464 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C35" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C39" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C43" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C49" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C50" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C52" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C53" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C54" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C55" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C59" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C60" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C62" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C63" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C64" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C67" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C70" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C72" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C73" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C74" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C75" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>323</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C76" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prevalence and infection number plotting
Custom characteristics are now calculated at the end of a model run and
subsequently plotted in the temporary plotting script within the Project
object.
Characteristics in the cascade workbook can be tagged to 'Plot
Percentage', so that at plotting time, a fraction may be multiplied by
100.
This thus allows for infections and prevalence to be calculated, as well
as metrics such as living people and so on.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="348">
   <si>
     <t>Code Label</t>
   </si>
@@ -994,9 +994,6 @@
     <t>Death Rate (Other Causes)</t>
   </si>
   <si>
-    <t>Dead</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -1030,21 +1027,6 @@
     <t>alive</t>
   </si>
   <si>
-    <t>Total Living Population</t>
-  </si>
-  <si>
-    <t>Latent Prevalence</t>
-  </si>
-  <si>
-    <t>Active Prevalence</t>
-  </si>
-  <si>
-    <t>Smear Positive Prevalence</t>
-  </si>
-  <si>
-    <t>Smear Negative Prevalence</t>
-  </si>
-  <si>
     <t>lt_prev</t>
   </si>
   <si>
@@ -1057,10 +1039,28 @@
     <t>s-_prev</t>
   </si>
   <si>
-    <t>s+inf</t>
-  </si>
-  <si>
     <t>Denominator</t>
+  </si>
+  <si>
+    <t>People Alive</t>
+  </si>
+  <si>
+    <t>Latent Prevalence (%)</t>
+  </si>
+  <si>
+    <t>Smear Positive Prevalence (%)</t>
+  </si>
+  <si>
+    <t>Smear Negative Prevalence (%)</t>
+  </si>
+  <si>
+    <t>Active Prevalence (%)</t>
+  </si>
+  <si>
+    <t>Dead Tag</t>
+  </si>
+  <si>
+    <t>Plot Percentage</t>
   </si>
 </sst>
 </file>
@@ -1574,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,7 +1597,7 @@
         <v>197</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1941,7 +1941,7 @@
         <v>308</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1952,7 +1952,7 @@
         <v>321</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -1963,245 +1963,261 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>347</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>207</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>213</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>215</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>217</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>219</v>
+      </c>
+      <c r="K4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" t="s">
+        <v>221</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E5" t="s">
+        <v>333</v>
+      </c>
+      <c r="F5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>331</v>
+      </c>
+      <c r="I6" t="s">
         <v>332</v>
       </c>
-      <c r="B2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>209</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>334</v>
-      </c>
-      <c r="B3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>213</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>215</v>
-      </c>
-      <c r="M3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D7" t="s">
         <v>335</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E7" t="s">
         <v>331</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>217</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>219</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" t="s">
-        <v>221</v>
-      </c>
-      <c r="M4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B8" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8" t="s">
+        <v>335</v>
+      </c>
+      <c r="E8" t="s">
         <v>333</v>
       </c>
-      <c r="B5" t="s">
-        <v>329</v>
-      </c>
-      <c r="D5" t="s">
-        <v>346</v>
-      </c>
-      <c r="E5" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>336</v>
-      </c>
-      <c r="B6" t="s">
-        <v>337</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>332</v>
-      </c>
-      <c r="H6" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B7" t="s">
-        <v>338</v>
-      </c>
-      <c r="C7" t="s">
-        <v>336</v>
-      </c>
-      <c r="D7" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" t="s">
         <v>344</v>
       </c>
-      <c r="B8" t="s">
-        <v>340</v>
-      </c>
-      <c r="C8" t="s">
-        <v>336</v>
-      </c>
-      <c r="D8" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>345</v>
-      </c>
-      <c r="B9" t="s">
-        <v>341</v>
-      </c>
-      <c r="C9" t="s">
-        <v>336</v>
+      <c r="C9" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="D9" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B10" t="s">
-        <v>339</v>
-      </c>
-      <c r="C10" t="s">
-        <v>336</v>
+        <v>345</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="D10" t="s">
-        <v>333</v>
+        <v>335</v>
+      </c>
+      <c r="E10" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compartment tag to suppress plots
Just a quick, hopefully robust edit that allows compartments in the
cascade workbook to be tagged with plot suppression.
Basically the nodes and relevant edges will not be plotted by
settings.plotCascade().
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="349">
   <si>
     <t>Code Label</t>
   </si>
@@ -940,12 +940,6 @@
     <t>(12,0)</t>
   </si>
   <si>
-    <t>(-5,-0.5)</t>
-  </si>
-  <si>
-    <t>(5,-0.5)</t>
-  </si>
-  <si>
     <t>(-9,3)</t>
   </si>
   <si>
@@ -1061,6 +1055,15 @@
   </si>
   <si>
     <t>Plot Percentage</t>
+  </si>
+  <si>
+    <t>No Plot</t>
+  </si>
+  <si>
+    <t>(0,0.5)</t>
+  </si>
+  <si>
+    <t>(0,0)</t>
   </si>
 </sst>
 </file>
@@ -1572,10 +1575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1583,10 +1586,10 @@
     <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
+    <col min="4" max="5" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1597,10 +1600,13 @@
         <v>197</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1608,10 +1614,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1619,10 +1625,10 @@
         <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1630,10 +1636,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1641,10 +1647,10 @@
         <v>223</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>207</v>
       </c>
@@ -1652,10 +1658,10 @@
         <v>208</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1663,10 +1669,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1674,10 +1680,10 @@
         <v>224</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -1685,10 +1691,10 @@
         <v>210</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1696,10 +1702,10 @@
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1710,7 +1716,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1721,7 +1727,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>211</v>
       </c>
@@ -1732,7 +1738,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>213</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1787,7 +1793,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>215</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1820,7 +1826,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>217</v>
       </c>
@@ -1842,7 +1848,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>219</v>
       </c>
@@ -1875,7 +1881,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1897,7 +1903,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>221</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1927,32 +1933,38 @@
         <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>316</v>
+      </c>
+      <c r="B32" t="s">
         <v>318</v>
       </c>
-      <c r="B32" t="s">
-        <v>320</v>
-      </c>
       <c r="C32" s="2" t="s">
-        <v>308</v>
+        <v>347</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>317</v>
+      </c>
+      <c r="B33" t="s">
         <v>319</v>
       </c>
-      <c r="B33" t="s">
-        <v>321</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -1965,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2001,21 +2013,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -2041,10 +2053,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -2079,10 +2091,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -2117,24 +2129,24 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E5" t="s">
+        <v>331</v>
+      </c>
+      <c r="F5" t="s">
         <v>332</v>
-      </c>
-      <c r="B5" t="s">
-        <v>328</v>
-      </c>
-      <c r="E5" t="s">
-        <v>333</v>
-      </c>
-      <c r="F5" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -2146,78 +2158,78 @@
         <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D10" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -2332,10 +2344,10 @@
         <v>35</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
@@ -2378,7 +2390,7 @@
       <c r="AE2" s="6"/>
       <c r="AF2" s="7"/>
       <c r="AG2" s="8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -2419,7 +2431,7 @@
       <c r="AE3" s="9"/>
       <c r="AF3" s="10"/>
       <c r="AG3" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -2462,7 +2474,7 @@
       <c r="AE4" s="9"/>
       <c r="AF4" s="10"/>
       <c r="AG4" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -2507,7 +2519,7 @@
       <c r="AE5" s="9"/>
       <c r="AF5" s="10"/>
       <c r="AG5" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
@@ -2552,7 +2564,7 @@
       <c r="AE6" s="9"/>
       <c r="AF6" s="10"/>
       <c r="AG6" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
@@ -2599,7 +2611,7 @@
       </c>
       <c r="AF7" s="10"/>
       <c r="AG7" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
@@ -2644,7 +2656,7 @@
       <c r="AE8" s="9"/>
       <c r="AF8" s="10"/>
       <c r="AG8" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
@@ -2689,7 +2701,7 @@
       <c r="AE9" s="9"/>
       <c r="AF9" s="10"/>
       <c r="AG9" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
@@ -2736,7 +2748,7 @@
       </c>
       <c r="AF10" s="13"/>
       <c r="AG10" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
@@ -2781,7 +2793,7 @@
       <c r="AE11" s="6"/>
       <c r="AF11" s="7"/>
       <c r="AG11" s="8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
@@ -2824,7 +2836,7 @@
         <v>283</v>
       </c>
       <c r="AG12" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
@@ -2867,7 +2879,7 @@
         <v>81</v>
       </c>
       <c r="AG13" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -2912,7 +2924,7 @@
         <v>82</v>
       </c>
       <c r="AG14" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
@@ -2955,7 +2967,7 @@
         <v>284</v>
       </c>
       <c r="AG15" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
@@ -2998,7 +3010,7 @@
         <v>83</v>
       </c>
       <c r="AG16" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
@@ -3043,7 +3055,7 @@
         <v>84</v>
       </c>
       <c r="AG17" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
@@ -3086,7 +3098,7 @@
         <v>285</v>
       </c>
       <c r="AG18" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
@@ -3129,7 +3141,7 @@
         <v>85</v>
       </c>
       <c r="AG19" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
@@ -3174,7 +3186,7 @@
         <v>86</v>
       </c>
       <c r="AG20" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
@@ -3219,7 +3231,7 @@
       <c r="AE21" s="6"/>
       <c r="AF21" s="7"/>
       <c r="AG21" s="8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
@@ -3262,7 +3274,7 @@
         <v>286</v>
       </c>
       <c r="AG22" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
@@ -3305,7 +3317,7 @@
         <v>87</v>
       </c>
       <c r="AG23" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
@@ -3350,7 +3362,7 @@
         <v>88</v>
       </c>
       <c r="AG24" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
@@ -3393,7 +3405,7 @@
         <v>287</v>
       </c>
       <c r="AG25" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.3">
@@ -3436,7 +3448,7 @@
         <v>89</v>
       </c>
       <c r="AG26" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.3">
@@ -3481,7 +3493,7 @@
         <v>90</v>
       </c>
       <c r="AG27" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.3">
@@ -3524,7 +3536,7 @@
         <v>288</v>
       </c>
       <c r="AG28" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.3">
@@ -3567,7 +3579,7 @@
         <v>91</v>
       </c>
       <c r="AG29" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.3">
@@ -3612,7 +3624,7 @@
         <v>92</v>
       </c>
       <c r="AG30" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.3">
@@ -3653,12 +3665,12 @@
       <c r="AE31" s="6"/>
       <c r="AF31" s="7"/>
       <c r="AG31" s="8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
@@ -3695,7 +3707,7 @@
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -4605,13 +4617,13 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C76" t="s">
         <v>322</v>
-      </c>
-      <c r="C76" t="s">
-        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setup for transition investigations
Timestep conversion is the main focus. If all transitions are given as
yearly values, how do we convert to quarterly or monthly values and
retain the same quality of results?
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -1036,9 +1036,6 @@
     <t>Denominator</t>
   </si>
   <si>
-    <t>People Alive</t>
-  </si>
-  <si>
     <t>Latent Prevalence (%)</t>
   </si>
   <si>
@@ -1064,6 +1061,9 @@
   </si>
   <si>
     <t>(0,0)</t>
+  </si>
+  <si>
+    <t>Population Count</t>
   </si>
 </sst>
 </file>
@@ -1577,7 +1577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -1600,10 +1600,10 @@
         <v>197</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,7 +1933,7 @@
         <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1944,7 +1944,7 @@
         <v>318</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>323</v>
@@ -1978,7 +1978,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2013,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>338</v>
@@ -2146,7 +2146,7 @@
         <v>333</v>
       </c>
       <c r="B6" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -2169,7 +2169,7 @@
         <v>334</v>
       </c>
       <c r="B7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>323</v>
@@ -2186,7 +2186,7 @@
         <v>336</v>
       </c>
       <c r="B8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>323</v>
@@ -2203,7 +2203,7 @@
         <v>337</v>
       </c>
       <c r="B9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>323</v>
@@ -2220,7 +2220,7 @@
         <v>335</v>
       </c>
       <c r="B10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>323</v>
@@ -3751,8 +3751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3799,7 +3799,7 @@
         <v>96</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3824,7 +3824,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3849,7 +3849,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3984,7 +3984,7 @@
         <v>240</v>
       </c>
       <c r="D19" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -4086,7 +4086,7 @@
         <v>113</v>
       </c>
       <c r="D28" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -4122,7 +4122,7 @@
         <v>271</v>
       </c>
       <c r="D31" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -4136,7 +4136,7 @@
         <v>114</v>
       </c>
       <c r="D32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -4161,7 +4161,7 @@
         <v>120</v>
       </c>
       <c r="D34" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Created epidemic characteristics databook page
Any epidemic characteristics defined in the cascade workbook (e.g.
cascade.xlsx) now have data entry blocks printed out for them in the
country databook (e.g. standard-test-data.xlsx).
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -1036,18 +1036,6 @@
     <t>Denominator</t>
   </si>
   <si>
-    <t>Latent Prevalence (%)</t>
-  </si>
-  <si>
-    <t>Smear Positive Prevalence (%)</t>
-  </si>
-  <si>
-    <t>Smear Negative Prevalence (%)</t>
-  </si>
-  <si>
-    <t>Active Prevalence (%)</t>
-  </si>
-  <si>
     <t>Dead Tag</t>
   </si>
   <si>
@@ -1064,6 +1052,18 @@
   </si>
   <si>
     <t>Population Count</t>
+  </si>
+  <si>
+    <t>Latent Prevalence</t>
+  </si>
+  <si>
+    <t>Smear Positive Prevalence</t>
+  </si>
+  <si>
+    <t>Smear Negative Prevalence</t>
+  </si>
+  <si>
+    <t>Active Prevalence</t>
   </si>
 </sst>
 </file>
@@ -1600,10 +1600,10 @@
         <v>197</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,7 +1933,7 @@
         <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1944,7 +1944,7 @@
         <v>318</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>323</v>
@@ -1977,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2013,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>338</v>
@@ -2146,7 +2146,7 @@
         <v>333</v>
       </c>
       <c r="B6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -2169,7 +2169,7 @@
         <v>334</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>323</v>
@@ -2186,7 +2186,7 @@
         <v>336</v>
       </c>
       <c r="B8" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>323</v>
@@ -2203,7 +2203,7 @@
         <v>337</v>
       </c>
       <c r="B9" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>323</v>
@@ -2220,7 +2220,7 @@
         <v>335</v>
       </c>
       <c r="B10" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>323</v>
@@ -3751,7 +3751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Characteristics are now ordered in databook
Column 'Databook Order' in cascade characteristics sheet allows
data-entry for population/prevalence/etc. to be ordered in the project
databooks as desired.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="350">
   <si>
     <t>Code Label</t>
   </si>
@@ -1064,6 +1064,9 @@
   </si>
   <si>
     <t>Active Prevalence</t>
+  </si>
+  <si>
+    <t>Databook Order</t>
   </si>
 </sst>
 </file>
@@ -1577,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -1975,37 +1978,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2013,224 +2018,251 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>329</v>
       </c>
       <c r="B2" t="s">
         <v>324</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>207</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>209</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>331</v>
       </c>
       <c r="B3" t="s">
         <v>327</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>211</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>213</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>215</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>332</v>
       </c>
       <c r="B4" t="s">
         <v>328</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>217</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>219</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>29</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>30</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>221</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>330</v>
       </c>
       <c r="B5" t="s">
         <v>326</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>331</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>333</v>
       </c>
       <c r="B6" t="s">
         <v>344</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="G6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>329</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>334</v>
       </c>
       <c r="B7" t="s">
         <v>345</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>333</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>336</v>
       </c>
       <c r="B8" t="s">
         <v>346</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>333</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>337</v>
       </c>
       <c r="B9" t="s">
         <v>347</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>333</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>335</v>
       </c>
       <c r="B10" t="s">
         <v>348</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>333</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>330</v>
       </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L12" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3752,7 +3784,7 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Characteristics propagated to parset
ParameterSet.pars is now subdivided into 'cascade' parameters and
'characs' parameters, the latter of which contains pop sizes and
prevalences.
Model even currently interpolates pop size to the start year and uses
that value as the starting susceptibles value.
Note: Collection compartments are currently not being counted as part of
standard cascade characteristics, despite having people in them. This
will be dealt with soon when collection compartments propagate
immediately...
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="353">
   <si>
     <t>Code Label</t>
   </si>
@@ -1699,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
@@ -2119,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2151,7 +2151,7 @@
     <col min="26" max="26" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -2182,28 +2182,25 @@
         <v>268</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>168</v>
       </c>
       <c r="I2" t="s">
-        <v>168</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>170</v>
       </c>
       <c r="L2" t="s">
-        <v>170</v>
-      </c>
-      <c r="M2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>275</v>
       </c>
@@ -2211,37 +2208,34 @@
         <v>271</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="I3" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>174</v>
       </c>
       <c r="L3" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N3" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="O3" t="s">
-        <v>176</v>
-      </c>
-      <c r="P3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -2249,37 +2243,34 @@
         <v>272</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>178</v>
       </c>
       <c r="I4" t="s">
-        <v>178</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>180</v>
       </c>
       <c r="L4" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N4" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="O4" t="s">
-        <v>182</v>
-      </c>
-      <c r="P4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>274</v>
       </c>
@@ -2293,7 +2284,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>277</v>
       </c>
@@ -2325,7 +2316,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>278</v>
       </c>
@@ -2345,7 +2336,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>280</v>
       </c>
@@ -2365,7 +2356,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>281</v>
       </c>
@@ -2385,7 +2376,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -2405,7 +2396,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L12" s="15"/>
     </row>
   </sheetData>
@@ -4070,7 +4061,7 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4123,6 +4114,9 @@
       <c r="C3" t="s">
         <v>77</v>
       </c>
+      <c r="D3" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
@@ -4165,6 +4159,9 @@
       <c r="C6" t="s">
         <v>322</v>
       </c>
+      <c r="D6" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
@@ -4179,6 +4176,9 @@
       <c r="C7" t="s">
         <v>79</v>
       </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -4279,7 +4279,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>317</v>
       </c>
@@ -4289,8 +4289,11 @@
       <c r="C17" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>318</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>319</v>
       </c>
@@ -4312,7 +4315,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>320</v>
       </c>
@@ -4323,7 +4326,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>327</v>
       </c>
@@ -4333,8 +4336,11 @@
       <c r="C21" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>328</v>
       </c>
@@ -4345,7 +4351,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -4355,8 +4361,11 @@
       <c r="C23" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -4367,7 +4376,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -4378,7 +4387,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>222</v>
       </c>
@@ -4388,8 +4397,11 @@
       <c r="C26" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>125</v>
       </c>
@@ -4399,8 +4411,11 @@
       <c r="C27" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>126</v>
       </c>
@@ -4411,7 +4426,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>131</v>
       </c>
@@ -4421,8 +4436,11 @@
       <c r="C29" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>342</v>
       </c>
@@ -4433,7 +4451,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>223</v>
       </c>
@@ -4444,7 +4462,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Upgraded recursive characteristics validation
Rather than relying on definition order to mean something for
characteristic entry-points (especially considering that this order is
already restricted, with earlier characteristics unable to include later
characteristics), an alternate form of validation has been developed.
If a characteristic 'includes' the entry-point of another characteristic
and that characteristic includes the entry-point of the original (or
some more complex cyclical reference), the program throws a
recursion-limit exception.
This enforces a valid ordering when calculating initial values.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="354">
   <si>
     <t>Code Label</t>
   </si>
@@ -2125,7 +2125,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2270,9 +2270,6 @@
       <c r="D4" s="2">
         <v>300000</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="H4" t="s">
         <v>7</v>
       </c>
@@ -2314,9 +2311,6 @@
       <c r="D5" s="2">
         <v>600000</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>351</v>
-      </c>
       <c r="H5" t="s">
         <v>351</v>
       </c>
@@ -2419,10 +2413,13 @@
         <v>2</v>
       </c>
       <c r="D9" s="2">
-        <v>0.3</v>
+        <v>300000</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>267</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="G9" t="s">
         <v>277</v>

</xml_diff>

<commit_message>
Initialisation with specified characteristics complete
Normalised characteristics (e.g. prevalence) can now be used to seed a
model, provided that the denominator (e.g. number of living people) is
also used to seed the model.
Run test.py with this commit to see default values for living-people,
active infections, latent infections and smear negative prevalence
(clearly interdependent) converted into appropriate initial values for a
model run.
Muck around with the 'Cascade Characteristics' sheet of cascade.xlsx to
either propagate alternative combinations or trigger numerous
settings.py validation checks.
On that point, it is not obvious to a user what is allowed/disallowed in
defining custom characteristics, so documentation will be required
eventually for devs.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -2125,7 +2125,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2226,9 +2226,6 @@
       <c r="D3" s="2">
         <v>250000</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="H3" t="s">
         <v>6</v>
       </c>
@@ -2311,6 +2308,9 @@
       <c r="D5" s="2">
         <v>600000</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>351</v>
+      </c>
       <c r="H5" t="s">
         <v>351</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="2">
-        <v>300000</v>
+        <v>0.3</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>267</v>

</xml_diff>

<commit_message>
Enabled hiding characteristics in databook
The 'Databook Order' column for both 'Cascade Characteristics' and
'Transition Parameters' now treats negative values as a tag to not print
out a data-entry block for the corresponding characteristic/parameter.
This will crash for a characteristic with an entry point, given that the
model cannot be initialised without values inserted in a databook. But
normal characteristics are nothing more than calculated outputs, so this
is not a problem for those.
Negative order is less advised for parameters as they are all used to
drive the model, but parameters missing from the databook are still
fine. They will simply be filled with relevant defaults or set to zero.
Note: Changes to a wide variety of files in this commit are cosmetic and
to do with OptimaException printouts.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
-    <sheet name="Cascade Characteristics" sheetId="4" r:id="rId2"/>
-    <sheet name="Transitions" sheetId="2" r:id="rId3"/>
-    <sheet name="Transition Parameters" sheetId="3" r:id="rId4"/>
+    <sheet name="Databook Sheet Names" sheetId="5" r:id="rId2"/>
+    <sheet name="Cascade Characteristics" sheetId="4" r:id="rId3"/>
+    <sheet name="Transitions" sheetId="2" r:id="rId4"/>
+    <sheet name="Transition Parameters" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="357">
   <si>
     <t>Code Label</t>
   </si>
@@ -1082,6 +1083,12 @@
   </si>
   <si>
     <t>s-x_prop</t>
+  </si>
+  <si>
+    <t>Sheet Label</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
   </si>
 </sst>
 </file>
@@ -1705,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2141,10 +2148,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2207,11 +2242,11 @@
       <c r="B2" t="s">
         <v>252</v>
       </c>
+      <c r="C2" s="2">
+        <v>-1</v>
+      </c>
       <c r="D2" s="2">
         <v>100000</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -2242,11 +2277,11 @@
       <c r="B3" t="s">
         <v>255</v>
       </c>
+      <c r="C3" s="2">
+        <v>-1</v>
+      </c>
       <c r="D3" s="2">
         <v>250000</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -2286,11 +2321,11 @@
       <c r="B4" t="s">
         <v>256</v>
       </c>
+      <c r="C4" s="2">
+        <v>-1</v>
+      </c>
       <c r="D4" s="2">
         <v>300000</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="H4" t="s">
         <v>7</v>
@@ -2330,6 +2365,9 @@
       <c r="B5" t="s">
         <v>254</v>
       </c>
+      <c r="C5" s="2">
+        <v>-1</v>
+      </c>
       <c r="D5" s="2">
         <v>600000</v>
       </c>
@@ -2385,14 +2423,14 @@
       <c r="B7" t="s">
         <v>273</v>
       </c>
-      <c r="C7" s="2">
-        <v>2</v>
-      </c>
       <c r="D7" s="2">
         <v>0.1</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>251</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="G7" t="s">
         <v>261</v>
@@ -2408,14 +2446,14 @@
       <c r="B8" t="s">
         <v>274</v>
       </c>
-      <c r="C8" s="2">
-        <v>2</v>
-      </c>
       <c r="D8" s="2">
         <v>0.2</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>251</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="G8" t="s">
         <v>261</v>
@@ -2431,14 +2469,14 @@
       <c r="B9" t="s">
         <v>275</v>
       </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
       <c r="D9" s="2">
         <v>0.3</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>251</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="G9" t="s">
         <v>261</v>
@@ -2455,7 +2493,7 @@
         <v>276</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D10" s="2">
         <v>0.6</v>
@@ -2479,7 +2517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI35"/>
   <sheetViews>
@@ -4130,12 +4168,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Definition of custom databook sheet names allowed
Cascade workbook (i.e. cascade.xlsx) can now have an optional worksheet
named 'Databook Sheet Names'. If it exists, custom sheet labels and
names will be stored via Settings.databook['custom_sheet_names'][label]
= name.
All characteristics and parameters will store 'charac' and 'linkpars',
respectively, as standard sheet names in their specs structures.
However, also-optional 'Sheet Label' columns in their respective
cascade.xlsx sheets can tag characteristics/parameters with the new
dev-defined custom sheet labels.
The next commit should implement this functionality in databook.py.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="359">
   <si>
     <t>Code Label</t>
   </si>
@@ -1089,6 +1089,12 @@
   </si>
   <si>
     <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>sh_test</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -2148,24 +2154,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -2176,40 +2190,41 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2217,299 +2232,305 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>257</v>
       </c>
       <c r="B2" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>-1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>100000</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>152</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>154</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>259</v>
       </c>
       <c r="B3" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>-1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>250000</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>156</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>14</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>158</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>160</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>260</v>
       </c>
       <c r="B4" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>-1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>300000</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>162</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>164</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>21</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>22</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>166</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>258</v>
       </c>
       <c r="B5" t="s">
         <v>254</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>-1</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>600000</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>327</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>259</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>261</v>
       </c>
       <c r="B6" t="s">
         <v>272</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>1000000</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>2</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>3</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>326</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>328</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>257</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>262</v>
       </c>
       <c r="B7" t="s">
         <v>273</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>0.1</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>261</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>264</v>
       </c>
       <c r="B8" t="s">
         <v>274</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>0.2</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>261</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>265</v>
       </c>
       <c r="B9" t="s">
         <v>275</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>0.3</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>261</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>263</v>
       </c>
       <c r="B10" t="s">
         <v>276</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>-1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>0.6</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>261</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="M12" s="15"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N12" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4170,10 +4191,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4182,10 +4203,11 @@
     <col min="2" max="2" width="4" customWidth="1"/>
     <col min="3" max="3" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4199,10 +4221,13 @@
         <v>151</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -4212,11 +4237,11 @@
       <c r="C2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -4229,11 +4254,11 @@
       <c r="D3" s="2">
         <v>0.5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -4243,11 +4268,11 @@
       <c r="C4" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>302</v>
       </c>
@@ -4257,11 +4282,14 @@
       <c r="C5" t="s">
         <v>300</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>303</v>
       </c>
@@ -4274,11 +4302,11 @@
       <c r="D6" s="2">
         <v>0.5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>335</v>
       </c>
@@ -4292,7 +4320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>336</v>
       </c>
@@ -4303,7 +4331,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>192</v>
       </c>
@@ -4314,7 +4342,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -4325,7 +4353,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -4336,7 +4364,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -4347,7 +4375,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>193</v>
       </c>
@@ -4358,7 +4386,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -4369,7 +4397,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -4380,7 +4408,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Parameters/Characteristics written to custom sheets
The order of the concatenated parameter/characteristic odicts is not
being preserved, so this will need to be fixed.
However, data entry blocks for parameters/characteristics are being
written to databook sheets of choice.
If all parameters/characteristics are customised (or not printed to the
databook at all), there is no need for the standard sheets and they are
excluded.
Next up, loading...
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="361">
   <si>
     <t>Code Label</t>
   </si>
@@ -1091,10 +1091,16 @@
     <t>Sheet Name</t>
   </si>
   <si>
-    <t>sh_test</t>
-  </si>
-  <si>
-    <t>Test</t>
+    <t>sh_pop</t>
+  </si>
+  <si>
+    <t>sh_prev</t>
+  </si>
+  <si>
+    <t>Prevalence</t>
+  </si>
+  <si>
+    <t>Population Size</t>
   </si>
 </sst>
 </file>
@@ -2154,16 +2160,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -2179,7 +2185,15 @@
         <v>357</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>358</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -2192,7 +2206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2410,7 +2424,7 @@
         <v>357</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
         <v>1000000</v>
@@ -2444,6 +2458,9 @@
       <c r="B7" t="s">
         <v>273</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="E7" s="2">
         <v>0.1</v>
       </c>
@@ -2467,6 +2484,9 @@
       <c r="B8" t="s">
         <v>274</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="E8" s="2">
         <v>0.2</v>
       </c>
@@ -2489,6 +2509,9 @@
       </c>
       <c r="B9" t="s">
         <v>275</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>358</v>
       </c>
       <c r="E9" s="2">
         <v>0.3</v>
@@ -4193,8 +4216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4237,6 +4260,9 @@
       <c r="C2" t="s">
         <v>76</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
@@ -4268,6 +4294,9 @@
       <c r="C4" t="s">
         <v>78</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
@@ -4302,6 +4331,9 @@
       <c r="D6" s="2">
         <v>0.5</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
@@ -4319,6 +4351,9 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -4330,6 +4365,9 @@
       <c r="C8" t="s">
         <v>343</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -4341,6 +4379,9 @@
       <c r="C9" t="s">
         <v>178</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -4352,6 +4393,9 @@
       <c r="C10" t="s">
         <v>79</v>
       </c>
+      <c r="E10" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -4363,6 +4407,9 @@
       <c r="C11" t="s">
         <v>80</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -4374,6 +4421,9 @@
       <c r="C12" t="s">
         <v>83</v>
       </c>
+      <c r="E12" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -4385,6 +4435,9 @@
       <c r="C13" t="s">
         <v>179</v>
       </c>
+      <c r="E13" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -4396,6 +4449,9 @@
       <c r="C14" t="s">
         <v>81</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -4407,6 +4463,9 @@
       <c r="C15" t="s">
         <v>82</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -4418,8 +4477,11 @@
       <c r="C16" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>296</v>
       </c>
@@ -4432,8 +4494,11 @@
       <c r="D17" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>297</v>
       </c>
@@ -4443,8 +4508,11 @@
       <c r="C18" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>298</v>
       </c>
@@ -4454,8 +4522,11 @@
       <c r="C19" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>299</v>
       </c>
@@ -4465,8 +4536,11 @@
       <c r="C20" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>337</v>
       </c>
@@ -4479,8 +4553,11 @@
       <c r="D21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>338</v>
       </c>
@@ -4490,8 +4567,11 @@
       <c r="C22" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>339</v>
       </c>
@@ -4504,8 +4584,11 @@
       <c r="D23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>340</v>
       </c>
@@ -4515,8 +4598,11 @@
       <c r="C24" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>341</v>
       </c>
@@ -4526,8 +4612,11 @@
       <c r="C25" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>206</v>
       </c>
@@ -4540,8 +4629,11 @@
       <c r="D26" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>112</v>
       </c>
@@ -4554,8 +4646,11 @@
       <c r="D27" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -4565,8 +4660,11 @@
       <c r="C28" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>118</v>
       </c>
@@ -4579,8 +4677,11 @@
       <c r="D29" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>317</v>
       </c>
@@ -4590,8 +4691,11 @@
       <c r="C30" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>207</v>
       </c>
@@ -4601,8 +4705,11 @@
       <c r="C31" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -4612,8 +4719,11 @@
       <c r="C32" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -4623,8 +4733,11 @@
       <c r="C33" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E33" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -4634,8 +4747,11 @@
       <c r="C34" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E34" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>318</v>
       </c>
@@ -4645,8 +4761,11 @@
       <c r="C35" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>208</v>
       </c>
@@ -4656,8 +4775,11 @@
       <c r="C36" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>116</v>
       </c>
@@ -4667,8 +4789,11 @@
       <c r="C37" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -4678,8 +4803,11 @@
       <c r="C38" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -4689,8 +4817,11 @@
       <c r="C39" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -4700,8 +4831,11 @@
       <c r="C40" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -4711,8 +4845,11 @@
       <c r="C41" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E41" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -4722,8 +4859,11 @@
       <c r="C42" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E42" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>123</v>
       </c>
@@ -4733,8 +4873,11 @@
       <c r="C43" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E43" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>187</v>
       </c>
@@ -4744,8 +4887,11 @@
       <c r="C44" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E44" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -4755,8 +4901,11 @@
       <c r="C45" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E45" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -4766,8 +4915,11 @@
       <c r="C46" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E46" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>188</v>
       </c>
@@ -4777,8 +4929,11 @@
       <c r="C47" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E47" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>126</v>
       </c>
@@ -4788,8 +4943,11 @@
       <c r="C48" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>352</v>
       </c>
@@ -4802,8 +4960,11 @@
       <c r="D49" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>353</v>
       </c>
@@ -4816,8 +4977,11 @@
       <c r="D50" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>354</v>
       </c>
@@ -4830,8 +4994,11 @@
       <c r="D51" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -4841,8 +5008,11 @@
       <c r="C52" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>127</v>
       </c>
@@ -4852,8 +5022,11 @@
       <c r="C53" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>128</v>
       </c>
@@ -4863,8 +5036,11 @@
       <c r="C54" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>133</v>
       </c>
@@ -4874,8 +5050,11 @@
       <c r="C55" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>320</v>
       </c>
@@ -4885,8 +5064,11 @@
       <c r="C56" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>210</v>
       </c>
@@ -4896,8 +5078,11 @@
       <c r="C57" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>129</v>
       </c>
@@ -4907,8 +5092,11 @@
       <c r="C58" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>130</v>
       </c>
@@ -4918,8 +5106,11 @@
       <c r="C59" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>134</v>
       </c>
@@ -4929,8 +5120,11 @@
       <c r="C60" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>322</v>
       </c>
@@ -4940,8 +5134,11 @@
       <c r="C61" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>211</v>
       </c>
@@ -4951,8 +5148,11 @@
       <c r="C62" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>131</v>
       </c>
@@ -4962,8 +5162,11 @@
       <c r="C63" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>132</v>
       </c>
@@ -4973,8 +5176,11 @@
       <c r="C64" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E64" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>135</v>
       </c>
@@ -4984,8 +5190,11 @@
       <c r="C65" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E65" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>136</v>
       </c>
@@ -4995,8 +5204,11 @@
       <c r="C66" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E66" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>189</v>
       </c>
@@ -5006,8 +5218,11 @@
       <c r="C67" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E67" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>137</v>
       </c>
@@ -5017,8 +5232,11 @@
       <c r="C68" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E68" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -5028,8 +5246,11 @@
       <c r="C69" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E69" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>190</v>
       </c>
@@ -5039,8 +5260,11 @@
       <c r="C70" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E70" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>139</v>
       </c>
@@ -5050,8 +5274,11 @@
       <c r="C71" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E71" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -5061,8 +5288,11 @@
       <c r="C72" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E72" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -5072,8 +5302,11 @@
       <c r="C73" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E73" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>141</v>
       </c>
@@ -5083,8 +5316,11 @@
       <c r="C74" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E74" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>250</v>
       </c>
@@ -5094,17 +5330,20 @@
       <c r="C75" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E75" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B79" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Standard-cascade example of sheet customisation
Run test.py and then check out standard-test-data.xlsx, as produced from
cascade.xlsx.
This example should split characteristics between a 'Population Sizes'
and 'Prevalence' page, while several death and infection cascade
parameters have been pulled to their own 'Mortality Rates' and
'Infection Rates' sheets.
Nothing appears to have changed the test model dynamics, so this feature
appears to be operating correctly, although testing that current
validation catches all common issues is of course advised.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="365">
   <si>
     <t>Code Label</t>
   </si>
@@ -1100,7 +1100,19 @@
     <t>Prevalence</t>
   </si>
   <si>
-    <t>Population Size</t>
+    <t>sh_death</t>
+  </si>
+  <si>
+    <t>Mortality Rates</t>
+  </si>
+  <si>
+    <t>sh_inf</t>
+  </si>
+  <si>
+    <t>Infection Rates</t>
+  </si>
+  <si>
+    <t>Population Sizes</t>
   </si>
 </sst>
 </file>
@@ -2160,10 +2172,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2185,7 +2197,7 @@
         <v>357</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2194,6 +2206,22 @@
       </c>
       <c r="B3" s="2" t="s">
         <v>359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -4216,8 +4244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4260,9 +4288,6 @@
       <c r="C2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>357</v>
-      </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
@@ -4280,6 +4305,9 @@
       <c r="D3" s="2">
         <v>0.5</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
@@ -4295,7 +4323,7 @@
         <v>78</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -4312,7 +4340,7 @@
         <v>300</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -4332,7 +4360,7 @@
         <v>0.5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -4351,9 +4379,6 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -4365,9 +4390,6 @@
       <c r="C8" t="s">
         <v>343</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -4379,9 +4401,6 @@
       <c r="C9" t="s">
         <v>178</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -4393,9 +4412,6 @@
       <c r="C10" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -4407,9 +4423,6 @@
       <c r="C11" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -4421,9 +4434,6 @@
       <c r="C12" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -4435,9 +4445,6 @@
       <c r="C13" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -4449,9 +4456,6 @@
       <c r="C14" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -4463,9 +4467,6 @@
       <c r="C15" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -4477,11 +4478,8 @@
       <c r="C16" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>296</v>
       </c>
@@ -4494,11 +4492,8 @@
       <c r="D17" s="2">
         <v>0.5</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>297</v>
       </c>
@@ -4508,11 +4503,8 @@
       <c r="C18" t="s">
         <v>293</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>298</v>
       </c>
@@ -4522,11 +4514,8 @@
       <c r="C19" t="s">
         <v>294</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>299</v>
       </c>
@@ -4536,11 +4525,8 @@
       <c r="C20" t="s">
         <v>295</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>337</v>
       </c>
@@ -4553,11 +4539,8 @@
       <c r="D21" s="2">
         <v>1</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>338</v>
       </c>
@@ -4567,11 +4550,8 @@
       <c r="C22" t="s">
         <v>346</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>339</v>
       </c>
@@ -4584,11 +4564,8 @@
       <c r="D23" s="2">
         <v>1</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>340</v>
       </c>
@@ -4598,11 +4575,8 @@
       <c r="C24" t="s">
         <v>347</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>341</v>
       </c>
@@ -4612,11 +4586,8 @@
       <c r="C25" t="s">
         <v>348</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>206</v>
       </c>
@@ -4629,11 +4600,8 @@
       <c r="D26" s="2">
         <v>0.5</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>112</v>
       </c>
@@ -4646,11 +4614,8 @@
       <c r="D27" s="2">
         <v>0.5</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -4660,11 +4625,8 @@
       <c r="C28" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>118</v>
       </c>
@@ -4677,11 +4639,8 @@
       <c r="D29" s="2">
         <v>0.5</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>317</v>
       </c>
@@ -4691,11 +4650,8 @@
       <c r="C30" t="s">
         <v>316</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>207</v>
       </c>
@@ -4705,11 +4661,8 @@
       <c r="C31" t="s">
         <v>201</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -4718,9 +4671,6 @@
       </c>
       <c r="C32" t="s">
         <v>87</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -4733,9 +4683,6 @@
       <c r="C33" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -4747,9 +4694,6 @@
       <c r="C34" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
@@ -4761,9 +4705,6 @@
       <c r="C35" t="s">
         <v>319</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -4775,9 +4716,6 @@
       <c r="C36" t="s">
         <v>202</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -4789,9 +4727,6 @@
       <c r="C37" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -4803,9 +4738,6 @@
       <c r="C38" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -4817,9 +4749,6 @@
       <c r="C39" t="s">
         <v>93</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -4832,7 +4761,7 @@
         <v>218</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -4846,7 +4775,7 @@
         <v>180</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -4860,7 +4789,7 @@
         <v>306</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -4874,7 +4803,7 @@
         <v>219</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -4888,7 +4817,7 @@
         <v>181</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -4902,7 +4831,7 @@
         <v>307</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -4916,7 +4845,7 @@
         <v>220</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -4930,7 +4859,7 @@
         <v>182</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -4944,10 +4873,10 @@
         <v>308</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>352</v>
       </c>
@@ -4960,11 +4889,8 @@
       <c r="D49" s="2">
         <v>3</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>353</v>
       </c>
@@ -4977,11 +4903,8 @@
       <c r="D50" s="2">
         <v>2</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>354</v>
       </c>
@@ -4994,11 +4917,8 @@
       <c r="D51" s="2">
         <v>1</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -5008,11 +4928,8 @@
       <c r="C52" t="s">
         <v>203</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>127</v>
       </c>
@@ -5022,11 +4939,8 @@
       <c r="C53" t="s">
         <v>94</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>128</v>
       </c>
@@ -5036,11 +4950,8 @@
       <c r="C54" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>133</v>
       </c>
@@ -5050,11 +4961,8 @@
       <c r="C55" t="s">
         <v>100</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>320</v>
       </c>
@@ -5064,11 +4972,8 @@
       <c r="C56" t="s">
         <v>321</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>210</v>
       </c>
@@ -5078,11 +4983,8 @@
       <c r="C57" t="s">
         <v>204</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>129</v>
       </c>
@@ -5092,11 +4994,8 @@
       <c r="C58" t="s">
         <v>96</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>130</v>
       </c>
@@ -5106,11 +5005,8 @@
       <c r="C59" t="s">
         <v>97</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>134</v>
       </c>
@@ -5120,11 +5016,8 @@
       <c r="C60" t="s">
         <v>101</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>322</v>
       </c>
@@ -5134,11 +5027,8 @@
       <c r="C61" t="s">
         <v>323</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>211</v>
       </c>
@@ -5148,11 +5038,8 @@
       <c r="C62" t="s">
         <v>205</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>131</v>
       </c>
@@ -5162,11 +5049,8 @@
       <c r="C63" t="s">
         <v>98</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>132</v>
       </c>
@@ -5176,11 +5060,8 @@
       <c r="C64" t="s">
         <v>99</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>135</v>
       </c>
@@ -5190,11 +5071,8 @@
       <c r="C65" t="s">
         <v>102</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>136</v>
       </c>
@@ -5205,10 +5083,10 @@
         <v>221</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>189</v>
       </c>
@@ -5219,10 +5097,10 @@
         <v>183</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>137</v>
       </c>
@@ -5233,10 +5111,10 @@
         <v>309</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -5247,10 +5125,10 @@
         <v>222</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>190</v>
       </c>
@@ -5261,10 +5139,10 @@
         <v>184</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>139</v>
       </c>
@@ -5275,10 +5153,10 @@
         <v>310</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -5289,10 +5167,10 @@
         <v>223</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -5303,10 +5181,10 @@
         <v>185</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>141</v>
       </c>
@@ -5317,10 +5195,10 @@
         <v>311</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>250</v>
       </c>
@@ -5331,19 +5209,22 @@
         <v>278</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+      <c r="F75" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B79" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated cascade for infectious prevalences
Infection rates are dependent on six prevalences, corresponding to the
coupled undiagnosed and diagnosed compartments of the six smear-strain
combinations.
It is assumed people on treatment are not infectious, in some cases due
to inherent quarantine for virulent strains, but this can be amended
later.
Characteristics have thus been refined to prepare for these
dependencies.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="391">
   <si>
     <t>Code Label</t>
   </si>
@@ -275,60 +275,6 @@
     <t>Fast-LTBI Treatment Success Rate</t>
   </si>
   <si>
-    <t>SPos DS Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SPos DS Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SPos MDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SPos MDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SPos XDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SPos XDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SPos DS Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SPos MDR Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SPos XDR Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SNeg DS Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SNeg DS Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SNeg MDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SNeg MDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SNeg XDR Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>SNeg XDR Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>SNeg DS Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SNeg MDR Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>SNeg XDR Treatment Success Rate</t>
-  </si>
-  <si>
     <t>v_rate</t>
   </si>
   <si>
@@ -560,24 +506,6 @@
     <t>Fast-LTBI Diagnosis Rate</t>
   </si>
   <si>
-    <t>SPos DS Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SPos MDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SPos XDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg DS Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg MDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg XDR Death Rate (Diagnosed)</t>
-  </si>
-  <si>
     <t>s+ddd_rate</t>
   </si>
   <si>
@@ -620,24 +548,6 @@
     <t>ef</t>
   </si>
   <si>
-    <t>SPos DS Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SPos MDR Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SPos XDR Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SNeg DS Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SNeg MDR Diagnosis Rate</t>
-  </si>
-  <si>
-    <t>SNeg XDR Diagnosis Rate</t>
-  </si>
-  <si>
     <t>s+ddiag_rate</t>
   </si>
   <si>
@@ -674,24 +584,6 @@
     <t>ff</t>
   </si>
   <si>
-    <t>SPos DS Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SPos MDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SPos XDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg DS Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg MDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
-    <t>SNeg XDR Death Rate (Undiagnosed)</t>
-  </si>
-  <si>
     <t>(-12,1)</t>
   </si>
   <si>
@@ -785,12 +677,6 @@
     <t>Active Infections</t>
   </si>
   <si>
-    <t>Smear Positive Infections</t>
-  </si>
-  <si>
-    <t>Smear Negative Infections</t>
-  </si>
-  <si>
     <t>lt_inf</t>
   </si>
   <si>
@@ -842,12 +728,6 @@
     <t>Latent Prevalence</t>
   </si>
   <si>
-    <t>Smear Positive Prevalence</t>
-  </si>
-  <si>
-    <t>Smear Negative Prevalence</t>
-  </si>
-  <si>
     <t>Active Prevalence</t>
   </si>
   <si>
@@ -938,24 +818,6 @@
     <t>Successfully Treated (Latent)</t>
   </si>
   <si>
-    <t>SPos DS Death Rate (On-Treatment)</t>
-  </si>
-  <si>
-    <t>SPos MDR Death Rate (On-Treatment)</t>
-  </si>
-  <si>
-    <t>SPos XDR Death Rate (On-Treatment)</t>
-  </si>
-  <si>
-    <t>SNeg DS Death Rate (On-Treatment)</t>
-  </si>
-  <si>
-    <t>SNeg MDR Death Rate (On-Treatment)</t>
-  </si>
-  <si>
-    <t>SNeg XDR Death Rate (On-Treatment)</t>
-  </si>
-  <si>
     <t>gf</t>
   </si>
   <si>
@@ -968,30 +830,18 @@
     <t>gi</t>
   </si>
   <si>
-    <t>SPos DS-MDR Escalation Rate</t>
-  </si>
-  <si>
     <t>s+dbad_rate</t>
   </si>
   <si>
     <t>s+mbad_rate</t>
   </si>
   <si>
-    <t>SPos MDR-XDR Escalation Rate</t>
-  </si>
-  <si>
     <t>s-dbad_rate</t>
   </si>
   <si>
-    <t>SNeg DS-MDR Escalation Rate</t>
-  </si>
-  <si>
     <t>s-mbad_rate</t>
   </si>
   <si>
-    <t>SNeg MDR-XDR Escalation Rate</t>
-  </si>
-  <si>
     <t>(0,2)</t>
   </si>
   <si>
@@ -1052,30 +902,6 @@
     <t>Fast-LTBI Proportion of Latent Infections</t>
   </si>
   <si>
-    <t>DS Proportion of SPos Infections</t>
-  </si>
-  <si>
-    <t>SPos Proportion of Active Infections</t>
-  </si>
-  <si>
-    <t>SNeg Proportion of Active Infections</t>
-  </si>
-  <si>
-    <t>MDR Proportion of SPos Infections</t>
-  </si>
-  <si>
-    <t>XDR Proportion of SPos Infections</t>
-  </si>
-  <si>
-    <t>DS Proportion of SNeg Infections</t>
-  </si>
-  <si>
-    <t>MDR Proportion of SNeg Infections</t>
-  </si>
-  <si>
-    <t>XDR Proportion of SNeg Infections</t>
-  </si>
-  <si>
     <t>s-d_prop</t>
   </si>
   <si>
@@ -1113,6 +939,258 @@
   </si>
   <si>
     <t>Population Sizes</t>
+  </si>
+  <si>
+    <t>s+d_infx</t>
+  </si>
+  <si>
+    <t>s+m_infx</t>
+  </si>
+  <si>
+    <t>s+x_infx</t>
+  </si>
+  <si>
+    <t>s-d_infx</t>
+  </si>
+  <si>
+    <t>s-m_infx</t>
+  </si>
+  <si>
+    <t>s-x_infx</t>
+  </si>
+  <si>
+    <t>s+d_prevx</t>
+  </si>
+  <si>
+    <t>s+m_prevx</t>
+  </si>
+  <si>
+    <t>s+x_prevx</t>
+  </si>
+  <si>
+    <t>s-d_prevx</t>
+  </si>
+  <si>
+    <t>s-m_prevx</t>
+  </si>
+  <si>
+    <t>s-x_prevx</t>
+  </si>
+  <si>
+    <t>sh_disagg</t>
+  </si>
+  <si>
+    <t>TB Disaggregation</t>
+  </si>
+  <si>
+    <t>SP DS Infectious Count</t>
+  </si>
+  <si>
+    <t>SP MDR Infectious Count</t>
+  </si>
+  <si>
+    <t>SP XDR Infectious Count</t>
+  </si>
+  <si>
+    <t>SP DS Infectious Prevalence</t>
+  </si>
+  <si>
+    <t>SP MDR Infectious Prevalence</t>
+  </si>
+  <si>
+    <t>SP XDR Infectious Prevalence</t>
+  </si>
+  <si>
+    <t>SP Proportion of Active Infections</t>
+  </si>
+  <si>
+    <t>DS Proportion of SP Infections</t>
+  </si>
+  <si>
+    <t>MDR Proportion of SP Infections</t>
+  </si>
+  <si>
+    <t>XDR Proportion of SP Infections</t>
+  </si>
+  <si>
+    <t>SP DS Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SP DS Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SP DS Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SP DS Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SP DS-MDR Escalation Rate</t>
+  </si>
+  <si>
+    <t>SP MDR Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SP MDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SP MDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SP MDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SP MDR-XDR Escalation Rate</t>
+  </si>
+  <si>
+    <t>SP XDR Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SP XDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SP XDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SP XDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SP DS Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SP DS Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SP DS Death Rate (On-Treatment)</t>
+  </si>
+  <si>
+    <t>SP MDR Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SP MDR Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SP MDR Death Rate (On-Treatment)</t>
+  </si>
+  <si>
+    <t>SP XDR Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SP XDR Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SP XDR Death Rate (On-Treatment)</t>
+  </si>
+  <si>
+    <t>SN DS Infectious Count</t>
+  </si>
+  <si>
+    <t>SN MDR Infectious Count</t>
+  </si>
+  <si>
+    <t>SN XDR Infectious Count</t>
+  </si>
+  <si>
+    <t>SN DS Infectious Prevalence</t>
+  </si>
+  <si>
+    <t>SN MDR Infectious Prevalence</t>
+  </si>
+  <si>
+    <t>SN XDR Infectious Prevalence</t>
+  </si>
+  <si>
+    <t>SN Proportion of Active Infections</t>
+  </si>
+  <si>
+    <t>DS Proportion of SN Infections</t>
+  </si>
+  <si>
+    <t>MDR Proportion of SN Infections</t>
+  </si>
+  <si>
+    <t>XDR Proportion of SN Infections</t>
+  </si>
+  <si>
+    <t>SN DS Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SN DS Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SN DS Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SN DS Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SN DS-MDR Escalation Rate</t>
+  </si>
+  <si>
+    <t>SN MDR Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SN MDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SN MDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SN MDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SN MDR-XDR Escalation Rate</t>
+  </si>
+  <si>
+    <t>SN XDR Diagnosis Rate</t>
+  </si>
+  <si>
+    <t>SN XDR Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>SN XDR Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>SN XDR Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>SN DS Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SN DS Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SN DS Death Rate (On-Treatment)</t>
+  </si>
+  <si>
+    <t>SN MDR Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SN MDR Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SN MDR Death Rate (On-Treatment)</t>
+  </si>
+  <si>
+    <t>SN XDR Death Rate (Undiagnosed)</t>
+  </si>
+  <si>
+    <t>SN XDR Death Rate (Diagnosed)</t>
+  </si>
+  <si>
+    <t>SN XDR Death Rate (On-Treatment)</t>
+  </si>
+  <si>
+    <t>Smear-Positive Infections</t>
+  </si>
+  <si>
+    <t>Smear-Positive Prevalence</t>
+  </si>
+  <si>
+    <t>Smear-Negative Infections</t>
+  </si>
+  <si>
+    <t>Smear-Negative Prevalence</t>
   </si>
 </sst>
 </file>
@@ -1736,7 +1814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1757,16 +1835,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1777,7 +1855,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>244</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1788,7 +1866,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1796,13 +1874,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1810,21 +1888,21 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>238</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>239</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1832,10 +1910,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>279</v>
+        <v>239</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>236</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1843,21 +1921,21 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>240</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1865,35 +1943,35 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>237</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="B11" t="s">
-        <v>305</v>
+        <v>265</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
       <c r="B12" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1901,13 +1979,13 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>333</v>
+        <v>283</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1915,21 +1993,21 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1937,10 +2015,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>286</v>
+        <v>246</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1948,21 +2026,21 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>231</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1970,10 +2048,10 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>287</v>
+        <v>247</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1981,21 +2059,21 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>232</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2003,10 +2081,10 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>288</v>
+        <v>248</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2014,13 +2092,13 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>334</v>
+        <v>284</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2028,21 +2106,21 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2050,10 +2128,10 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2061,21 +2139,21 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,10 +2161,10 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>290</v>
+        <v>250</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2094,21 +2172,21 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>226</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2116,52 +2194,52 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>291</v>
+        <v>251</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>227</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="B33" t="s">
-        <v>304</v>
+        <v>264</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="B34" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="B35" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2172,56 +2250,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>355</v>
+        <v>297</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>356</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>357</v>
+        <v>299</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>364</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>358</v>
+        <v>300</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>359</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>362</v>
+        <v>304</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>361</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2232,10 +2318,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2248,13 +2334,7 @@
     <col min="6" max="6" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="8.77734375" customWidth="1"/>
     <col min="16" max="17" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.44140625" bestFit="1" customWidth="1"/>
@@ -2266,7 +2346,7 @@
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2274,40 +2354,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>355</v>
+        <v>297</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>277</v>
+        <v>237</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>329</v>
+        <v>279</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="D2" s="2">
         <v>-1</v>
       </c>
-      <c r="E2" s="2">
-        <v>100000</v>
-      </c>
       <c r="I2" t="s">
         <v>5</v>
       </c>
@@ -2315,7 +2392,7 @@
         <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="L2" t="s">
         <v>10</v>
@@ -2324,264 +2401,442 @@
         <v>9</v>
       </c>
       <c r="N2" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="O2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>307</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>321</v>
       </c>
       <c r="D3" s="2">
         <v>-1</v>
       </c>
-      <c r="E3" s="2">
-        <v>250000</v>
-      </c>
       <c r="I3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" t="s">
-        <v>156</v>
-      </c>
-      <c r="L3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" t="s">
-        <v>158</v>
-      </c>
-      <c r="O3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>160</v>
-      </c>
-      <c r="R3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>308</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
+        <v>322</v>
       </c>
       <c r="D4" s="2">
         <v>-1</v>
       </c>
-      <c r="E4" s="2">
-        <v>300000</v>
-      </c>
       <c r="I4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>162</v>
-      </c>
-      <c r="L4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" t="s">
-        <v>164</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>166</v>
-      </c>
-      <c r="R4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>323</v>
       </c>
       <c r="D5" s="2">
         <v>-1</v>
       </c>
-      <c r="E5" s="2">
-        <v>600000</v>
-      </c>
       <c r="I5" t="s">
-        <v>327</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>259</v>
-      </c>
-      <c r="K5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>261</v>
+        <v>310</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D6" s="2">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="I6" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" t="s">
-        <v>326</v>
-      </c>
-      <c r="L6" t="s">
-        <v>328</v>
-      </c>
-      <c r="M6" t="s">
-        <v>257</v>
-      </c>
-      <c r="N6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>262</v>
+        <v>311</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>261</v>
+        <v>355</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-1</v>
       </c>
       <c r="I7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
       <c r="B8" t="s">
-        <v>274</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G8" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" t="s">
+        <v>387</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I9" t="s">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
-        <v>261</v>
-      </c>
-      <c r="I8" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B9" t="s">
-        <v>275</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" t="s">
-        <v>261</v>
-      </c>
-      <c r="I9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>307</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>308</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" t="s">
+        <v>309</v>
+      </c>
+      <c r="O9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>263</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
-        <v>276</v>
+        <v>389</v>
       </c>
       <c r="D10" s="2">
         <v>-1</v>
       </c>
-      <c r="E10" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="H10" t="s">
-        <v>261</v>
-      </c>
       <c r="I10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="N12" s="15"/>
+        <v>7</v>
+      </c>
+      <c r="J10" t="s">
+        <v>310</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" t="s">
+        <v>311</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" t="s">
+        <v>312</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>277</v>
+      </c>
+      <c r="J11" t="s">
+        <v>221</v>
+      </c>
+      <c r="K11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>276</v>
+      </c>
+      <c r="L12" t="s">
+        <v>278</v>
+      </c>
+      <c r="M12" t="s">
+        <v>219</v>
+      </c>
+      <c r="N12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>223</v>
+      </c>
+      <c r="I13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" t="s">
+        <v>324</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H14" t="s">
+        <v>223</v>
+      </c>
+      <c r="I14" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B15" t="s">
+        <v>325</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H15" t="s">
+        <v>223</v>
+      </c>
+      <c r="I15" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B16" t="s">
+        <v>326</v>
+      </c>
+      <c r="D16" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H16" t="s">
+        <v>223</v>
+      </c>
+      <c r="I16" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>316</v>
+      </c>
+      <c r="B17" t="s">
+        <v>357</v>
+      </c>
+      <c r="D17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H17" t="s">
+        <v>223</v>
+      </c>
+      <c r="I17" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>317</v>
+      </c>
+      <c r="B18" t="s">
+        <v>358</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H18" t="s">
+        <v>223</v>
+      </c>
+      <c r="I18" t="s">
+        <v>311</v>
+      </c>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B19" t="s">
+        <v>359</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H19" t="s">
+        <v>223</v>
+      </c>
+      <c r="I19" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B20" t="s">
+        <v>388</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>223</v>
+      </c>
+      <c r="I20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" t="s">
+        <v>390</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>223</v>
+      </c>
+      <c r="I21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>225</v>
+      </c>
+      <c r="B22" t="s">
+        <v>236</v>
+      </c>
+      <c r="D22" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H22" t="s">
+        <v>223</v>
+      </c>
+      <c r="I22" t="s">
+        <v>220</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2617,7 +2872,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>10</v>
@@ -2626,16 +2881,16 @@
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="L1" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>6</v>
@@ -2644,7 +2899,7 @@
         <v>12</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>13</v>
@@ -2653,7 +2908,7 @@
         <v>14</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>15</v>
@@ -2662,7 +2917,7 @@
         <v>16</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>17</v>
@@ -2674,7 +2929,7 @@
         <v>18</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="Z1" s="5" t="s">
         <v>19</v>
@@ -2683,7 +2938,7 @@
         <v>20</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="AC1" s="5" t="s">
         <v>21</v>
@@ -2692,19 +2947,19 @@
         <v>22</v>
       </c>
       <c r="AE1" s="5" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="AF1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="AH1" s="4" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
@@ -2749,7 +3004,7 @@
       <c r="AG2" s="6"/>
       <c r="AH2" s="7"/>
       <c r="AI2" s="8" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
@@ -2792,7 +3047,7 @@
       <c r="AG3" s="9"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
@@ -2847,7 +3102,7 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -2880,12 +3135,12 @@
       <c r="AG5" s="9"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
@@ -2925,7 +3180,7 @@
       <c r="AG6" s="9"/>
       <c r="AH6" s="10"/>
       <c r="AI6" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
@@ -2944,7 +3199,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10" t="s">
-        <v>281</v>
+        <v>241</v>
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="9"/>
@@ -2970,7 +3225,7 @@
       <c r="AG7" s="9"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
@@ -2985,7 +3240,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -3015,12 +3270,12 @@
       <c r="AG8" s="9"/>
       <c r="AH8" s="10"/>
       <c r="AI8" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
@@ -3060,7 +3315,7 @@
       <c r="AG9" s="9"/>
       <c r="AH9" s="10"/>
       <c r="AI9" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
@@ -3079,7 +3334,7 @@
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10" t="s">
-        <v>282</v>
+        <v>242</v>
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="9"/>
@@ -3105,12 +3360,12 @@
       <c r="AG10" s="9"/>
       <c r="AH10" s="10"/>
       <c r="AI10" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
@@ -3123,7 +3378,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="17" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="10"/>
@@ -3148,12 +3403,12 @@
       <c r="AG11" s="9"/>
       <c r="AH11" s="10"/>
       <c r="AI11" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="20"/>
@@ -3167,7 +3422,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="21"/>
       <c r="M12" s="19" t="s">
-        <v>284</v>
+        <v>244</v>
       </c>
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
@@ -3179,7 +3434,7 @@
       <c r="U12" s="20"/>
       <c r="V12" s="22"/>
       <c r="W12" s="19" t="s">
-        <v>285</v>
+        <v>245</v>
       </c>
       <c r="X12" s="20"/>
       <c r="Y12" s="20"/>
@@ -3257,7 +3512,7 @@
       <c r="M14" s="9"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
@@ -3278,15 +3533,15 @@
       <c r="AF14" s="11"/>
       <c r="AG14" s="9"/>
       <c r="AH14" s="10" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="AI14" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
@@ -3326,7 +3581,7 @@
         <v>62</v>
       </c>
       <c r="AI15" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.3">
@@ -3352,7 +3607,7 @@
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10" t="s">
-        <v>312</v>
+        <v>266</v>
       </c>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
@@ -3375,7 +3630,7 @@
         <v>63</v>
       </c>
       <c r="AI16" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
@@ -3399,7 +3654,7 @@
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
@@ -3417,15 +3672,15 @@
       <c r="AF17" s="11"/>
       <c r="AG17" s="9"/>
       <c r="AH17" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AI17" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="AI17" s="11" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -3465,7 +3720,7 @@
         <v>64</v>
       </c>
       <c r="AI18" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
@@ -3494,7 +3749,7 @@
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
       <c r="U19" s="10" t="s">
-        <v>313</v>
+        <v>267</v>
       </c>
       <c r="V19" s="11"/>
       <c r="W19" s="9"/>
@@ -3514,7 +3769,7 @@
         <v>65</v>
       </c>
       <c r="AI19" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
@@ -3541,7 +3796,7 @@
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
       <c r="U20" s="10" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="V20" s="11"/>
       <c r="W20" s="9"/>
@@ -3556,15 +3811,15 @@
       <c r="AF20" s="11"/>
       <c r="AG20" s="9"/>
       <c r="AH20" s="10" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="AI20" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
@@ -3604,7 +3859,7 @@
         <v>66</v>
       </c>
       <c r="AI21" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.3">
@@ -3651,7 +3906,7 @@
         <v>67</v>
       </c>
       <c r="AI22" s="14" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
@@ -3727,7 +3982,7 @@
       <c r="W24" s="9"/>
       <c r="X24" s="10"/>
       <c r="Y24" s="10" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="Z24" s="10"/>
       <c r="AA24" s="10"/>
@@ -3738,15 +3993,15 @@
       <c r="AF24" s="11"/>
       <c r="AG24" s="9"/>
       <c r="AH24" s="10" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="AI24" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -3786,7 +4041,7 @@
         <v>68</v>
       </c>
       <c r="AI25" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.3">
@@ -3822,7 +4077,7 @@
       <c r="Z26" s="10"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="10" t="s">
-        <v>314</v>
+        <v>268</v>
       </c>
       <c r="AC26" s="10"/>
       <c r="AD26" s="10"/>
@@ -3835,7 +4090,7 @@
         <v>69</v>
       </c>
       <c r="AI26" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.3">
@@ -3869,7 +4124,7 @@
       <c r="Z27" s="10"/>
       <c r="AA27" s="10"/>
       <c r="AB27" s="10" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="AC27" s="10"/>
       <c r="AD27" s="10"/>
@@ -3877,15 +4132,15 @@
       <c r="AF27" s="11"/>
       <c r="AG27" s="9"/>
       <c r="AH27" s="10" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="AI27" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
@@ -3925,7 +4180,7 @@
         <v>70</v>
       </c>
       <c r="AI28" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.3">
@@ -3964,7 +4219,7 @@
       <c r="AC29" s="10"/>
       <c r="AD29" s="10"/>
       <c r="AE29" s="10" t="s">
-        <v>315</v>
+        <v>269</v>
       </c>
       <c r="AF29" s="11"/>
       <c r="AG29" s="9" t="s">
@@ -3974,7 +4229,7 @@
         <v>71</v>
       </c>
       <c r="AI29" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.3">
@@ -4011,20 +4266,20 @@
       <c r="AC30" s="10"/>
       <c r="AD30" s="10"/>
       <c r="AE30" s="10" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="AF30" s="11"/>
       <c r="AG30" s="9"/>
       <c r="AH30" s="10" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="AI30" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
@@ -4064,7 +4319,7 @@
         <v>72</v>
       </c>
       <c r="AI31" s="11" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
@@ -4111,12 +4366,12 @@
         <v>73</v>
       </c>
       <c r="AI32" s="14" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -4154,12 +4409,12 @@
       <c r="AG33" s="6"/>
       <c r="AH33" s="7"/>
       <c r="AI33" s="8" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
@@ -4198,7 +4453,7 @@
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="13"/>
@@ -4244,8 +4499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4269,18 +4524,18 @@
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>355</v>
+        <v>297</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>277</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>25</v>
@@ -4288,13 +4543,10 @@
       <c r="C2" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -4306,15 +4558,12 @@
         <v>0.5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
@@ -4323,88 +4572,85 @@
         <v>78</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>302</v>
+        <v>262</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>303</v>
+        <v>263</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>301</v>
+        <v>261</v>
       </c>
       <c r="D6" s="2">
         <v>0.5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>335</v>
+        <v>285</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>342</v>
+        <v>292</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>286</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>343</v>
+        <v>293</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>30</v>
@@ -4415,7 +4661,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>31</v>
@@ -4426,10 +4672,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>281</v>
+        <v>241</v>
       </c>
       <c r="C12" t="s">
         <v>83</v>
@@ -4437,18 +4683,18 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>32</v>
@@ -4459,7 +4705,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>33</v>
@@ -4470,746 +4716,770 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>282</v>
+        <v>242</v>
       </c>
       <c r="C16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>296</v>
+        <v>256</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>292</v>
+        <v>252</v>
       </c>
       <c r="D17" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>257</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>298</v>
+        <v>258</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>299</v>
+        <v>259</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>337</v>
+        <v>287</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>284</v>
+        <v>244</v>
       </c>
       <c r="C21" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>338</v>
+        <v>288</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>285</v>
+        <v>245</v>
       </c>
       <c r="C22" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>339</v>
+        <v>289</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>340</v>
+        <v>290</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>341</v>
+        <v>291</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s">
-        <v>200</v>
+        <v>331</v>
       </c>
       <c r="D26" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>332</v>
       </c>
       <c r="D27" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>334</v>
       </c>
       <c r="D29" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>317</v>
+        <v>270</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>312</v>
+        <v>266</v>
       </c>
       <c r="C30" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="C31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>338</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>339</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>318</v>
+        <v>271</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>313</v>
+        <v>267</v>
       </c>
       <c r="C35" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="C36" t="s">
-        <v>202</v>
+        <v>341</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>343</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>344</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
-        <v>218</v>
+        <v>345</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>180</v>
+        <v>346</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>306</v>
+        <v>347</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="C43" t="s">
-        <v>219</v>
+        <v>348</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>181</v>
+        <v>349</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>220</v>
+        <v>351</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>182</v>
+        <v>352</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>352</v>
+        <v>294</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="D49" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>353</v>
+        <v>295</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="D50" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>354</v>
+        <v>296</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="D51" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>320</v>
+        <v>272</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>314</v>
+        <v>268</v>
       </c>
       <c r="C56" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="C57" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>322</v>
+        <v>273</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>315</v>
+        <v>269</v>
       </c>
       <c r="C61" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C62" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C63" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C64" t="s">
-        <v>99</v>
+        <v>376</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>102</v>
+        <v>377</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="C66" t="s">
-        <v>221</v>
+        <v>378</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C67" t="s">
-        <v>183</v>
+        <v>379</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C68" t="s">
-        <v>309</v>
+        <v>380</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="C69" t="s">
-        <v>222</v>
+        <v>381</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C70" t="s">
-        <v>184</v>
+        <v>382</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C71" t="s">
-        <v>310</v>
+        <v>383</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C72" t="s">
-        <v>223</v>
+        <v>384</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>185</v>
+        <v>385</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C74" t="s">
-        <v>311</v>
+        <v>386</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>250</v>
+        <v>214</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="C75" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
       <c r="F75" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Trying custom function-string parser
Generalisation of dependencies for parameters requires a method of
parsing.
Using the Anaconda built-in pyparsing package, parser.py introduces a
functionParser class to decompose an expression into tokens and
evaluate.
BODMAS, negative numbers and powers should be operational in the current
version.
The next few commits should hopefully read in custom functions from
cascade.xlsx and then evaluate them via the parser...
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="406">
   <si>
     <t>Code Label</t>
   </si>
@@ -38,12 +38,6 @@
     <t>lte</t>
   </si>
   <si>
-    <t>s+e</t>
-  </si>
-  <si>
-    <t>s-e</t>
-  </si>
-  <si>
     <t>ltsu</t>
   </si>
   <si>
@@ -56,42 +50,6 @@
     <t>ltft</t>
   </si>
   <si>
-    <t>s+du</t>
-  </si>
-  <si>
-    <t>s+dt</t>
-  </si>
-  <si>
-    <t>s+mu</t>
-  </si>
-  <si>
-    <t>s+mt</t>
-  </si>
-  <si>
-    <t>s+xu</t>
-  </si>
-  <si>
-    <t>s+xt</t>
-  </si>
-  <si>
-    <t>s-du</t>
-  </si>
-  <si>
-    <t>s-dt</t>
-  </si>
-  <si>
-    <t>s-mu</t>
-  </si>
-  <si>
-    <t>s-mt</t>
-  </si>
-  <si>
-    <t>s-xu</t>
-  </si>
-  <si>
-    <t>s-xt</t>
-  </si>
-  <si>
     <t>Vaccinated</t>
   </si>
   <si>
@@ -299,96 +257,6 @@
     <t>ltfsuc_rate</t>
   </si>
   <si>
-    <t>s+dyes_rate</t>
-  </si>
-  <si>
-    <t>s+dno_rate</t>
-  </si>
-  <si>
-    <t>s+myes_rate</t>
-  </si>
-  <si>
-    <t>s+mno_rate</t>
-  </si>
-  <si>
-    <t>s+xyes_rate</t>
-  </si>
-  <si>
-    <t>s+xno_rate</t>
-  </si>
-  <si>
-    <t>s+dsuc_rate</t>
-  </si>
-  <si>
-    <t>s+msuc_rate</t>
-  </si>
-  <si>
-    <t>s+xsuc_rate</t>
-  </si>
-  <si>
-    <t>s+dud_rate</t>
-  </si>
-  <si>
-    <t>s+dtd_rate</t>
-  </si>
-  <si>
-    <t>s+mud_rate</t>
-  </si>
-  <si>
-    <t>s+mtd_rate</t>
-  </si>
-  <si>
-    <t>s+xud_rate</t>
-  </si>
-  <si>
-    <t>s+xtd_rate</t>
-  </si>
-  <si>
-    <t>s-dyes_rate</t>
-  </si>
-  <si>
-    <t>s-dno_rate</t>
-  </si>
-  <si>
-    <t>s-myes_rate</t>
-  </si>
-  <si>
-    <t>s-mno_rate</t>
-  </si>
-  <si>
-    <t>s-xyes_rate</t>
-  </si>
-  <si>
-    <t>s-xno_rate</t>
-  </si>
-  <si>
-    <t>s-dsuc_rate</t>
-  </si>
-  <si>
-    <t>s-msuc_rate</t>
-  </si>
-  <si>
-    <t>s-xsuc_rate</t>
-  </si>
-  <si>
-    <t>s-dud_rate</t>
-  </si>
-  <si>
-    <t>s-dtd_rate</t>
-  </si>
-  <si>
-    <t>s-mud_rate</t>
-  </si>
-  <si>
-    <t>s-mtd_rate</t>
-  </si>
-  <si>
-    <t>s-xud_rate</t>
-  </si>
-  <si>
-    <t>s-xtd_rate</t>
-  </si>
-  <si>
     <t>Plot Coordinates</t>
   </si>
   <si>
@@ -431,39 +299,21 @@
     <t>Fast Latent Diagnosed</t>
   </si>
   <si>
-    <t>s+dd</t>
-  </si>
-  <si>
     <t>Drug-Susceptible Smear-Positive Diagnosed</t>
   </si>
   <si>
-    <t>s+md</t>
-  </si>
-  <si>
     <t>Multidrug-Resistant Smear-Positive Diagnosed</t>
   </si>
   <si>
-    <t>s+xd</t>
-  </si>
-  <si>
     <t>Extensively Drug-Resistant Smear-Positive Diagnosed</t>
   </si>
   <si>
-    <t>s-dd</t>
-  </si>
-  <si>
     <t>Drug-Susceptible Smear-Negative Diagnosed</t>
   </si>
   <si>
-    <t>s-md</t>
-  </si>
-  <si>
     <t>Multidrug-Resistant Smear-Negative Diagnosed</t>
   </si>
   <si>
-    <t>s-xd</t>
-  </si>
-  <si>
     <t>Extensively Drug-Resistant Smear-Negative Diagnosed</t>
   </si>
   <si>
@@ -503,24 +353,6 @@
     <t>Fast-LTBI Diagnosis Rate</t>
   </si>
   <si>
-    <t>s+ddd_rate</t>
-  </si>
-  <si>
-    <t>s+mdd_rate</t>
-  </si>
-  <si>
-    <t>s+xdd_rate</t>
-  </si>
-  <si>
-    <t>s-ddd_rate</t>
-  </si>
-  <si>
-    <t>s-mdd_rate</t>
-  </si>
-  <si>
-    <t>s-xdd_rate</t>
-  </si>
-  <si>
     <t>ltsdiag_rate</t>
   </si>
   <si>
@@ -545,24 +377,6 @@
     <t>ef</t>
   </si>
   <si>
-    <t>s+ddiag_rate</t>
-  </si>
-  <si>
-    <t>s+mdiag_rate</t>
-  </si>
-  <si>
-    <t>s+xdiag_rate</t>
-  </si>
-  <si>
-    <t>s-ddiag_rate</t>
-  </si>
-  <si>
-    <t>s-mdiag_rate</t>
-  </si>
-  <si>
-    <t>s-xdiag_rate</t>
-  </si>
-  <si>
     <t>fa</t>
   </si>
   <si>
@@ -680,12 +494,6 @@
     <t>ac_inf</t>
   </si>
   <si>
-    <t>s+_inf</t>
-  </si>
-  <si>
-    <t>s-_inf</t>
-  </si>
-  <si>
     <t>alive</t>
   </si>
   <si>
@@ -695,12 +503,6 @@
     <t>ac_prev</t>
   </si>
   <si>
-    <t>s+_prev</t>
-  </si>
-  <si>
-    <t>s-_prev</t>
-  </si>
-  <si>
     <t>Denominator</t>
   </si>
   <si>
@@ -827,18 +629,6 @@
     <t>gi</t>
   </si>
   <si>
-    <t>s+dbad_rate</t>
-  </si>
-  <si>
-    <t>s+mbad_rate</t>
-  </si>
-  <si>
-    <t>s-dbad_rate</t>
-  </si>
-  <si>
-    <t>s-mbad_rate</t>
-  </si>
-  <si>
     <t>(0,2)</t>
   </si>
   <si>
@@ -878,36 +668,12 @@
     <t>ltf_prop</t>
   </si>
   <si>
-    <t>s+_prop</t>
-  </si>
-  <si>
-    <t>s-_prop</t>
-  </si>
-  <si>
-    <t>s+d_prop</t>
-  </si>
-  <si>
-    <t>s+m_prop</t>
-  </si>
-  <si>
-    <t>s+x_prop</t>
-  </si>
-  <si>
     <t>Slow-LTBI Proportion of Latent Infections</t>
   </si>
   <si>
     <t>Fast-LTBI Proportion of Latent Infections</t>
   </si>
   <si>
-    <t>s-d_prop</t>
-  </si>
-  <si>
-    <t>s-m_prop</t>
-  </si>
-  <si>
-    <t>s-x_prop</t>
-  </si>
-  <si>
     <t>Sheet Label</t>
   </si>
   <si>
@@ -938,42 +704,6 @@
     <t>Population Sizes</t>
   </si>
   <si>
-    <t>s+d_infx</t>
-  </si>
-  <si>
-    <t>s+m_infx</t>
-  </si>
-  <si>
-    <t>s+x_infx</t>
-  </si>
-  <si>
-    <t>s-d_infx</t>
-  </si>
-  <si>
-    <t>s-m_infx</t>
-  </si>
-  <si>
-    <t>s-x_infx</t>
-  </si>
-  <si>
-    <t>s+d_prevx</t>
-  </si>
-  <si>
-    <t>s+m_prevx</t>
-  </si>
-  <si>
-    <t>s+x_prevx</t>
-  </si>
-  <si>
-    <t>s-d_prevx</t>
-  </si>
-  <si>
-    <t>s-m_prevx</t>
-  </si>
-  <si>
-    <t>s-x_prevx</t>
-  </si>
-  <si>
     <t>sh_disagg</t>
   </si>
   <si>
@@ -1022,9 +752,6 @@
     <t>SP DS Treatment Success Rate</t>
   </si>
   <si>
-    <t>SP DS-MDR Escalation Rate</t>
-  </si>
-  <si>
     <t>SP MDR Diagnosis Rate</t>
   </si>
   <si>
@@ -1121,9 +848,6 @@
     <t>SN DS Treatment Success Rate</t>
   </si>
   <si>
-    <t>SN DS-MDR Escalation Rate</t>
-  </si>
-  <si>
     <t>SN MDR Diagnosis Rate</t>
   </si>
   <si>
@@ -1199,24 +923,6 @@
     <t>Arguments</t>
   </si>
   <si>
-    <t>s+d_infxness</t>
-  </si>
-  <si>
-    <t>s+m_infxness</t>
-  </si>
-  <si>
-    <t>s+x_infxness</t>
-  </si>
-  <si>
-    <t>s-d_infxness</t>
-  </si>
-  <si>
-    <t>s-m_infxness</t>
-  </si>
-  <si>
-    <t>s-x_infxness</t>
-  </si>
-  <si>
     <t>SP DS Infectiousness</t>
   </si>
   <si>
@@ -1233,6 +939,303 @@
   </si>
   <si>
     <t>SN XDR Infectiousness</t>
+  </si>
+  <si>
+    <t>spe</t>
+  </si>
+  <si>
+    <t>spdu</t>
+  </si>
+  <si>
+    <t>spdd</t>
+  </si>
+  <si>
+    <t>spdt</t>
+  </si>
+  <si>
+    <t>spmu</t>
+  </si>
+  <si>
+    <t>spmd</t>
+  </si>
+  <si>
+    <t>spmt</t>
+  </si>
+  <si>
+    <t>spxu</t>
+  </si>
+  <si>
+    <t>spxd</t>
+  </si>
+  <si>
+    <t>spxt</t>
+  </si>
+  <si>
+    <t>sne</t>
+  </si>
+  <si>
+    <t>sndu</t>
+  </si>
+  <si>
+    <t>sndd</t>
+  </si>
+  <si>
+    <t>sndt</t>
+  </si>
+  <si>
+    <t>snmu</t>
+  </si>
+  <si>
+    <t>snmd</t>
+  </si>
+  <si>
+    <t>snmt</t>
+  </si>
+  <si>
+    <t>snxu</t>
+  </si>
+  <si>
+    <t>snxd</t>
+  </si>
+  <si>
+    <t>snxt</t>
+  </si>
+  <si>
+    <t>spd_infx</t>
+  </si>
+  <si>
+    <t>spm_infx</t>
+  </si>
+  <si>
+    <t>spx_infx</t>
+  </si>
+  <si>
+    <t>sp_inf</t>
+  </si>
+  <si>
+    <t>spd_prevx</t>
+  </si>
+  <si>
+    <t>spm_prevx</t>
+  </si>
+  <si>
+    <t>spx_prevx</t>
+  </si>
+  <si>
+    <t>sp_prev</t>
+  </si>
+  <si>
+    <t>spd_infxness</t>
+  </si>
+  <si>
+    <t>spm_infxness</t>
+  </si>
+  <si>
+    <t>spx_infxness</t>
+  </si>
+  <si>
+    <t>sp_prop</t>
+  </si>
+  <si>
+    <t>spd_prop</t>
+  </si>
+  <si>
+    <t>spm_prop</t>
+  </si>
+  <si>
+    <t>spx_prop</t>
+  </si>
+  <si>
+    <t>spddiag_rate</t>
+  </si>
+  <si>
+    <t>spdyes_rate</t>
+  </si>
+  <si>
+    <t>spdno_rate</t>
+  </si>
+  <si>
+    <t>spdsuc_rate</t>
+  </si>
+  <si>
+    <t>spdbad_rate</t>
+  </si>
+  <si>
+    <t>spmdiag_rate</t>
+  </si>
+  <si>
+    <t>spmyes_rate</t>
+  </si>
+  <si>
+    <t>spmno_rate</t>
+  </si>
+  <si>
+    <t>spmsuc_rate</t>
+  </si>
+  <si>
+    <t>spmbad_rate</t>
+  </si>
+  <si>
+    <t>spxdiag_rate</t>
+  </si>
+  <si>
+    <t>spxyes_rate</t>
+  </si>
+  <si>
+    <t>spxno_rate</t>
+  </si>
+  <si>
+    <t>spxsuc_rate</t>
+  </si>
+  <si>
+    <t>spdud_rate</t>
+  </si>
+  <si>
+    <t>spddd_rate</t>
+  </si>
+  <si>
+    <t>spdtd_rate</t>
+  </si>
+  <si>
+    <t>spmud_rate</t>
+  </si>
+  <si>
+    <t>spmdd_rate</t>
+  </si>
+  <si>
+    <t>spmtd_rate</t>
+  </si>
+  <si>
+    <t>spxud_rate</t>
+  </si>
+  <si>
+    <t>spxdd_rate</t>
+  </si>
+  <si>
+    <t>spxtd_rate</t>
+  </si>
+  <si>
+    <t>snd_infx</t>
+  </si>
+  <si>
+    <t>snm_infx</t>
+  </si>
+  <si>
+    <t>snx_infx</t>
+  </si>
+  <si>
+    <t>sn_inf</t>
+  </si>
+  <si>
+    <t>snd_prevx</t>
+  </si>
+  <si>
+    <t>snm_prevx</t>
+  </si>
+  <si>
+    <t>snx_prevx</t>
+  </si>
+  <si>
+    <t>sn_prev</t>
+  </si>
+  <si>
+    <t>snd_infxness</t>
+  </si>
+  <si>
+    <t>snm_infxness</t>
+  </si>
+  <si>
+    <t>snx_infxness</t>
+  </si>
+  <si>
+    <t>sn_prop</t>
+  </si>
+  <si>
+    <t>SP DsnMDR Escalation Rate</t>
+  </si>
+  <si>
+    <t>snd_prop</t>
+  </si>
+  <si>
+    <t>snm_prop</t>
+  </si>
+  <si>
+    <t>snx_prop</t>
+  </si>
+  <si>
+    <t>snddiag_rate</t>
+  </si>
+  <si>
+    <t>sndyes_rate</t>
+  </si>
+  <si>
+    <t>sndno_rate</t>
+  </si>
+  <si>
+    <t>sndsuc_rate</t>
+  </si>
+  <si>
+    <t>sndbad_rate</t>
+  </si>
+  <si>
+    <t>SN DsnMDR Escalation Rate</t>
+  </si>
+  <si>
+    <t>snmdiag_rate</t>
+  </si>
+  <si>
+    <t>snmyes_rate</t>
+  </si>
+  <si>
+    <t>snmno_rate</t>
+  </si>
+  <si>
+    <t>snmsuc_rate</t>
+  </si>
+  <si>
+    <t>snmbad_rate</t>
+  </si>
+  <si>
+    <t>snxdiag_rate</t>
+  </si>
+  <si>
+    <t>snxyes_rate</t>
+  </si>
+  <si>
+    <t>snxno_rate</t>
+  </si>
+  <si>
+    <t>snxsuc_rate</t>
+  </si>
+  <si>
+    <t>sndud_rate</t>
+  </si>
+  <si>
+    <t>snddd_rate</t>
+  </si>
+  <si>
+    <t>sndtd_rate</t>
+  </si>
+  <si>
+    <t>snmud_rate</t>
+  </si>
+  <si>
+    <t>snmdd_rate</t>
+  </si>
+  <si>
+    <t>snmtd_rate</t>
+  </si>
+  <si>
+    <t>snxud_rate</t>
+  </si>
+  <si>
+    <t>snxdd_rate</t>
+  </si>
+  <si>
+    <t>snxtd_rate</t>
+  </si>
+  <si>
+    <t>(spd_infxness*spd_infx)/alive</t>
   </si>
 </sst>
 </file>
@@ -1877,16 +1880,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>279</v>
+        <v>209</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>228</v>
+        <v>162</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>230</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1897,7 +1900,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>207</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1905,10 +1908,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1916,372 +1919,372 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>280</v>
+        <v>210</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>205</v>
+        <v>143</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>201</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>202</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>172</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>199</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>203</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>204</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>239</v>
+        <v>173</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>200</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>275</v>
+        <v>205</v>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>198</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>274</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>276</v>
+        <v>206</v>
       </c>
       <c r="B12" t="s">
-        <v>281</v>
+        <v>211</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>273</v>
+        <v>203</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>307</v>
       </c>
       <c r="B13" t="s">
-        <v>282</v>
+        <v>212</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>191</v>
+        <v>129</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>308</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>187</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>309</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>193</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>310</v>
       </c>
       <c r="B16" t="s">
-        <v>245</v>
+        <v>179</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>188</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>312</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>194</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="B19" t="s">
-        <v>246</v>
+        <v>180</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>314</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>315</v>
       </c>
       <c r="B21" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>195</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>316</v>
       </c>
       <c r="B22" t="s">
-        <v>247</v>
+        <v>181</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>317</v>
       </c>
       <c r="B23" t="s">
-        <v>283</v>
+        <v>213</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>192</v>
+        <v>130</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>318</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>319</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>320</v>
       </c>
       <c r="B26" t="s">
-        <v>248</v>
+        <v>182</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="B27" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>145</v>
+        <v>322</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>323</v>
       </c>
       <c r="B29" t="s">
-        <v>249</v>
+        <v>183</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>324</v>
       </c>
       <c r="B30" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>189</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>325</v>
       </c>
       <c r="B31" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>198</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>326</v>
       </c>
       <c r="B32" t="s">
-        <v>250</v>
+        <v>184</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>190</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>277</v>
+        <v>207</v>
       </c>
       <c r="B33" t="s">
-        <v>263</v>
+        <v>197</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>232</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="B34" t="s">
-        <v>210</v>
+        <v>148</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>231</v>
+        <v>165</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>209</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
+        <v>149</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2315,97 +2318,97 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>275</v>
+        <v>205</v>
       </c>
       <c r="L1" t="s">
-        <v>276</v>
+        <v>206</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>6</v>
+        <v>307</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>12</v>
+        <v>308</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>137</v>
+        <v>309</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>13</v>
+        <v>310</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>139</v>
+        <v>312</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>16</v>
+        <v>314</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>141</v>
+        <v>315</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>17</v>
+        <v>316</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>7</v>
+        <v>317</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>18</v>
+        <v>318</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>143</v>
+        <v>319</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>19</v>
+        <v>320</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>145</v>
+        <v>322</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>21</v>
+        <v>323</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>22</v>
+        <v>324</v>
       </c>
       <c r="AE1" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI1" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
@@ -2414,10 +2417,10 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -2450,7 +2453,7 @@
       <c r="AG2" s="6"/>
       <c r="AH2" s="7"/>
       <c r="AI2" s="8" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
@@ -2460,7 +2463,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -2493,7 +2496,7 @@
       <c r="AG3" s="9"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
@@ -2504,12 +2507,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -2541,14 +2544,14 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -2556,7 +2559,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="17" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="10"/>
@@ -2581,12 +2584,12 @@
       <c r="AG5" s="9"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
@@ -2594,14 +2597,14 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="17" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="10"/>
@@ -2626,26 +2629,26 @@
       <c r="AG6" s="9"/>
       <c r="AH6" s="10"/>
       <c r="AI6" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10" t="s">
-        <v>240</v>
+        <v>174</v>
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="9"/>
@@ -2671,12 +2674,12 @@
       <c r="AG7" s="9"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
@@ -2686,12 +2689,12 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="17" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
@@ -2716,12 +2719,12 @@
       <c r="AG8" s="9"/>
       <c r="AH8" s="10"/>
       <c r="AI8" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
@@ -2732,11 +2735,11 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K9" s="10"/>
       <c r="L9" s="17" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="10"/>
@@ -2761,12 +2764,12 @@
       <c r="AG9" s="9"/>
       <c r="AH9" s="10"/>
       <c r="AI9" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
@@ -2776,11 +2779,11 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10" t="s">
-        <v>241</v>
+        <v>175</v>
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="9"/>
@@ -2806,12 +2809,12 @@
       <c r="AG10" s="9"/>
       <c r="AH10" s="10"/>
       <c r="AI10" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>275</v>
+        <v>205</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
@@ -2824,7 +2827,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="17" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="10"/>
@@ -2849,12 +2852,12 @@
       <c r="AG11" s="9"/>
       <c r="AH11" s="10"/>
       <c r="AI11" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>276</v>
+        <v>206</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="20"/>
@@ -2868,7 +2871,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="21"/>
       <c r="M12" s="19" t="s">
-        <v>243</v>
+        <v>177</v>
       </c>
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
@@ -2880,7 +2883,7 @@
       <c r="U12" s="20"/>
       <c r="V12" s="22"/>
       <c r="W12" s="19" t="s">
-        <v>244</v>
+        <v>178</v>
       </c>
       <c r="X12" s="20"/>
       <c r="Y12" s="20"/>
@@ -2897,7 +2900,7 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>6</v>
+        <v>307</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
@@ -2912,17 +2915,17 @@
       <c r="L13" s="16"/>
       <c r="M13" s="6"/>
       <c r="N13" s="7" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="7" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="U13" s="7"/>
       <c r="V13" s="8"/>
@@ -2942,7 +2945,7 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>308</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
@@ -2958,7 +2961,7 @@
       <c r="M14" s="9"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10" t="s">
-        <v>169</v>
+        <v>113</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
@@ -2979,15 +2982,15 @@
       <c r="AF14" s="11"/>
       <c r="AG14" s="9"/>
       <c r="AH14" s="10" t="s">
-        <v>181</v>
+        <v>119</v>
       </c>
       <c r="AI14" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>137</v>
+        <v>309</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
@@ -3004,7 +3007,7 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
@@ -3024,15 +3027,15 @@
       <c r="AF15" s="11"/>
       <c r="AG15" s="9"/>
       <c r="AH15" s="10" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="AI15" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>13</v>
+        <v>310</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -3048,12 +3051,12 @@
       <c r="M16" s="9"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10" t="s">
-        <v>265</v>
+        <v>199</v>
       </c>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
@@ -3070,18 +3073,18 @@
       <c r="AE16" s="10"/>
       <c r="AF16" s="11"/>
       <c r="AG16" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="AH16" s="10" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="AI16" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
@@ -3100,7 +3103,7 @@
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
@@ -3118,15 +3121,15 @@
       <c r="AF17" s="11"/>
       <c r="AG17" s="9"/>
       <c r="AH17" s="10" t="s">
-        <v>182</v>
+        <v>120</v>
       </c>
       <c r="AI17" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>139</v>
+        <v>312</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -3146,7 +3149,7 @@
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
@@ -3163,15 +3166,15 @@
       <c r="AF18" s="11"/>
       <c r="AG18" s="9"/>
       <c r="AH18" s="10" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="AI18" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
@@ -3190,12 +3193,12 @@
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
       <c r="U19" s="10" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="V19" s="11"/>
       <c r="W19" s="9"/>
@@ -3209,18 +3212,18 @@
       <c r="AE19" s="10"/>
       <c r="AF19" s="11"/>
       <c r="AG19" s="9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="AH19" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="AI19" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>16</v>
+        <v>314</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -3242,7 +3245,7 @@
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
       <c r="U20" s="10" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="V20" s="11"/>
       <c r="W20" s="9"/>
@@ -3257,15 +3260,15 @@
       <c r="AF20" s="11"/>
       <c r="AG20" s="9"/>
       <c r="AH20" s="10" t="s">
-        <v>183</v>
+        <v>121</v>
       </c>
       <c r="AI20" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>141</v>
+        <v>315</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
@@ -3288,7 +3291,7 @@
       <c r="T21" s="10"/>
       <c r="U21" s="10"/>
       <c r="V21" s="11" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="W21" s="9"/>
       <c r="X21" s="10"/>
@@ -3302,15 +3305,15 @@
       <c r="AF21" s="11"/>
       <c r="AG21" s="9"/>
       <c r="AH21" s="10" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="AI21" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>17</v>
+        <v>316</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
@@ -3332,7 +3335,7 @@
       <c r="S22" s="13"/>
       <c r="T22" s="13"/>
       <c r="U22" s="13" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="V22" s="14"/>
       <c r="W22" s="12"/>
@@ -3346,18 +3349,18 @@
       <c r="AE22" s="13"/>
       <c r="AF22" s="14"/>
       <c r="AG22" s="12" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="AH22" s="13" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="AI22" s="14" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>7</v>
+        <v>317</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -3382,17 +3385,17 @@
       <c r="V23" s="8"/>
       <c r="W23" s="6"/>
       <c r="X23" s="7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="Y23" s="7"/>
       <c r="Z23" s="7"/>
       <c r="AA23" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="AB23" s="7"/>
       <c r="AC23" s="7"/>
       <c r="AD23" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="AE23" s="7"/>
       <c r="AF23" s="8"/>
@@ -3402,7 +3405,7 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>18</v>
+        <v>318</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -3428,7 +3431,7 @@
       <c r="W24" s="9"/>
       <c r="X24" s="10"/>
       <c r="Y24" s="10" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="Z24" s="10"/>
       <c r="AA24" s="10"/>
@@ -3439,15 +3442,15 @@
       <c r="AF24" s="11"/>
       <c r="AG24" s="9"/>
       <c r="AH24" s="10" t="s">
-        <v>184</v>
+        <v>122</v>
       </c>
       <c r="AI24" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>143</v>
+        <v>319</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -3474,7 +3477,7 @@
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
       <c r="Z25" s="10" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="AA25" s="10"/>
       <c r="AB25" s="10"/>
@@ -3484,15 +3487,15 @@
       <c r="AF25" s="11"/>
       <c r="AG25" s="9"/>
       <c r="AH25" s="10" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="AI25" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>19</v>
+        <v>320</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
@@ -3518,30 +3521,30 @@
       <c r="W26" s="9"/>
       <c r="X26" s="10"/>
       <c r="Y26" s="10" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="Z26" s="10"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="10" t="s">
-        <v>267</v>
+        <v>201</v>
       </c>
       <c r="AC26" s="10"/>
       <c r="AD26" s="10"/>
       <c r="AE26" s="10"/>
       <c r="AF26" s="11"/>
       <c r="AG26" s="9" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="AH26" s="10" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="AI26" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
@@ -3570,7 +3573,7 @@
       <c r="Z27" s="10"/>
       <c r="AA27" s="10"/>
       <c r="AB27" s="10" t="s">
-        <v>173</v>
+        <v>117</v>
       </c>
       <c r="AC27" s="10"/>
       <c r="AD27" s="10"/>
@@ -3578,15 +3581,15 @@
       <c r="AF27" s="11"/>
       <c r="AG27" s="9"/>
       <c r="AH27" s="10" t="s">
-        <v>185</v>
+        <v>123</v>
       </c>
       <c r="AI27" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>145</v>
+        <v>322</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
@@ -3616,22 +3619,22 @@
       <c r="AA28" s="10"/>
       <c r="AB28" s="10"/>
       <c r="AC28" s="10" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="AD28" s="10"/>
       <c r="AE28" s="10"/>
       <c r="AF28" s="11"/>
       <c r="AG28" s="9"/>
       <c r="AH28" s="10" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="AI28" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>21</v>
+        <v>323</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
@@ -3660,27 +3663,27 @@
       <c r="Z29" s="10"/>
       <c r="AA29" s="10"/>
       <c r="AB29" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="AC29" s="10"/>
       <c r="AD29" s="10"/>
       <c r="AE29" s="10" t="s">
-        <v>268</v>
+        <v>202</v>
       </c>
       <c r="AF29" s="11"/>
       <c r="AG29" s="9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="AH29" s="10" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="AI29" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>22</v>
+        <v>324</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -3712,20 +3715,20 @@
       <c r="AC30" s="10"/>
       <c r="AD30" s="10"/>
       <c r="AE30" s="10" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="AF30" s="11"/>
       <c r="AG30" s="9"/>
       <c r="AH30" s="10" t="s">
-        <v>186</v>
+        <v>124</v>
       </c>
       <c r="AI30" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>147</v>
+        <v>325</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
@@ -3758,19 +3761,19 @@
       <c r="AD31" s="10"/>
       <c r="AE31" s="10"/>
       <c r="AF31" s="11" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="AG31" s="9"/>
       <c r="AH31" s="10" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="AI31" s="11" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>23</v>
+        <v>326</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
@@ -3802,22 +3805,22 @@
       <c r="AC32" s="13"/>
       <c r="AD32" s="13"/>
       <c r="AE32" s="13" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="AF32" s="14"/>
       <c r="AG32" s="12" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="AH32" s="13" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="AI32" s="14" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>277</v>
+        <v>207</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -3830,7 +3833,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="16" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="M33" s="9"/>
       <c r="N33" s="10"/>
@@ -3855,12 +3858,12 @@
       <c r="AG33" s="6"/>
       <c r="AH33" s="7"/>
       <c r="AI33" s="8" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
@@ -3899,7 +3902,7 @@
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>209</v>
+        <v>147</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="13"/>
@@ -3946,7 +3949,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3979,33 +3982,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>296</v>
+        <v>218</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>236</v>
+        <v>170</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>229</v>
+        <v>163</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>278</v>
+        <v>208</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>227</v>
+        <v>161</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>216</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>153</v>
       </c>
       <c r="D2" s="2">
         <v>-1</v>
@@ -4014,219 +4017,219 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
       <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" t="s">
         <v>9</v>
-      </c>
-      <c r="N2" t="s">
-        <v>135</v>
-      </c>
-      <c r="O2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>327</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>230</v>
       </c>
       <c r="D3" s="2">
         <v>-1</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>308</v>
       </c>
       <c r="J3" t="s">
-        <v>137</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
       <c r="B4" t="s">
-        <v>321</v>
+        <v>231</v>
       </c>
       <c r="D4" s="2">
         <v>-1</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
       <c r="J4" t="s">
-        <v>139</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="B5" t="s">
-        <v>322</v>
+        <v>232</v>
       </c>
       <c r="D5" s="2">
         <v>-1</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>314</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>309</v>
+        <v>365</v>
       </c>
       <c r="B6" t="s">
-        <v>353</v>
+        <v>262</v>
       </c>
       <c r="D6" s="2">
         <v>-1</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>318</v>
       </c>
       <c r="J6" t="s">
-        <v>143</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>366</v>
       </c>
       <c r="B7" t="s">
-        <v>354</v>
+        <v>263</v>
       </c>
       <c r="D7" s="2">
         <v>-1</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="J7" t="s">
-        <v>145</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>311</v>
+        <v>367</v>
       </c>
       <c r="B8" t="s">
-        <v>355</v>
+        <v>264</v>
       </c>
       <c r="D8" s="2">
         <v>-1</v>
       </c>
       <c r="I8" t="s">
-        <v>22</v>
+        <v>324</v>
       </c>
       <c r="J8" t="s">
-        <v>147</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>220</v>
+        <v>330</v>
       </c>
       <c r="B9" t="s">
-        <v>386</v>
+        <v>294</v>
       </c>
       <c r="D9" s="2">
         <v>-1</v>
       </c>
       <c r="I9" t="s">
-        <v>6</v>
+        <v>307</v>
       </c>
       <c r="J9" t="s">
-        <v>306</v>
+        <v>327</v>
       </c>
       <c r="K9" t="s">
-        <v>13</v>
+        <v>310</v>
       </c>
       <c r="L9" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
       <c r="M9" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="N9" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="O9" t="s">
-        <v>17</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>368</v>
       </c>
       <c r="B10" t="s">
-        <v>388</v>
+        <v>296</v>
       </c>
       <c r="D10" s="2">
         <v>-1</v>
       </c>
       <c r="I10" t="s">
-        <v>7</v>
+        <v>317</v>
       </c>
       <c r="J10" t="s">
-        <v>309</v>
+        <v>365</v>
       </c>
       <c r="K10" t="s">
-        <v>19</v>
+        <v>320</v>
       </c>
       <c r="L10" t="s">
-        <v>310</v>
+        <v>366</v>
       </c>
       <c r="M10" t="s">
-        <v>21</v>
+        <v>323</v>
       </c>
       <c r="N10" t="s">
-        <v>311</v>
+        <v>367</v>
       </c>
       <c r="O10" t="s">
-        <v>23</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>217</v>
+        <v>155</v>
       </c>
       <c r="D11" s="2">
         <v>-1</v>
       </c>
       <c r="I11" t="s">
-        <v>276</v>
+        <v>206</v>
       </c>
       <c r="J11" t="s">
-        <v>220</v>
+        <v>330</v>
       </c>
       <c r="K11" t="s">
-        <v>221</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>233</v>
+        <v>167</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>298</v>
+        <v>220</v>
       </c>
       <c r="E12" s="2">
         <v>1000000</v>
@@ -4241,226 +4244,226 @@
         <v>3</v>
       </c>
       <c r="K12" t="s">
-        <v>275</v>
+        <v>205</v>
       </c>
       <c r="L12" t="s">
-        <v>277</v>
+        <v>207</v>
       </c>
       <c r="M12" t="s">
-        <v>218</v>
+        <v>156</v>
       </c>
       <c r="N12" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>223</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>234</v>
+        <v>168</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I13" t="s">
-        <v>218</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="B14" t="s">
-        <v>323</v>
+        <v>233</v>
       </c>
       <c r="D14" s="2">
         <v>-1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="H14" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I14" t="s">
-        <v>306</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="B15" t="s">
-        <v>324</v>
+        <v>234</v>
       </c>
       <c r="D15" s="2">
         <v>-1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="H15" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I15" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="B16" t="s">
-        <v>325</v>
+        <v>235</v>
       </c>
       <c r="D16" s="2">
         <v>-1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="H16" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I16" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>315</v>
+        <v>369</v>
       </c>
       <c r="B17" t="s">
-        <v>356</v>
+        <v>265</v>
       </c>
       <c r="D17" s="2">
         <v>-1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="H17" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I17" t="s">
-        <v>309</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>316</v>
+        <v>370</v>
       </c>
       <c r="B18" t="s">
-        <v>357</v>
+        <v>266</v>
       </c>
       <c r="D18" s="2">
         <v>-1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="H18" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I18" t="s">
-        <v>310</v>
+        <v>366</v>
       </c>
       <c r="N18" s="15"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>317</v>
+        <v>371</v>
       </c>
       <c r="B19" t="s">
-        <v>358</v>
+        <v>267</v>
       </c>
       <c r="D19" s="2">
         <v>-1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="H19" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I19" t="s">
-        <v>311</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>225</v>
+        <v>334</v>
       </c>
       <c r="B20" t="s">
-        <v>387</v>
+        <v>295</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>6</v>
+        <v>307</v>
       </c>
       <c r="H20" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I20" t="s">
-        <v>220</v>
+        <v>330</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>226</v>
+        <v>372</v>
       </c>
       <c r="B21" t="s">
-        <v>389</v>
+        <v>297</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>7</v>
+        <v>317</v>
       </c>
       <c r="H21" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I21" t="s">
-        <v>221</v>
+        <v>368</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>224</v>
+        <v>160</v>
       </c>
       <c r="B22" t="s">
-        <v>235</v>
+        <v>169</v>
       </c>
       <c r="D22" s="2">
         <v>-1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="H22" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="I22" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4474,7 +4477,7 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4485,7 +4488,7 @@
     <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4494,282 +4497,285 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>390</v>
+        <v>298</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>296</v>
+        <v>218</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>236</v>
+        <v>170</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>391</v>
+        <v>299</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>392</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>393</v>
+        <v>335</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>399</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>394</v>
+        <v>336</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>400</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>395</v>
+        <v>337</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>401</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s">
-        <v>402</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>404</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2">
         <v>0.5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>303</v>
+        <v>225</v>
+      </c>
+      <c r="G9" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>303</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>261</v>
+        <v>195</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="C11" t="s">
-        <v>259</v>
+        <v>193</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>303</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>262</v>
+        <v>196</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>260</v>
+        <v>194</v>
       </c>
       <c r="D12" s="2">
         <v>0.5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>303</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>284</v>
+        <v>214</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>291</v>
+        <v>216</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>285</v>
+        <v>215</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>292</v>
+        <v>217</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>240</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>112</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>241</v>
+        <v>175</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>255</v>
+        <v>189</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>251</v>
+        <v>185</v>
       </c>
       <c r="D23" s="2">
         <v>0.5</v>
@@ -4777,122 +4783,122 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>256</v>
+        <v>190</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>252</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>257</v>
+        <v>191</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>253</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>258</v>
+        <v>192</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>254</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>286</v>
+        <v>338</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>243</v>
+        <v>177</v>
       </c>
       <c r="C27" t="s">
-        <v>326</v>
+        <v>236</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>287</v>
+        <v>376</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>244</v>
+        <v>178</v>
       </c>
       <c r="C28" t="s">
-        <v>359</v>
+        <v>268</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>288</v>
+        <v>339</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>327</v>
+        <v>237</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>289</v>
+        <v>340</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>328</v>
+        <v>238</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>329</v>
+        <v>239</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>175</v>
+        <v>342</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>169</v>
+        <v>113</v>
       </c>
       <c r="C32" t="s">
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="D32" s="2">
         <v>0.5</v>
@@ -4900,13 +4906,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>343</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C33" t="s">
-        <v>331</v>
+        <v>241</v>
       </c>
       <c r="D33" s="2">
         <v>0.5</v>
@@ -4914,24 +4920,24 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>344</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>332</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>345</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>333</v>
+        <v>243</v>
       </c>
       <c r="D35" s="2">
         <v>0.5</v>
@@ -4939,583 +4945,583 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>269</v>
+        <v>346</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>265</v>
+        <v>199</v>
       </c>
       <c r="C36" t="s">
-        <v>334</v>
+        <v>377</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>347</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
-        <v>335</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>348</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>336</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>349</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>337</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>338</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>270</v>
+        <v>351</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="C41" t="s">
-        <v>339</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>352</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="C42" t="s">
-        <v>340</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>353</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>341</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>354</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>342</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>355</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>343</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>356</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>181</v>
+        <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>344</v>
+        <v>253</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>357</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>345</v>
+        <v>254</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>358</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>346</v>
+        <v>255</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>359</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>182</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
-        <v>347</v>
+        <v>256</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>360</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>348</v>
+        <v>257</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>361</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>349</v>
+        <v>258</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>362</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>183</v>
+        <v>121</v>
       </c>
       <c r="C52" t="s">
-        <v>350</v>
+        <v>259</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>163</v>
+        <v>363</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>351</v>
+        <v>260</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>364</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>352</v>
+        <v>261</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>293</v>
+        <v>378</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>360</v>
+        <v>269</v>
       </c>
       <c r="D55" s="2">
         <v>3</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>294</v>
+        <v>379</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C56" t="s">
-        <v>361</v>
+        <v>270</v>
       </c>
       <c r="D56" s="2">
         <v>2</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>295</v>
+        <v>380</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>362</v>
+        <v>271</v>
       </c>
       <c r="D57" s="2">
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>178</v>
+        <v>381</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="C58" t="s">
-        <v>363</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>382</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>364</v>
+        <v>273</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>109</v>
+        <v>383</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>365</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>114</v>
+        <v>384</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>366</v>
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>271</v>
+        <v>385</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>267</v>
+        <v>201</v>
       </c>
       <c r="C62" t="s">
-        <v>367</v>
+        <v>386</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>387</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>173</v>
+        <v>117</v>
       </c>
       <c r="C63" t="s">
-        <v>368</v>
+        <v>276</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>388</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C64" t="s">
-        <v>369</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>111</v>
+        <v>389</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C65" t="s">
-        <v>370</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>390</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C66" t="s">
-        <v>371</v>
+        <v>279</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>272</v>
+        <v>391</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>268</v>
+        <v>202</v>
       </c>
       <c r="C67" t="s">
-        <v>372</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>392</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="C68" t="s">
-        <v>373</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>112</v>
+        <v>393</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C69" t="s">
-        <v>374</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>113</v>
+        <v>394</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C70" t="s">
-        <v>375</v>
+        <v>283</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>116</v>
+        <v>395</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C71" t="s">
-        <v>376</v>
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>117</v>
+        <v>396</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>184</v>
+        <v>122</v>
       </c>
       <c r="C72" t="s">
-        <v>377</v>
+        <v>285</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>164</v>
+        <v>397</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C73" t="s">
-        <v>378</v>
+        <v>286</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>398</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C74" t="s">
-        <v>379</v>
+        <v>287</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>119</v>
+        <v>399</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>185</v>
+        <v>123</v>
       </c>
       <c r="C75" t="s">
-        <v>380</v>
+        <v>288</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>165</v>
+        <v>400</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C76" t="s">
-        <v>381</v>
+        <v>289</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C77" t="s">
-        <v>382</v>
+        <v>290</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>402</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>186</v>
+        <v>124</v>
       </c>
       <c r="C78" t="s">
-        <v>383</v>
+        <v>291</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>166</v>
+        <v>403</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C79" t="s">
-        <v>384</v>
+        <v>292</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>122</v>
+        <v>404</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C80" t="s">
-        <v>385</v>
+        <v>293</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>213</v>
+        <v>151</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
       <c r="C81" t="s">
-        <v>237</v>
+        <v>171</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
       <c r="F81" s="2">
         <v>1</v>
@@ -5555,50 +5561,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>296</v>
+        <v>218</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>297</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>298</v>
+        <v>220</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>305</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>300</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>303</v>
+        <v>225</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>304</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>302</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>319</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parser improved with dependencies and comments
The commented parser.py file now separates token stack production and
evaluation.
This means that the Settings object will be able to carry around token
stacks related to variables, delaying their evaluation until in the
Model object.
A deps dictionary can also be passed in during evaluation to replace
variable names with their values.
Run parser.py in this commit to test functionality. The next commits
will now link this infrastructure to the codebase.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="405">
   <si>
     <t>Code Label</t>
   </si>
@@ -918,9 +918,6 @@
   </si>
   <si>
     <t>Function</t>
-  </si>
-  <si>
-    <t>Arguments</t>
   </si>
   <si>
     <t>SP DS Infectiousness</t>
@@ -1487,7 +1484,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1552,6 +1549,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2021,7 +2021,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B13" t="s">
         <v>212</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B14" t="s">
         <v>101</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B15" t="s">
         <v>93</v>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B16" t="s">
         <v>179</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B17" t="s">
         <v>102</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B18" t="s">
         <v>94</v>
@@ -2090,7 +2090,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B19" t="s">
         <v>180</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B20" t="s">
         <v>103</v>
@@ -2112,7 +2112,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B21" t="s">
         <v>95</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B22" t="s">
         <v>181</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B23" t="s">
         <v>213</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B24" t="s">
         <v>104</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B25" t="s">
         <v>96</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B26" t="s">
         <v>182</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B27" t="s">
         <v>105</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B28" t="s">
         <v>97</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B29" t="s">
         <v>183</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B30" t="s">
         <v>106</v>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B31" t="s">
         <v>98</v>
@@ -2236,7 +2236,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B32" t="s">
         <v>184</v>
@@ -2342,64 +2342,64 @@
         <v>206</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>325</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>326</v>
       </c>
       <c r="AG1" s="4" t="s">
         <v>207</v>
@@ -2900,7 +2900,7 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
@@ -2990,7 +2990,7 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
@@ -3129,7 +3129,7 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
@@ -3223,7 +3223,7 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -3268,7 +3268,7 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
@@ -3313,7 +3313,7 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -3405,7 +3405,7 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -3495,7 +3495,7 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
@@ -3544,7 +3544,7 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
@@ -3589,7 +3589,7 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
@@ -3634,7 +3634,7 @@
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
@@ -3773,7 +3773,7 @@
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
@@ -4037,7 +4037,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B3" t="s">
         <v>230</v>
@@ -4046,15 +4046,15 @@
         <v>-1</v>
       </c>
       <c r="I3" t="s">
+        <v>307</v>
+      </c>
+      <c r="J3" t="s">
         <v>308</v>
-      </c>
-      <c r="J3" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B4" t="s">
         <v>231</v>
@@ -4063,15 +4063,15 @@
         <v>-1</v>
       </c>
       <c r="I4" t="s">
+        <v>310</v>
+      </c>
+      <c r="J4" t="s">
         <v>311</v>
-      </c>
-      <c r="J4" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B5" t="s">
         <v>232</v>
@@ -4080,15 +4080,15 @@
         <v>-1</v>
       </c>
       <c r="I5" t="s">
+        <v>313</v>
+      </c>
+      <c r="J5" t="s">
         <v>314</v>
-      </c>
-      <c r="J5" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B6" t="s">
         <v>262</v>
@@ -4097,15 +4097,15 @@
         <v>-1</v>
       </c>
       <c r="I6" t="s">
+        <v>317</v>
+      </c>
+      <c r="J6" t="s">
         <v>318</v>
-      </c>
-      <c r="J6" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7" t="s">
         <v>263</v>
@@ -4114,15 +4114,15 @@
         <v>-1</v>
       </c>
       <c r="I7" t="s">
+        <v>320</v>
+      </c>
+      <c r="J7" t="s">
         <v>321</v>
-      </c>
-      <c r="J7" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B8" t="s">
         <v>264</v>
@@ -4131,15 +4131,15 @@
         <v>-1</v>
       </c>
       <c r="I8" t="s">
+        <v>323</v>
+      </c>
+      <c r="J8" t="s">
         <v>324</v>
-      </c>
-      <c r="J8" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B9" t="s">
         <v>294</v>
@@ -4148,30 +4148,30 @@
         <v>-1</v>
       </c>
       <c r="I9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J9" t="s">
+        <v>326</v>
+      </c>
+      <c r="K9" t="s">
+        <v>309</v>
+      </c>
+      <c r="L9" t="s">
         <v>327</v>
       </c>
-      <c r="K9" t="s">
-        <v>310</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
+        <v>312</v>
+      </c>
+      <c r="N9" t="s">
         <v>328</v>
       </c>
-      <c r="M9" t="s">
-        <v>313</v>
-      </c>
-      <c r="N9" t="s">
-        <v>329</v>
-      </c>
       <c r="O9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B10" t="s">
         <v>296</v>
@@ -4180,25 +4180,25 @@
         <v>-1</v>
       </c>
       <c r="I10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J10" t="s">
+        <v>364</v>
+      </c>
+      <c r="K10" t="s">
+        <v>319</v>
+      </c>
+      <c r="L10" t="s">
         <v>365</v>
       </c>
-      <c r="K10" t="s">
-        <v>320</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
+        <v>322</v>
+      </c>
+      <c r="N10" t="s">
         <v>366</v>
       </c>
-      <c r="M10" t="s">
-        <v>323</v>
-      </c>
-      <c r="N10" t="s">
-        <v>367</v>
-      </c>
       <c r="O10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -4215,10 +4215,10 @@
         <v>206</v>
       </c>
       <c r="J11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -4281,7 +4281,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B14" t="s">
         <v>233</v>
@@ -4296,12 +4296,12 @@
         <v>158</v>
       </c>
       <c r="I14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B15" t="s">
         <v>234</v>
@@ -4316,12 +4316,12 @@
         <v>158</v>
       </c>
       <c r="I15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B16" t="s">
         <v>235</v>
@@ -4336,12 +4336,12 @@
         <v>158</v>
       </c>
       <c r="I16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B17" t="s">
         <v>265</v>
@@ -4356,12 +4356,12 @@
         <v>158</v>
       </c>
       <c r="I17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B18" t="s">
         <v>266</v>
@@ -4376,13 +4376,13 @@
         <v>158</v>
       </c>
       <c r="I18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="N18" s="15"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B19" t="s">
         <v>267</v>
@@ -4397,12 +4397,12 @@
         <v>158</v>
       </c>
       <c r="I19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B20" t="s">
         <v>295</v>
@@ -4414,18 +4414,18 @@
         <v>152</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H20" t="s">
         <v>158</v>
       </c>
       <c r="I20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B21" t="s">
         <v>297</v>
@@ -4437,13 +4437,13 @@
         <v>152</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H21" t="s">
         <v>158</v>
       </c>
       <c r="I21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -4477,7 +4477,7 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4488,18 +4488,18 @@
     <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" style="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
@@ -4514,9 +4514,7 @@
       <c r="G1" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>300</v>
-      </c>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4531,56 +4529,56 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -4599,8 +4597,8 @@
       <c r="E9" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G9" t="s">
-        <v>405</v>
+      <c r="G9" s="23" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -4816,7 +4814,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>177</v>
@@ -4833,7 +4831,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>178</v>
@@ -4847,7 +4845,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>24</v>
@@ -4864,7 +4862,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>25</v>
@@ -4878,7 +4876,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>26</v>
@@ -4892,7 +4890,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>113</v>
@@ -4906,7 +4904,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>27</v>
@@ -4920,7 +4918,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>28</v>
@@ -4931,7 +4929,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>42</v>
@@ -4945,18 +4943,18 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>199</v>
       </c>
       <c r="C36" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>114</v>
@@ -4967,7 +4965,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>29</v>
@@ -4978,7 +4976,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>30</v>
@@ -4989,7 +4987,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>43</v>
@@ -5000,7 +4998,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>200</v>
@@ -5011,7 +5009,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>115</v>
@@ -5022,7 +5020,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>31</v>
@@ -5033,7 +5031,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>32</v>
@@ -5044,7 +5042,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>44</v>
@@ -5055,7 +5053,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>119</v>
@@ -5069,7 +5067,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>48</v>
@@ -5083,7 +5081,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>49</v>
@@ -5097,7 +5095,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>120</v>
@@ -5111,7 +5109,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>50</v>
@@ -5125,7 +5123,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>51</v>
@@ -5139,7 +5137,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>121</v>
@@ -5153,7 +5151,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>52</v>
@@ -5167,7 +5165,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>53</v>
@@ -5181,7 +5179,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>33</v>
@@ -5198,7 +5196,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>34</v>
@@ -5215,7 +5213,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>35</v>
@@ -5232,7 +5230,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>116</v>
@@ -5243,7 +5241,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>36</v>
@@ -5254,7 +5252,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>37</v>
@@ -5265,7 +5263,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>45</v>
@@ -5276,18 +5274,18 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>201</v>
       </c>
       <c r="C62" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>117</v>
@@ -5298,7 +5296,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>38</v>
@@ -5309,7 +5307,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>39</v>
@@ -5320,7 +5318,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>46</v>
@@ -5331,7 +5329,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>202</v>
@@ -5342,7 +5340,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>118</v>
@@ -5353,7 +5351,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>40</v>
@@ -5364,7 +5362,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>41</v>
@@ -5375,7 +5373,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>47</v>
@@ -5386,7 +5384,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>122</v>
@@ -5400,7 +5398,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>54</v>
@@ -5414,7 +5412,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>55</v>
@@ -5428,7 +5426,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>123</v>
@@ -5442,7 +5440,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>56</v>
@@ -5456,7 +5454,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>57</v>
@@ -5470,7 +5468,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>124</v>
@@ -5484,7 +5482,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>58</v>
@@ -5498,7 +5496,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Simplest dependency case seemingly working
Run test.py for this commit to see slow-latent diagnosis rate be equal
to another parameter, as defined in cascade.xlsx.
Note: Performance does slow down quite a bit even for this simple
parameter-as-a-function-of-parameters step, which indicates complete
array pre-calculation should be done if there is no recursive
dependencies on characteristics. However, this is finnicky and can be
delayed.
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="405">
   <si>
     <t>Code Label</t>
   </si>
@@ -4477,7 +4477,7 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4489,7 +4489,7 @@
     <col min="5" max="5" width="11.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4535,6 +4535,9 @@
       <c r="C3" t="s">
         <v>300</v>
       </c>
+      <c r="D3" s="2">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -4597,7 +4600,7 @@
       <c r="E9" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="H9" s="23" t="s">
         <v>404</v>
       </c>
     </row>
@@ -4686,6 +4689,9 @@
       </c>
       <c r="C15" t="s">
         <v>109</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Functional parameters calculated in proper order
Handled a situation where a tagged parameter may depend on an untagged
parameter that then depends on another untagged parameter. More
practically; a transition rate that may be another transition rate times
a suppression factor.
All parameters that are functions of other parameters are now listed as
par_funcs in settings.py, which helps in proper-ordered evaluation after
characteristics in Model's updateDependencies().
</commit_message>
<xml_diff>
--- a/optima/cascade.xlsx
+++ b/optima/cascade.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="406">
   <si>
     <t>Code Label</t>
   </si>
@@ -1178,12 +1178,6 @@
     <t>Active Infection Rate (Active Recovered)</t>
   </si>
   <si>
-    <t>(-2,3)</t>
-  </si>
-  <si>
-    <t>(2,3)</t>
-  </si>
-  <si>
     <t>SP DS Infectiousness</t>
   </si>
   <si>
@@ -1202,28 +1196,46 @@
     <t>SN XDR Infectiousness</t>
   </si>
   <si>
-    <t>(6,3)</t>
-  </si>
-  <si>
-    <t>(0,4)</t>
-  </si>
-  <si>
-    <t>(-4,4)</t>
-  </si>
-  <si>
-    <t>(4,4)</t>
-  </si>
-  <si>
-    <t>(-6,3)</t>
-  </si>
-  <si>
-    <t>(-2,5)</t>
-  </si>
-  <si>
-    <t>(2,5)</t>
-  </si>
-  <si>
     <t>spd_infxness*spd_prevx+spm_infxness*spm_prevx+spx_infxness*spx_prevx+snd_infxness*snd_prevx+snm_infxness*snm_prevx+snx_infxness*snx_prevx</t>
+  </si>
+  <si>
+    <t>(0,5)</t>
+  </si>
+  <si>
+    <t>(9,4)</t>
+  </si>
+  <si>
+    <t>(-9,4)</t>
+  </si>
+  <si>
+    <t>(-3,4)</t>
+  </si>
+  <si>
+    <t>(3,4)</t>
+  </si>
+  <si>
+    <t>(-9,3)</t>
+  </si>
+  <si>
+    <t>(-3,3)</t>
+  </si>
+  <si>
+    <t>(3,3)</t>
+  </si>
+  <si>
+    <t>(9,3)</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>yo</t>
+  </si>
+  <si>
+    <t>0.25*infs_rate</t>
+  </si>
+  <si>
+    <t>check+check</t>
   </si>
 </sst>
 </file>
@@ -1851,7 +1863,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1891,7 +1903,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1902,7 +1914,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1913,7 +1925,7 @@
         <v>345</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1924,7 +1936,7 @@
         <v>346</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1957,7 +1969,7 @@
         <v>349</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1968,7 +1980,7 @@
         <v>350</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1979,7 +1991,7 @@
         <v>148</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -4379,10 +4391,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4431,6 +4443,9 @@
       <c r="C2" t="s">
         <v>56</v>
       </c>
+      <c r="D2" s="2">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -4438,7 +4453,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D3" s="2">
         <v>0.25</v>
@@ -4450,7 +4465,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D4" s="2">
         <v>0.5</v>
@@ -4462,7 +4477,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4471,7 +4486,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -4480,7 +4495,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4489,7 +4504,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -4509,50 +4524,55 @@
         <v>-1</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>402</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>383</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>165</v>
-      </c>
+        <v>403</v>
+      </c>
+      <c r="F10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>136</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>165</v>
       </c>
+      <c r="F11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
-        <v>385</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.5</v>
+        <v>384</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>165</v>
@@ -4560,189 +4580,192 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>355</v>
+        <v>146</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>364</v>
-      </c>
-      <c r="H13" s="23"/>
+        <v>385</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>371</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>134</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="C17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>380</v>
-      </c>
-      <c r="H21" s="23"/>
+        <v>377</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>381</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="H22" s="23"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>354</v>
+        <v>379</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>360</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.5</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>361</v>
+        <v>360</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>269</v>
+        <v>359</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>137</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>168</v>
+        <v>363</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
-        <v>208</v>
+        <v>176</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>168</v>
@@ -4750,16 +4773,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>177</v>
-      </c>
-      <c r="D29" s="2">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>168</v>
@@ -4767,16 +4787,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D30" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>168</v>
@@ -4784,13 +4804,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>179</v>
+        <v>178</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>168</v>
@@ -4798,27 +4821,27 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>180</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.5</v>
+        <v>179</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D33" s="2">
         <v>0.5</v>
@@ -4826,162 +4849,162 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>183</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.5</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>149</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>308</v>
+        <v>183</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
-        <v>184</v>
+        <v>308</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>150</v>
+        <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="C42" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>193</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>163</v>
@@ -4989,13 +5012,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>163</v>
@@ -5003,13 +5026,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>163</v>
@@ -5017,13 +5040,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>163</v>
@@ -5031,13 +5054,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>163</v>
@@ -5045,13 +5068,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>163</v>
@@ -5059,13 +5082,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>163</v>
@@ -5073,13 +5096,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C54" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>163</v>
@@ -5087,33 +5110,30 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C55" t="s">
-        <v>209</v>
-      </c>
-      <c r="D55" s="2">
-        <v>3</v>
+        <v>201</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D56" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>168</v>
@@ -5121,16 +5141,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C57" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D57" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>168</v>
@@ -5138,181 +5158,184 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="C58" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C59" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C60" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C61" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>151</v>
+        <v>40</v>
       </c>
       <c r="C62" t="s">
-        <v>317</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
       <c r="C63" t="s">
-        <v>216</v>
+        <v>317</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="C64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C65" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>152</v>
+        <v>41</v>
       </c>
       <c r="C67" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="C68" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C70" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C72" t="s">
-        <v>225</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>163</v>
+        <v>224</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>163</v>
@@ -5320,13 +5343,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>163</v>
@@ -5334,13 +5357,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="C75" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>163</v>
@@ -5348,13 +5371,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="C76" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>163</v>
@@ -5362,13 +5385,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C77" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>163</v>
@@ -5376,13 +5399,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="C78" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>163</v>
@@ -5390,13 +5413,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="C79" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>163</v>
@@ -5404,13 +5427,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C80" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>163</v>
@@ -5418,23 +5441,34 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>113</v>
+        <v>335</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="C81" t="s">
-        <v>133</v>
+        <v>233</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F81" s="2">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C82" t="s">
+        <v>133</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F82" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B83" s="2"/>
@@ -5444,6 +5478,9 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B86" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>